<commit_message>
add aimpoint footprint reworks
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15251CD3-F141-4E57-B4FB-691FC9D130D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A445B2C-27DD-4A81-8C54-5A1614857833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
   <si>
     <t>new</t>
   </si>
@@ -234,6 +234,141 @@
   </si>
   <si>
     <t>Primary Arms SLx 1x MicroPrism ACSS-G2</t>
+  </si>
+  <si>
+    <t>unity_fast_micro_mount</t>
+  </si>
+  <si>
+    <t>Unity Fast Micro</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo_cowitness_qd_mount</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo Cowitness QD Mount</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo4_mount</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo4</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo4_low</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo4 Low</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo4t_1/3_cowitness_mount</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo4T Lower Hex Bolt 1/3 Co-witness</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo5_low_mount</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo5 Low Mount</t>
+  </si>
+  <si>
+    <t>scalarworks_leap01_swo100_1.42_mount</t>
+  </si>
+  <si>
+    <t>Scalarworks Leap01 SWO 100 1.42 Mount</t>
+  </si>
+  <si>
+    <t>scalarworks_leap01_swo110_1.57_mount</t>
+  </si>
+  <si>
+    <t>Scalarworks Leap01 SWO 110 1.57 Mount</t>
+  </si>
+  <si>
+    <t>scalarworks_leap01_swo120_1.93_mount</t>
+  </si>
+  <si>
+    <t>Scalarworks Leap01 SWO 120 1.93 Mount</t>
+  </si>
+  <si>
+    <t>aimpoint_amm_dovetail_11mm_mount</t>
+  </si>
+  <si>
+    <t>Aimpoint AMM Dovetail Groove 11mm Mount</t>
+  </si>
+  <si>
+    <t>aimpoint_micro_lrp_qd_mount</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro LRP QD Mount</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo4_sight</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo4t_sight</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo4T</t>
+  </si>
+  <si>
+    <t>aimpoint_micro_spacer_high_39mm</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro Spacer High 39mm</t>
+  </si>
+  <si>
+    <t>aimpoint_micro_spacer_low_30mm</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro Spacer Low 30mm</t>
+  </si>
+  <si>
+    <t>aimpoint_micro_t1_sight</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro T1</t>
+  </si>
+  <si>
+    <t>aimpoint_micro_t2_sight</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro T2</t>
+  </si>
+  <si>
+    <t>aimpoint_compm5_sight</t>
+  </si>
+  <si>
+    <t>Aimpoint CompM5</t>
+  </si>
+  <si>
+    <t>sig_sauer_romeo5_1x20_sight</t>
+  </si>
+  <si>
+    <t>Sig Sauer Romeo5 1x20 Sight</t>
+  </si>
+  <si>
+    <t>aimpoint_micro_t2_lens_caps</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro T2 Lens Caps</t>
+  </si>
+  <si>
+    <t>romeo4t_lens_caps</t>
+  </si>
+  <si>
+    <t>Romeo4T Lens</t>
+  </si>
+  <si>
+    <t>romeo4t_folded_lens_caps</t>
+  </si>
+  <si>
+    <t>Romeo4T Folded Lens</t>
+  </si>
+  <si>
+    <t>aimpoint_compm5_lens_caps</t>
+  </si>
+  <si>
+    <t>Aimpoint CompM5 Lens Caps</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1323,7 @@
         <v>-0.4</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q41" si="0">P3*0.015+0.02</f>
+        <f t="shared" ref="Q3:Q32" si="0">P3*0.015+0.02</f>
         <v>0.02</v>
       </c>
     </row>
@@ -1283,7 +1418,7 @@
         <v>1100</v>
       </c>
       <c r="N6" s="1">
-        <f>C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
+        <f t="shared" ref="N6:N12" si="2">C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
         <v>-1.8</v>
       </c>
       <c r="P6">
@@ -1322,7 +1457,7 @@
         <v>1200</v>
       </c>
       <c r="N7" s="1">
-        <f>C7-D7*20-E7*0.8-F7*0.6-H7*5+I7*10+J7/300</f>
+        <f t="shared" si="2"/>
         <v>-1.8</v>
       </c>
       <c r="P7">
@@ -1361,7 +1496,7 @@
         <v>1000</v>
       </c>
       <c r="N8" s="1">
-        <f>C8-D8*20-E8*0.8-F8*0.6-H8*5+I8*10+J8/300</f>
+        <f t="shared" si="2"/>
         <v>-1.8</v>
       </c>
       <c r="P8">
@@ -1400,7 +1535,7 @@
         <v>800</v>
       </c>
       <c r="N9" s="1">
-        <f>C9-D9*20-E9*0.8-F9*0.6-H9*5+I9*10+J9/300</f>
+        <f t="shared" si="2"/>
         <v>-2.8</v>
       </c>
       <c r="P9">
@@ -1429,7 +1564,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1">
-        <f>C10-D10*20-E10*0.8-F10*0.6-H10*5+I10*10+J10/300</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q10">
@@ -1462,7 +1597,7 @@
         <v>400</v>
       </c>
       <c r="N11" s="1">
-        <f>C11-D11*20-E11*0.8-F11*0.6-H11*5+I11*10+J11/300</f>
+        <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
       <c r="Q11">
@@ -1495,7 +1630,7 @@
         <v>200</v>
       </c>
       <c r="N12" s="1">
-        <f>C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="Q12">
@@ -1520,7 +1655,7 @@
         <v>350</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" ref="N13:N28" si="2">C13-D13*20-E13*0.8-F13*0.6-H13*5+I13*10+J13/300</f>
+        <f t="shared" ref="N13:N28" si="3">C13-D13*20-E13*0.8-F13*0.6-H13*5+I13*10+J13/300</f>
         <v>-0.6</v>
       </c>
       <c r="Q13">
@@ -1545,7 +1680,7 @@
         <v>200</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.6</v>
       </c>
       <c r="Q14">
@@ -1570,7 +1705,7 @@
         <v>100</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="Q15">
@@ -1598,7 +1733,7 @@
         <v>1200</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-4.2</v>
       </c>
       <c r="P16">
@@ -1629,7 +1764,7 @@
         <v>1200</v>
       </c>
       <c r="N17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-4.2</v>
       </c>
       <c r="Q17">
@@ -1657,7 +1792,7 @@
         <v>1500</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-4.2</v>
       </c>
       <c r="Q18">
@@ -1685,7 +1820,7 @@
         <v>1500</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-4.2</v>
       </c>
       <c r="Q19">
@@ -1710,7 +1845,7 @@
         <v>1300</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.6</v>
       </c>
       <c r="P20">
@@ -1736,7 +1871,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q21">
@@ -1769,7 +1904,7 @@
         <v>200</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.4</v>
       </c>
       <c r="Q22">
@@ -1802,7 +1937,7 @@
         <v>250</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="Q23">
@@ -1835,7 +1970,7 @@
         <v>300</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.4000000000000001</v>
       </c>
       <c r="Q24">
@@ -1860,7 +1995,7 @@
         <v>800</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.8</v>
       </c>
       <c r="Q25">
@@ -1893,7 +2028,7 @@
         <v>1200</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2.2000000000000002</v>
       </c>
       <c r="P26">
@@ -1929,7 +2064,7 @@
         <v>1100</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="P27">
@@ -1955,7 +2090,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q28">
@@ -1977,10 +2112,10 @@
         <v>0.04</v>
       </c>
       <c r="M29">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N29" s="1">
-        <f>C29-D29*20-E29*0.8-F29*0.6-H29*5+I29*10+J29/300</f>
+        <f t="shared" ref="N29:N55" si="4">C29-D29*20-E29*0.8-F29*0.6-H29*5+I29*10+J29/300</f>
         <v>-0.8</v>
       </c>
       <c r="Q29">
@@ -2005,7 +2140,7 @@
         <v>200</v>
       </c>
       <c r="N30" s="1">
-        <f>C30-D30*20-E30*0.8-F30*0.6-H30*5+I30*10+J30/300</f>
+        <f t="shared" si="4"/>
         <v>-0.4</v>
       </c>
       <c r="Q30">
@@ -2030,7 +2165,7 @@
         <v>900</v>
       </c>
       <c r="N31" s="1">
-        <f>C31-D31*20-E31*0.8-F31*0.6-H31*5+I31*10+J31/300</f>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="Q31">
@@ -2040,7 +2175,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N32" s="1">
-        <f>C32-D32*20-E32*0.8-F32*0.6-H32*5+I32*10+J32/300</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q32">
@@ -2048,107 +2183,604 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0.02</v>
+      </c>
+      <c r="M33">
+        <v>200</v>
+      </c>
       <c r="N33" s="1">
         <f>C33-D33*20-E33*0.8-F33*0.6-H33*5+I33*10+J33/300</f>
+        <v>-0.4</v>
+      </c>
+      <c r="Q33">
+        <f>P33*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34">
         <v>0</v>
       </c>
-      <c r="P33">
-        <v>17</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="0"/>
-        <v>0.27500000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>0.02</v>
+      </c>
+      <c r="M34">
+        <v>200</v>
+      </c>
       <c r="N34" s="1">
         <f>C34-D34*20-E34*0.8-F34*0.6-H34*5+I34*10+J34/300</f>
+        <v>-0.4</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" ref="Q34:Q55" si="5">P34*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35">
         <v>0</v>
       </c>
-      <c r="Q34">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>0.03</v>
+      </c>
+      <c r="M35">
+        <v>300</v>
+      </c>
       <c r="N35" s="1">
         <f>C35-D35*20-E35*0.8-F35*0.6-H35*5+I35*10+J35/300</f>
+        <v>-0.6</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36">
         <v>0</v>
       </c>
-      <c r="Q35">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="36" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0.03</v>
+      </c>
+      <c r="M36">
+        <v>200</v>
+      </c>
       <c r="N36" s="1">
         <f>C36-D36*20-E36*0.8-F36*0.6-H36*5+I36*10+J36/300</f>
-        <v>0</v>
+        <v>-0.6</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="37" spans="14:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37">
+        <v>-1</v>
+      </c>
+      <c r="D37">
+        <v>0.04</v>
+      </c>
+      <c r="M37">
+        <v>200</v>
+      </c>
       <c r="N37" s="1">
         <f>C37-D37*20-E37*0.8-F37*0.6-H37*5+I37*10+J37/300</f>
-        <v>0</v>
+        <v>-1.8</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="38" spans="14:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
+        <v>-0.5</v>
+      </c>
+      <c r="D38">
+        <v>0.05</v>
+      </c>
+      <c r="M38">
+        <v>300</v>
+      </c>
       <c r="N38" s="1">
         <f>C38-D38*20-E38*0.8-F38*0.6-H38*5+I38*10+J38/300</f>
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="39" spans="14:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39">
+        <v>-0.5</v>
+      </c>
+      <c r="D39">
+        <v>0.05</v>
+      </c>
+      <c r="M39">
+        <v>400</v>
+      </c>
       <c r="N39" s="1">
         <f>C39-D39*20-E39*0.8-F39*0.6-H39*5+I39*10+J39/300</f>
+        <v>-1.5</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40">
+        <v>-1</v>
+      </c>
+      <c r="D40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M40">
+        <v>500</v>
+      </c>
+      <c r="N40" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.4000000000000004</v>
+      </c>
+      <c r="P40">
+        <v>3.5</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41">
+        <v>-1</v>
+      </c>
+      <c r="D41">
+        <v>0.04</v>
+      </c>
+      <c r="M41">
+        <v>500</v>
+      </c>
+      <c r="N41" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.8</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42">
+        <v>-1</v>
+      </c>
+      <c r="D42">
+        <v>0.05</v>
+      </c>
+      <c r="M42">
+        <v>550</v>
+      </c>
+      <c r="N42" s="1">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43">
+        <v>-1</v>
+      </c>
+      <c r="D43">
+        <v>0.06</v>
+      </c>
+      <c r="M43">
+        <v>600</v>
+      </c>
+      <c r="N43" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44">
+        <v>-0.5</v>
+      </c>
+      <c r="D44">
+        <v>0.03</v>
+      </c>
+      <c r="M44">
+        <v>200</v>
+      </c>
+      <c r="N44" s="1">
+        <f>C44-D44*20-E44*0.8-F44*0.6-H44*5+I44*10+J44/300</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45">
+        <v>-0.5</v>
+      </c>
+      <c r="D45">
+        <v>0.04</v>
+      </c>
+      <c r="M45">
+        <v>200</v>
+      </c>
+      <c r="N45" s="1">
+        <f>C45-D45*20-E45*0.8-F45*0.6-H45*5+I45*10+J45/300</f>
+        <v>-1.3</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46">
+        <v>-1</v>
+      </c>
+      <c r="D46">
+        <v>0.08</v>
+      </c>
+      <c r="M46">
+        <v>1000</v>
+      </c>
+      <c r="N46" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.6</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+      <c r="R46">
+        <v>369.99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47">
+        <v>-1</v>
+      </c>
+      <c r="D47">
+        <v>0.08</v>
+      </c>
+      <c r="M47">
+        <v>1100</v>
+      </c>
+      <c r="N47" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.6</v>
+      </c>
+      <c r="P47">
+        <v>7.6</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="5"/>
+        <v>0.13399999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48">
+        <v>-1</v>
+      </c>
+      <c r="D48">
+        <v>0.06</v>
+      </c>
+      <c r="M48">
+        <v>1200</v>
+      </c>
+      <c r="N48" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49">
+        <v>-1</v>
+      </c>
+      <c r="D49">
+        <v>0.06</v>
+      </c>
+      <c r="M49">
+        <v>1300</v>
+      </c>
+      <c r="N49" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="P49">
+        <v>3</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="5"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="R49">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50">
+        <v>-0.5</v>
+      </c>
+      <c r="D50">
+        <v>0.1</v>
+      </c>
+      <c r="M50">
+        <v>1400</v>
+      </c>
+      <c r="N50" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.5</v>
+      </c>
+      <c r="P50">
+        <v>5.2</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="5"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="R50">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51">
+        <v>-1</v>
+      </c>
+      <c r="D51">
+        <v>0.06</v>
+      </c>
+      <c r="M51">
+        <v>700</v>
+      </c>
+      <c r="N51" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+      <c r="R51">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.02</v>
+      </c>
+      <c r="M52">
         <v>0</v>
       </c>
-      <c r="Q39">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="40" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N40" s="1">
-        <f>C40-D40*20-E40*0.8-F40*0.6-H40*5+I40*10+J40/300</f>
+      <c r="N52" s="1">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>0.02</v>
+      </c>
+      <c r="M53">
         <v>0</v>
       </c>
-      <c r="Q40">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="41" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N41" s="1"/>
-      <c r="Q41">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="42" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="14:17" x14ac:dyDescent="0.25">
-      <c r="N45" s="1"/>
+      <c r="N53" s="1">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0.01</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54" s="1">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0.01</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55" s="1">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="5"/>
+        <v>0.02</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add eotechs and acro
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A445B2C-27DD-4A81-8C54-5A1614857833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FECE03-613C-4831-BBB4-DDA32123680E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="152">
   <si>
     <t>new</t>
   </si>
@@ -369,6 +369,126 @@
   </si>
   <si>
     <t>Aimpoint CompM5 Lens Caps</t>
+  </si>
+  <si>
+    <t>bt_qd_nar_acro_22mm_mount</t>
+  </si>
+  <si>
+    <t>B&amp;T QD NAR ACRO 22m Mount</t>
+  </si>
+  <si>
+    <t>bt_qd_nar_acro_30mm_mount</t>
+  </si>
+  <si>
+    <t>B&amp;T QD NAR ACRO 30m Mount</t>
+  </si>
+  <si>
+    <t>bt_qd_nar_acro_39mm_mount</t>
+  </si>
+  <si>
+    <t>B&amp;T QD NAR ACRO 39m Mount</t>
+  </si>
+  <si>
+    <t>aimpoint_acro_p2_reflex_sight</t>
+  </si>
+  <si>
+    <t>Aimpoint ACRO P-2 Reflex</t>
+  </si>
+  <si>
+    <t>eotech_553_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech 553</t>
+  </si>
+  <si>
+    <t>eotech_552_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech 552</t>
+  </si>
+  <si>
+    <t>eotech_512_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech 512</t>
+  </si>
+  <si>
+    <t>eotech_exps3_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech EXPS-3</t>
+  </si>
+  <si>
+    <t>eotech_exps2_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech EXPS-2</t>
+  </si>
+  <si>
+    <t>eotech_xps3_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech XPS3</t>
+  </si>
+  <si>
+    <t>eotech_xps2_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech XPS2</t>
+  </si>
+  <si>
+    <t>eotech_xps2_green_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech XPS2 Green Holo Sight</t>
+  </si>
+  <si>
+    <t>eotech_xps2z_zombie_stopper_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech XPS2Z Zombie Stopper Holo Sight</t>
+  </si>
+  <si>
+    <t>eotech_exps2_green_holo_sight</t>
+  </si>
+  <si>
+    <t>Eotech EXPS2 Green Holo Sight</t>
+  </si>
+  <si>
+    <t>eotech_exps2_mount</t>
+  </si>
+  <si>
+    <t>Eotech EXPS2 Mount</t>
+  </si>
+  <si>
+    <t>eotech_exps3_mount</t>
+  </si>
+  <si>
+    <t>Eotech EXPS3 Mount</t>
+  </si>
+  <si>
+    <t>eotech_exps2_hood</t>
+  </si>
+  <si>
+    <t>Eotech EXPS 2 Hood</t>
+  </si>
+  <si>
+    <t>eotech_exps3_hood</t>
+  </si>
+  <si>
+    <t>Eotech EXPS 3 Hood</t>
+  </si>
+  <si>
+    <t>eotech_exps2_green_hood</t>
+  </si>
+  <si>
+    <t>Eotech EXPS2 Green Hood</t>
+  </si>
+  <si>
+    <t>eotech_553_hood</t>
+  </si>
+  <si>
+    <t>Eotech 553 Hood</t>
   </si>
 </sst>
 </file>
@@ -1210,20 +1330,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="21" width="6.7109375" customWidth="1"/>
+    <col min="3" max="21" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1241,7 +1361,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1294,7 +1414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1323,11 +1443,11 @@
         <v>-0.4</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q32" si="0">P3*0.015+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q3:Q21" si="0">P3*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1360,7 +1480,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1393,7 +1513,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1418,7 +1538,7 @@
         <v>1100</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:N12" si="2">C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
+        <f t="shared" ref="N6:N10" si="2">C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
         <v>-1.8</v>
       </c>
       <c r="P6">
@@ -1432,7 +1552,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1471,7 +1591,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1510,7 +1630,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1549,7 +1669,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1572,18 +1692,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1594,29 +1714,29 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.8</v>
+        <f t="shared" ref="N11:N17" si="3">C11-D11*20-E11*0.8-F11*0.6-H11*5+I11*10+J11/300</f>
+        <v>-0.4</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1627,251 +1747,248 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.4</v>
+        <f t="shared" si="3"/>
+        <v>-1</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0.03</v>
-      </c>
-      <c r="M13">
-        <v>350</v>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1">
+        <v>300</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" ref="N13:N28" si="3">C13-D13*20-E13*0.8-F13*0.6-H13*5+I13*10+J13/300</f>
-        <v>-0.6</v>
+        <f t="shared" si="3"/>
+        <v>-1.4000000000000001</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D14">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="M14">
-        <v>200</v>
+        <v>800</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="3"/>
-        <v>-0.6</v>
+        <v>-1.8</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0.05</v>
-      </c>
-      <c r="M15">
-        <v>100</v>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1">
+        <v>1200</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="P15">
+        <v>1.9</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16">
-        <v>-3</v>
-      </c>
-      <c r="D16">
-        <v>0.12</v>
-      </c>
-      <c r="F16">
-        <v>-2</v>
-      </c>
-      <c r="M16">
-        <v>1200</v>
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1">
+        <v>1100</v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="3"/>
-        <v>-4.2</v>
+        <v>-2</v>
       </c>
       <c r="P16">
-        <v>7.9</v>
+        <v>1.4</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
-        <v>0.13849999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17">
-        <v>-3</v>
-      </c>
-      <c r="D17">
-        <v>0.12</v>
-      </c>
-      <c r="F17">
-        <v>-2</v>
-      </c>
-      <c r="M17">
-        <v>1200</v>
-      </c>
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
       <c r="N17" s="1">
         <f t="shared" si="3"/>
-        <v>-4.2</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C18">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0.12</v>
-      </c>
-      <c r="F18">
-        <v>-2</v>
+        <v>0.04</v>
       </c>
       <c r="M18">
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="3"/>
-        <v>-4.2</v>
+        <f t="shared" ref="N18:N50" si="4">C18-D18*20-E18*0.8-F18*0.6-H18*5+I18*10+J18/300</f>
+        <v>-0.8</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C19">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0.12</v>
-      </c>
-      <c r="F19">
-        <v>-2</v>
+        <v>0.02</v>
       </c>
       <c r="M19">
-        <v>1500</v>
+        <v>200</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" si="3"/>
-        <v>-4.2</v>
+        <f t="shared" si="4"/>
+        <v>-0.4</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>-1</v>
       </c>
       <c r="D20">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="M20">
-        <v>1300</v>
+        <v>900</v>
       </c>
       <c r="N20" s="1">
-        <f t="shared" si="3"/>
-        <v>-2.6</v>
-      </c>
-      <c r="P20">
-        <v>5.5</v>
+        <f t="shared" si="4"/>
+        <v>-2</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
-        <v>0.10249999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q21">
@@ -1879,281 +1996,240 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.02</v>
+      </c>
+      <c r="M22">
         <v>200</v>
       </c>
       <c r="N22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="N22:N28" si="5">C22-D22*20-E22*0.8-F22*0.6-H22*5+I22*10+J22/300</f>
         <v>-0.4</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
+        <f>P22*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.02</v>
+      </c>
+      <c r="M23">
+        <v>200</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.4</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" ref="Q23:Q50" si="6">P23*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.03</v>
+      </c>
+      <c r="M24">
+        <v>300</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.6</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.03</v>
+      </c>
+      <c r="M25">
+        <v>200</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.6</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26">
+        <v>-1</v>
+      </c>
+      <c r="D26">
+        <v>0.04</v>
+      </c>
+      <c r="M26">
+        <v>200</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.8</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27">
+        <v>-0.5</v>
+      </c>
+      <c r="D27">
         <v>0.05</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1">
-        <v>250</v>
-      </c>
-      <c r="N23" s="1">
-        <f t="shared" si="3"/>
+      <c r="M27">
+        <v>300</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.5</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28">
+        <v>-0.5</v>
+      </c>
+      <c r="D28">
+        <v>0.05</v>
+      </c>
+      <c r="M28">
+        <v>400</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.5</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29">
         <v>-1</v>
       </c>
-      <c r="Q23">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="D29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1">
-        <v>300</v>
-      </c>
-      <c r="N24" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.4000000000000001</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25">
+      <c r="M29">
+        <v>500</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.4000000000000004</v>
+      </c>
+      <c r="P29">
+        <v>3.5</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="6"/>
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30">
         <v>-1</v>
       </c>
-      <c r="D25">
+      <c r="D30">
         <v>0.04</v>
       </c>
-      <c r="M25">
-        <v>800</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.8</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1">
-        <v>1200</v>
-      </c>
-      <c r="N26" s="1">
-        <f t="shared" si="3"/>
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="P26">
-        <v>1.9</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="0"/>
-        <v>4.8500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1">
-        <v>1100</v>
-      </c>
-      <c r="N27" s="1">
-        <f t="shared" si="3"/>
-        <v>-2</v>
-      </c>
-      <c r="P27">
-        <v>1.4</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="0"/>
-        <v>4.0999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0.04</v>
-      </c>
-      <c r="M29">
-        <v>300</v>
-      </c>
-      <c r="N29" s="1">
-        <f t="shared" ref="N29:N55" si="4">C29-D29*20-E29*0.8-F29*0.6-H29*5+I29*10+J29/300</f>
-        <v>-0.8</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0.02</v>
-      </c>
       <c r="M30">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="N30" s="1">
         <f t="shared" si="4"/>
-        <v>-0.4</v>
+        <v>-1.8</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2162,623 +2238,1217 @@
         <v>0.05</v>
       </c>
       <c r="M31">
-        <v>900</v>
+        <v>550</v>
       </c>
       <c r="N31" s="1">
         <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32">
+        <v>-1</v>
+      </c>
+      <c r="D32">
+        <v>0.06</v>
+      </c>
+      <c r="M32">
+        <v>600</v>
+      </c>
       <c r="N32" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D33">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M33">
         <v>200</v>
       </c>
       <c r="N33" s="1">
         <f>C33-D33*20-E33*0.8-F33*0.6-H33*5+I33*10+J33/300</f>
-        <v>-0.4</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="Q33">
-        <f>P33*0.015+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D34">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="M34">
         <v>200</v>
       </c>
       <c r="N34" s="1">
         <f>C34-D34*20-E34*0.8-F34*0.6-H34*5+I34*10+J34/300</f>
-        <v>-0.4</v>
+        <v>-1.3</v>
       </c>
       <c r="Q34">
-        <f t="shared" ref="Q34:Q55" si="5">P34*0.015+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D35">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="M35">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="N35" s="1">
-        <f>C35-D35*20-E35*0.8-F35*0.6-H35*5+I35*10+J35/300</f>
-        <v>-0.6</v>
+        <f t="shared" si="4"/>
+        <v>-2.6</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+      <c r="R35">
+        <v>369.99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D36">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="M36">
-        <v>200</v>
+        <v>1100</v>
       </c>
       <c r="N36" s="1">
-        <f>C36-D36*20-E36*0.8-F36*0.6-H36*5+I36*10+J36/300</f>
-        <v>-0.6</v>
+        <f t="shared" si="4"/>
+        <v>-2.6</v>
+      </c>
+      <c r="P36">
+        <v>7.6</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.13399999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="C37">
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="M37">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="N37" s="1">
-        <f>C37-D37*20-E37*0.8-F37*0.6-H37*5+I37*10+J37/300</f>
-        <v>-1.8</v>
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C38">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="D38">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="M38">
-        <v>300</v>
+        <v>1300</v>
       </c>
       <c r="N38" s="1">
-        <f>C38-D38*20-E38*0.8-F38*0.6-H38*5+I38*10+J38/300</f>
-        <v>-1.5</v>
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="P38">
+        <v>3</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="R38">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C39">
         <v>-0.5</v>
       </c>
       <c r="D39">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="M39">
-        <v>400</v>
+        <v>1400</v>
       </c>
       <c r="N39" s="1">
-        <f>C39-D39*20-E39*0.8-F39*0.6-H39*5+I39*10+J39/300</f>
-        <v>-1.5</v>
+        <f t="shared" si="4"/>
+        <v>-2.5</v>
+      </c>
+      <c r="P39">
+        <v>5.2</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="R39">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="C40">
         <v>-1</v>
       </c>
       <c r="D40">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M40">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="N40" s="1">
         <f t="shared" si="4"/>
-        <v>-2.4000000000000004</v>
-      </c>
-      <c r="P40">
-        <v>3.5</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="5"/>
-        <v>7.2499999999999995E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+      <c r="R40">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="M41">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="N41" s="1">
         <f t="shared" si="4"/>
-        <v>-1.8</v>
+        <v>0.6</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="C42">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="M42">
-        <v>550</v>
+        <v>0</v>
       </c>
       <c r="N42" s="1">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>1.6</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="M43">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="N43" s="1">
         <f t="shared" si="4"/>
-        <v>-2.2000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C44">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="D44">
+        <v>0.01</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N45" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
         <v>0.03</v>
       </c>
-      <c r="M44">
-        <v>200</v>
-      </c>
-      <c r="N44" s="1">
-        <f>C44-D44*20-E44*0.8-F44*0.6-H44*5+I44*10+J44/300</f>
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="Q44">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45">
-        <v>-0.5</v>
-      </c>
-      <c r="D45">
-        <v>0.04</v>
-      </c>
-      <c r="M45">
-        <v>200</v>
-      </c>
-      <c r="N45" s="1">
-        <f>C45-D45*20-E45*0.8-F45*0.6-H45*5+I45*10+J45/300</f>
-        <v>-1.3</v>
-      </c>
-      <c r="Q45">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46">
-        <v>-1</v>
-      </c>
-      <c r="D46">
-        <v>0.08</v>
-      </c>
       <c r="M46">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N46" s="1">
         <f t="shared" si="4"/>
-        <v>-2.6</v>
+        <v>-0.6</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-      <c r="R46">
-        <v>369.99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C47">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D47">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="M47">
-        <v>1100</v>
+        <v>550</v>
       </c>
       <c r="N47" s="1">
         <f t="shared" si="4"/>
-        <v>-2.6</v>
-      </c>
-      <c r="P47">
-        <v>7.6</v>
+        <v>-1.3</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="5"/>
-        <v>0.13399999999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C48">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D48">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="M48">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="N48" s="1">
         <f t="shared" si="4"/>
-        <v>-2.2000000000000002</v>
+        <v>-1.5</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C49">
         <v>-1</v>
       </c>
       <c r="D49">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="M49">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="N49" s="1">
         <f t="shared" si="4"/>
-        <v>-2.2000000000000002</v>
+        <v>-2</v>
       </c>
       <c r="P49">
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="5"/>
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="6"/>
+        <v>5.1500000000000004E-2</v>
       </c>
       <c r="R49">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>100</v>
-      </c>
-      <c r="B50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50">
-        <v>-0.5</v>
-      </c>
-      <c r="D50">
-        <v>0.1</v>
-      </c>
-      <c r="M50">
-        <v>1400</v>
-      </c>
+        <v>599</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N50" s="1">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="6"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51">
         <v>-2.5</v>
       </c>
-      <c r="P50">
-        <v>5.2</v>
-      </c>
-      <c r="Q50">
-        <f t="shared" si="5"/>
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="R50">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51">
+      <c r="D51">
+        <v>0.2</v>
+      </c>
+      <c r="M51">
+        <v>1400</v>
+      </c>
+      <c r="N51" s="1">
+        <f t="shared" ref="N51:N65" si="7">C51-D51*20-E51*0.8-F51*0.6-H51*5+I51*10+J51/300</f>
+        <v>-6.5</v>
+      </c>
+      <c r="P51">
+        <v>12.3</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" ref="Q51:Q65" si="8">P51*0.015+0.02</f>
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="R51">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52">
+        <v>-2.5</v>
+      </c>
+      <c r="D52">
+        <v>0.18</v>
+      </c>
+      <c r="M52">
+        <v>1300</v>
+      </c>
+      <c r="N52" s="1">
+        <f t="shared" si="7"/>
+        <v>-6.1</v>
+      </c>
+      <c r="P52">
+        <v>11.5</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="8"/>
+        <v>0.19249999999999998</v>
+      </c>
+      <c r="R52">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53">
+        <v>-1.5</v>
+      </c>
+      <c r="D53">
+        <v>0.18</v>
+      </c>
+      <c r="M53">
+        <v>1100</v>
+      </c>
+      <c r="N53" s="1">
+        <f t="shared" si="7"/>
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="P53">
+        <v>11.5</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="8"/>
+        <v>0.19249999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54">
+        <v>-2.5</v>
+      </c>
+      <c r="D54">
+        <v>0.15</v>
+      </c>
+      <c r="M54">
+        <v>1800</v>
+      </c>
+      <c r="N54" s="1">
+        <f t="shared" si="7"/>
+        <v>-5.5</v>
+      </c>
+      <c r="P54">
+        <v>9</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="8"/>
+        <v>0.155</v>
+      </c>
+      <c r="R54">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55">
         <v>-1</v>
       </c>
-      <c r="D51">
-        <v>0.06</v>
-      </c>
-      <c r="M51">
-        <v>700</v>
-      </c>
-      <c r="N51" s="1">
-        <f t="shared" si="4"/>
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="Q51">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-      <c r="R51">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>0.02</v>
-      </c>
-      <c r="M52">
-        <v>0</v>
-      </c>
-      <c r="N52" s="1">
-        <f t="shared" si="4"/>
-        <v>0.6</v>
-      </c>
-      <c r="Q52">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53">
-        <v>0.02</v>
-      </c>
-      <c r="M53">
-        <v>0</v>
-      </c>
-      <c r="N53" s="1">
-        <f t="shared" si="4"/>
-        <v>1.6</v>
-      </c>
-      <c r="Q53">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>0.01</v>
-      </c>
-      <c r="M54">
-        <v>0</v>
-      </c>
-      <c r="N54" s="1">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
-      </c>
-      <c r="Q54">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
       <c r="D55">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
       <c r="M55">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="N55" s="1">
-        <f t="shared" si="4"/>
-        <v>0.8</v>
+        <f t="shared" si="7"/>
+        <v>-4</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56">
+        <v>-1</v>
+      </c>
+      <c r="D56">
+        <v>0.15</v>
+      </c>
+      <c r="M56">
+        <v>1700</v>
+      </c>
+      <c r="N56" s="1">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57">
+        <v>-1</v>
+      </c>
+      <c r="D57">
+        <v>0.15</v>
+      </c>
+      <c r="M57">
+        <v>2000</v>
+      </c>
+      <c r="N57" s="1">
+        <f t="shared" si="7"/>
+        <v>-4</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0.03</v>
+      </c>
+      <c r="M58">
+        <v>300</v>
+      </c>
+      <c r="N58" s="1">
+        <f>C58-D58*20-E58*0.8-F58*0.6-H58*5+I58*10+J58/300</f>
+        <v>-0.6</v>
+      </c>
+      <c r="Q58">
+        <f>P58*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0.03</v>
+      </c>
+      <c r="M59">
+        <v>300</v>
+      </c>
+      <c r="N59" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.6</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60">
+        <v>-2.5</v>
+      </c>
+      <c r="D60">
+        <v>0.11</v>
+      </c>
+      <c r="M60">
+        <v>1700</v>
+      </c>
+      <c r="N60" s="1">
+        <f t="shared" si="7"/>
+        <v>-4.7</v>
+      </c>
+      <c r="P60">
+        <v>11.2</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="8"/>
+        <v>0.18799999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61">
+        <v>-1</v>
+      </c>
+      <c r="D61">
+        <v>0.11</v>
+      </c>
+      <c r="M61">
+        <v>1500</v>
+      </c>
+      <c r="N61" s="1">
+        <f t="shared" si="7"/>
+        <v>-3.2</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62">
+        <v>-1</v>
+      </c>
+      <c r="D62">
+        <v>0.11</v>
+      </c>
+      <c r="M62">
+        <v>1600</v>
+      </c>
+      <c r="N62" s="1">
+        <f>C62-D62*20-E62*0.8-F62*0.6-H62*5+I62*10+J62/300</f>
+        <v>-3.2</v>
+      </c>
+      <c r="Q62">
+        <f>P62*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>146</v>
+      </c>
+      <c r="B63" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63" s="1">
+        <f>C63-D63*20-E63*0.8-F63*0.6-H63*5+I63*10+J63/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <f>P63*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="8"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>150</v>
+      </c>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66" s="1">
+        <f>C66-D66*20-E66*0.8-F66*0.6-H66*5+I66*10+J66/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <f>P66*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1">
+        <v>400</v>
+      </c>
+      <c r="N68" s="1">
+        <f>C68-D68*20-E68*0.8-F68*0.6-H68*5+I68*10+J68/300</f>
+        <v>-0.8</v>
+      </c>
+      <c r="Q68">
+        <f>P68*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1">
+        <v>200</v>
+      </c>
+      <c r="N69" s="1">
+        <f>C69-D69*20-E69*0.8-F69*0.6-H69*5+I69*10+J69/300</f>
+        <v>-0.4</v>
+      </c>
+      <c r="Q69">
+        <f>P69*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>54</v>
+      </c>
+      <c r="B70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0.03</v>
+      </c>
+      <c r="M70">
+        <v>350</v>
+      </c>
+      <c r="N70" s="1">
+        <f>C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
+        <v>-0.6</v>
+      </c>
+      <c r="Q70">
+        <f>P70*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0.03</v>
+      </c>
+      <c r="M71">
+        <v>200</v>
+      </c>
+      <c r="N71" s="1">
+        <f>C71-D71*20-E71*0.8-F71*0.6-H71*5+I71*10+J71/300</f>
+        <v>-0.6</v>
+      </c>
+      <c r="Q71">
+        <f>P71*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0.05</v>
+      </c>
+      <c r="M72">
+        <v>100</v>
+      </c>
+      <c r="N72" s="1">
+        <f>C72-D72*20-E72*0.8-F72*0.6-H72*5+I72*10+J72/300</f>
+        <v>-1</v>
+      </c>
+      <c r="Q72">
+        <f>P72*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C73">
+        <v>-3</v>
+      </c>
+      <c r="D73">
+        <v>0.12</v>
+      </c>
+      <c r="F73">
+        <v>-2</v>
+      </c>
+      <c r="M73">
+        <v>1200</v>
+      </c>
+      <c r="N73" s="1">
+        <f>C73-D73*20-E73*0.8-F73*0.6-H73*5+I73*10+J73/300</f>
+        <v>-4.2</v>
+      </c>
+      <c r="P73">
+        <v>7.9</v>
+      </c>
+      <c r="Q73">
+        <f>P73*0.015+0.02</f>
+        <v>0.13849999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74">
+        <v>-3</v>
+      </c>
+      <c r="D74">
+        <v>0.12</v>
+      </c>
+      <c r="F74">
+        <v>-2</v>
+      </c>
+      <c r="M74">
+        <v>1200</v>
+      </c>
+      <c r="N74" s="1">
+        <f>C74-D74*20-E74*0.8-F74*0.6-H74*5+I74*10+J74/300</f>
+        <v>-4.2</v>
+      </c>
+      <c r="Q74">
+        <f>P74*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75">
+        <v>-3</v>
+      </c>
+      <c r="D75">
+        <v>0.12</v>
+      </c>
+      <c r="F75">
+        <v>-2</v>
+      </c>
+      <c r="M75">
+        <v>1500</v>
+      </c>
+      <c r="N75" s="1">
+        <f>C75-D75*20-E75*0.8-F75*0.6-H75*5+I75*10+J75/300</f>
+        <v>-4.2</v>
+      </c>
+      <c r="Q75">
+        <f>P75*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>62</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76">
+        <v>-3</v>
+      </c>
+      <c r="D76">
+        <v>0.12</v>
+      </c>
+      <c r="F76">
+        <v>-2</v>
+      </c>
+      <c r="M76">
+        <v>1500</v>
+      </c>
+      <c r="N76" s="1">
+        <f>C76-D76*20-E76*0.8-F76*0.6-H76*5+I76*10+J76/300</f>
+        <v>-4.2</v>
+      </c>
+      <c r="Q76">
+        <f>P76*0.015+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77">
+        <v>-1</v>
+      </c>
+      <c r="D77">
+        <v>0.08</v>
+      </c>
+      <c r="M77">
+        <v>1300</v>
+      </c>
+      <c r="N77" s="1">
+        <f>C77-D77*20-E77*0.8-F77*0.6-H77*5+I77*10+J77/300</f>
+        <v>-2.6</v>
+      </c>
+      <c r="P77">
+        <v>5.5</v>
+      </c>
+      <c r="Q77">
+        <f>P77*0.015+0.02</f>
+        <v>0.10249999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1">
+        <f>C78-D78*20-E78*0.8-F78*0.6-H78*5+I78*10+J78/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <f>P78*0.015+0.02</f>
         <v>0.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjust small red dots
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A8E423-738B-44A8-BC09-EC2978A81C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F87044F-D623-49EA-908E-6081CA0B9689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K98" sqref="K98"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,7 +1818,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D6" s="1">
         <v>0.04</v>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" ref="N6:N10" si="2">C6-D6*20-E6*0.8-F6*0.6-H6*5+I6*10+J6/300</f>
-        <v>-1.8</v>
+        <v>-2.8</v>
       </c>
       <c r="P6">
         <v>1.2</v>
@@ -1857,7 +1857,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D7" s="1">
         <v>0.04</v>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="N7" s="1">
         <f t="shared" si="2"/>
-        <v>-1.8</v>
+        <v>-2.8</v>
       </c>
       <c r="P7">
         <v>1.2</v>
@@ -1896,7 +1896,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D8" s="1">
         <v>0.04</v>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="N8" s="1">
         <f t="shared" si="2"/>
-        <v>-1.8</v>
+        <v>-2.8</v>
       </c>
       <c r="P8">
         <v>1.2</v>
@@ -2096,7 +2096,7 @@
         <v>43</v>
       </c>
       <c r="C14">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D14">
         <v>0.04</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="N14" s="1">
         <f t="shared" si="3"/>
-        <v>-1.8</v>
+        <v>-2.8</v>
       </c>
       <c r="Q14">
         <f t="shared" si="1"/>
@@ -2121,7 +2121,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="1">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="D15" s="1">
         <v>0.05</v>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="P15">
         <v>1.9</v>
@@ -2157,7 +2157,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="1">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="D16" s="1">
         <v>0.05</v>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="P16">
         <v>1.4</v>
@@ -2266,7 +2266,7 @@
         <v>53</v>
       </c>
       <c r="C20">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="D20">
         <v>0.05</v>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="N20" s="1">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="Q20">
         <f t="shared" si="1"/>
@@ -3469,11 +3469,11 @@
         <v>200</v>
       </c>
       <c r="N68" s="1">
-        <f>C68-D68*20-E68*0.8-F68*0.6-H68*5+I68*10+J68/300</f>
+        <f t="shared" ref="N68:N78" si="8">C68-D68*20-E68*0.8-F68*0.6-H68*5+I68*10+J68/300</f>
         <v>-0.8</v>
       </c>
       <c r="Q68">
-        <f>P68*0.013+0.02</f>
+        <f t="shared" ref="Q68:Q78" si="9">P68*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
@@ -3494,14 +3494,14 @@
         <v>900</v>
       </c>
       <c r="N69" s="1">
-        <f>C69-D69*20-E69*0.8-F69*0.6-H69*5+I69*10+J69/300</f>
+        <f t="shared" si="8"/>
         <v>-3.6</v>
       </c>
       <c r="P69">
         <v>4.2</v>
       </c>
       <c r="Q69">
-        <f>P69*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>7.46E-2</v>
       </c>
     </row>
@@ -3522,21 +3522,21 @@
         <v>900</v>
       </c>
       <c r="N70" s="1">
-        <f>C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
+        <f t="shared" si="8"/>
         <v>-3.6</v>
       </c>
       <c r="Q70">
-        <f>P70*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N71" s="1">
-        <f>C71-D71*20-E71*0.8-F71*0.6-H71*5+I71*10+J71/300</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q71">
-        <f>P71*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3557,11 +3557,11 @@
         <v>200</v>
       </c>
       <c r="N72" s="1">
-        <f>C72-D72*20-E72*0.8-F72*0.6-H72*5+I72*10+J72/300</f>
+        <f t="shared" si="8"/>
         <v>-1.1000000000000001</v>
       </c>
       <c r="Q72">
-        <f>P72*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3582,11 +3582,11 @@
         <v>300</v>
       </c>
       <c r="N73" s="1">
-        <f>C73-D73*20-E73*0.8-F73*0.6-H73*5+I73*10+J73/300</f>
+        <f t="shared" si="8"/>
         <v>-2.2000000000000002</v>
       </c>
       <c r="Q73">
-        <f>P73*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3607,24 +3607,24 @@
         <v>800</v>
       </c>
       <c r="N74" s="1">
-        <f>C74-D74*20-E74*0.8-F74*0.6-H74*5+I74*10+J74/300</f>
+        <f t="shared" si="8"/>
         <v>-4.2</v>
       </c>
       <c r="P74">
         <v>7.1</v>
       </c>
       <c r="Q74">
-        <f>P74*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.1123</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N75" s="1">
-        <f>C75-D75*20-E75*0.8-F75*0.6-H75*5+I75*10+J75/300</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q75">
-        <f>P75*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3645,11 +3645,11 @@
         <v>300</v>
       </c>
       <c r="N76" s="1">
-        <f>C76-D76*20-E76*0.8-F76*0.6-H76*5+I76*10+J76/300</f>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="Q76">
-        <f>P76*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3670,24 +3670,24 @@
         <v>1000</v>
       </c>
       <c r="N77" s="1">
-        <f>C77-D77*20-E77*0.8-F77*0.6-H77*5+I77*10+J77/300</f>
+        <f t="shared" si="8"/>
         <v>-5.4</v>
       </c>
       <c r="P77">
         <v>15.8</v>
       </c>
       <c r="Q77">
-        <f>P77*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.22539999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N78" s="1">
-        <f>C78-D78*20-E78*0.8-F78*0.6-H78*5+I78*10+J78/300</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q78">
-        <f>P78*0.013+0.02</f>
+        <f t="shared" si="9"/>
         <v>0.02</v>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
         <v>3.1746569999999998</v>
       </c>
       <c r="Q79">
-        <f t="shared" ref="Q79:Q102" si="8">P79*0.013+0.02</f>
+        <f t="shared" ref="Q79:Q102" si="10">P79*0.013+0.02</f>
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
@@ -3743,7 +3743,7 @@
         <v>8</v>
       </c>
       <c r="Q80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.124</v>
       </c>
     </row>
@@ -3771,7 +3771,7 @@
         <v>5.6085599999999998</v>
       </c>
       <c r="Q81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
         <v>13.4041</v>
       </c>
       <c r="Q82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.19425329999999999</v>
       </c>
     </row>
@@ -3830,7 +3830,7 @@
         <v>4</v>
       </c>
       <c r="Q83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
@@ -3861,7 +3861,7 @@
         <v>9.6</v>
       </c>
       <c r="Q84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.14479999999999998</v>
       </c>
     </row>
@@ -3889,7 +3889,7 @@
         <v>10.5116</v>
       </c>
       <c r="Q85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.15665079999999998</v>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
         <v>10.93493</v>
       </c>
       <c r="Q86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.16215408999999997</v>
       </c>
     </row>
@@ -3945,7 +3945,7 @@
         <v>10.9</v>
       </c>
       <c r="Q87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.16169999999999998</v>
       </c>
     </row>
@@ -3973,7 +3973,7 @@
         <v>13.9</v>
       </c>
       <c r="Q88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.20069999999999999</v>
       </c>
     </row>
@@ -3998,7 +3998,7 @@
         <v>-5.4</v>
       </c>
       <c r="Q89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
         <v>11.6</v>
       </c>
       <c r="Q90">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.17079999999999998</v>
       </c>
     </row>
@@ -4036,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="Q91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4069,7 +4069,7 @@
         <v>-0.8</v>
       </c>
       <c r="Q92">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4102,7 +4102,7 @@
         <v>-0.4</v>
       </c>
       <c r="Q93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4127,7 +4127,7 @@
         <v>-0.6</v>
       </c>
       <c r="Q94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4152,7 +4152,7 @@
         <v>-0.6</v>
       </c>
       <c r="Q95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4177,7 +4177,7 @@
         <v>-1</v>
       </c>
       <c r="Q96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4198,14 +4198,14 @@
         <v>1200</v>
       </c>
       <c r="N97" s="1">
-        <f t="shared" ref="N97:N139" si="9">C97-D97*20-E97*0.8-F97*0.6-H97*5+I97*10+J97/300</f>
+        <f t="shared" ref="N97:N139" si="11">C97-D97*20-E97*0.8-F97*0.6-H97*5+I97*10+J97/300</f>
         <v>-5.4</v>
       </c>
       <c r="P97">
         <v>7.9</v>
       </c>
       <c r="Q97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.1227</v>
       </c>
     </row>
@@ -4226,11 +4226,11 @@
         <v>1200</v>
       </c>
       <c r="N98" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-5.4</v>
       </c>
       <c r="Q98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4251,11 +4251,11 @@
         <v>1500</v>
       </c>
       <c r="N99" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-5.4</v>
       </c>
       <c r="Q99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4276,11 +4276,11 @@
         <v>1500</v>
       </c>
       <c r="N100" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-5.4</v>
       </c>
       <c r="Q100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4301,14 +4301,14 @@
         <v>1300</v>
       </c>
       <c r="N101" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-2.6</v>
       </c>
       <c r="P101">
         <v>5.5</v>
       </c>
       <c r="Q101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
@@ -4327,11 +4327,11 @@
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
       <c r="N102" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Q102">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4459,11 +4459,11 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N108" s="1">
-        <f t="shared" ref="N108:N136" si="10">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
+        <f t="shared" ref="N108:N136" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
         <v>0</v>
       </c>
       <c r="Q108">
-        <f t="shared" ref="Q108:Q139" si="11">P108*0.013+0.02</f>
+        <f t="shared" ref="Q108:Q139" si="13">P108*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
@@ -4484,11 +4484,11 @@
         <v>400</v>
       </c>
       <c r="N109" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
       <c r="Q109">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4509,24 +4509,24 @@
         <v>750</v>
       </c>
       <c r="N110" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
       <c r="P110">
         <v>10.5822</v>
       </c>
       <c r="Q110">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.15756859999999998</v>
       </c>
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N111" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q111">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4547,11 +4547,11 @@
         <v>400</v>
       </c>
       <c r="N112" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
       <c r="Q112">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4572,14 +4572,14 @@
         <v>750</v>
       </c>
       <c r="N113" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.3000000000000007</v>
       </c>
       <c r="P113">
         <v>9.5239700000000003</v>
       </c>
       <c r="Q113">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.14381161000000001</v>
       </c>
     </row>
@@ -4600,21 +4600,21 @@
         <v>800</v>
       </c>
       <c r="N114" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
       <c r="Q114">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N115" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q115">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4635,14 +4635,14 @@
         <v>400</v>
       </c>
       <c r="N116" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
       <c r="P116">
         <v>4</v>
       </c>
       <c r="Q116">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
@@ -4663,11 +4663,11 @@
         <v>400</v>
       </c>
       <c r="N117" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
       <c r="Q117">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4691,14 +4691,14 @@
         <v>1000</v>
       </c>
       <c r="N118" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.4</v>
       </c>
       <c r="P118">
         <v>16.600000000000001</v>
       </c>
       <c r="Q118">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.23580000000000001</v>
       </c>
     </row>
@@ -4722,14 +4722,14 @@
         <v>1750</v>
       </c>
       <c r="N119" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.6</v>
       </c>
       <c r="P119">
         <v>17.600000000000001</v>
       </c>
       <c r="Q119">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.24879999999999999</v>
       </c>
     </row>
@@ -4753,24 +4753,24 @@
         <v>1500</v>
       </c>
       <c r="N120" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
       <c r="P120">
         <v>15.6</v>
       </c>
       <c r="Q120">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.22279999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N121" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q121">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4791,14 +4791,14 @@
         <v>1000</v>
       </c>
       <c r="N122" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.6</v>
       </c>
       <c r="P122">
         <v>6.5</v>
       </c>
       <c r="Q122">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.1045</v>
       </c>
     </row>
@@ -4819,14 +4819,14 @@
         <v>800</v>
       </c>
       <c r="N123" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.2</v>
       </c>
       <c r="P123">
         <v>8.6999999999999993</v>
       </c>
       <c r="Q123">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.1331</v>
       </c>
     </row>
@@ -4847,14 +4847,14 @@
         <v>750</v>
       </c>
       <c r="N124" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.5</v>
       </c>
       <c r="P124">
         <v>7.5</v>
       </c>
       <c r="Q124">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.11749999999999999</v>
       </c>
     </row>
@@ -4875,14 +4875,14 @@
         <v>500</v>
       </c>
       <c r="N125" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.8</v>
       </c>
       <c r="P125">
         <v>6.7</v>
       </c>
       <c r="Q125">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.1071</v>
       </c>
     </row>
@@ -4903,11 +4903,11 @@
         <v>500</v>
       </c>
       <c r="N126" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3</v>
       </c>
       <c r="Q126">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4931,24 +4931,24 @@
         <v>4000</v>
       </c>
       <c r="N127" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-9.4000000000000021</v>
       </c>
       <c r="P127">
         <v>20.100000000000001</v>
       </c>
       <c r="Q127">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.28130000000000005</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N128" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q128">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -4969,14 +4969,14 @@
         <v>1000</v>
       </c>
       <c r="N129" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-2.8</v>
       </c>
       <c r="P129">
         <v>6.6</v>
       </c>
       <c r="Q129">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.10579999999999999</v>
       </c>
     </row>
@@ -4997,14 +4997,14 @@
         <v>500</v>
       </c>
       <c r="N130" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-3.2</v>
       </c>
       <c r="P130">
         <v>7.0195183999999999</v>
       </c>
       <c r="Q130">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.11125373919999999</v>
       </c>
     </row>
@@ -5028,24 +5028,24 @@
         <v>5000</v>
       </c>
       <c r="N131" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-13</v>
       </c>
       <c r="P131">
         <v>39.299999999999997</v>
       </c>
       <c r="Q131">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.53089999999999993</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N132" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
@@ -5074,14 +5074,14 @@
         <v>1000</v>
       </c>
       <c r="N133" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
       <c r="P133">
         <v>15</v>
       </c>
       <c r="Q133">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.21499999999999997</v>
       </c>
     </row>
@@ -5105,14 +5105,14 @@
         <v>1000</v>
       </c>
       <c r="N134" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-6.3000000000000007</v>
       </c>
       <c r="P134">
         <v>15.4</v>
       </c>
       <c r="Q134">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
@@ -5136,14 +5136,14 @@
         <v>2000</v>
       </c>
       <c r="N135" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-9</v>
       </c>
       <c r="P135">
         <v>17.3</v>
       </c>
       <c r="Q135">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
@@ -5167,14 +5167,14 @@
         <v>3000</v>
       </c>
       <c r="N136" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-7.8000000000000016</v>
       </c>
       <c r="P136">
         <v>24.162700000000001</v>
       </c>
       <c r="Q136">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
@@ -5198,14 +5198,14 @@
         <v>3000</v>
       </c>
       <c r="N137" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-6.6</v>
       </c>
       <c r="P137">
         <v>17.399999999999999</v>
       </c>
       <c r="Q137">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
@@ -5229,14 +5229,14 @@
         <v>5000</v>
       </c>
       <c r="N138" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-8.0000000000000018</v>
       </c>
       <c r="P138">
         <v>21.9</v>
       </c>
       <c r="Q138">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
@@ -5260,14 +5260,14 @@
         <v>2000</v>
       </c>
       <c r="N139" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-7.2</v>
       </c>
       <c r="P139">
         <v>19.3</v>
       </c>
       <c r="Q139">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add barska scope and fix other carry handle scopes
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7B4AD7-C89C-4105-9E14-8AD8BCB75938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C8E3D7-AEC2-4180-9CE4-111958BE597A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="280">
   <si>
     <t>new</t>
   </si>
@@ -840,6 +840,39 @@
   </si>
   <si>
     <t>Badger Ordnance C.O.M.M. T1/T2 Sight</t>
+  </si>
+  <si>
+    <t>barska_4x20_scope_carry_handle_mount</t>
+  </si>
+  <si>
+    <t>Barska 4x20 Scope Carry Handle Mount</t>
+  </si>
+  <si>
+    <t>barska_eletrco_4x20_bdc_scope</t>
+  </si>
+  <si>
+    <t>Barska Electro 4x20 BDC Turret Scope</t>
+  </si>
+  <si>
+    <t>colt_retro_a1_scope_carry_handle_mount</t>
+  </si>
+  <si>
+    <t>Colt Retro A1 Scope Carry Handle Mount</t>
+  </si>
+  <si>
+    <t>colt_retro_a1_4x21_scope</t>
+  </si>
+  <si>
+    <t>Colt Retro A1 4x21 Scope</t>
+  </si>
+  <si>
+    <t>trijicon_ta01nsn_carry_handle</t>
+  </si>
+  <si>
+    <t>burris_prism_ar332_carry_handle</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta11d_bac_carry_handle</t>
   </si>
 </sst>
 </file>
@@ -1681,20 +1714,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R158"/>
+  <dimension ref="A1:R165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="21" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="57.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="21" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1712,7 +1745,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1765,7 +1798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1798,7 +1831,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1831,7 +1864,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1864,7 +1897,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1903,7 +1936,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1942,7 +1975,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1981,7 +2014,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2020,7 +2053,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2043,7 +2076,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2076,7 +2109,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2109,7 +2142,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2142,7 +2175,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2200,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -2203,7 +2236,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -2239,7 +2272,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2262,7 +2295,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2287,7 +2320,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2312,7 +2345,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2337,7 +2370,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N21" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2347,7 +2380,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2372,7 +2405,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -2397,7 +2430,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2422,7 +2455,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2447,7 +2480,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2472,7 +2505,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2497,7 +2530,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2522,7 +2555,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2550,7 +2583,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2575,7 +2608,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2600,7 +2633,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2625,7 +2658,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -2650,7 +2683,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -2675,7 +2708,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2703,7 +2736,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2731,7 +2764,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2756,7 +2789,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2787,7 +2820,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2818,7 +2851,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -2846,7 +2879,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2871,7 +2904,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -2896,7 +2929,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -2921,7 +2954,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -2946,7 +2979,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N45" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2956,7 +2989,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -2981,7 +3014,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -3006,7 +3039,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>116</v>
       </c>
@@ -3031,7 +3064,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -3062,7 +3095,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N50" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3072,7 +3105,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>120</v>
       </c>
@@ -3103,7 +3136,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -3134,7 +3167,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -3162,7 +3195,7 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>130</v>
       </c>
@@ -3193,7 +3226,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -3218,7 +3251,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -3243,7 +3276,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>136</v>
       </c>
@@ -3268,7 +3301,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -3293,7 +3326,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>140</v>
       </c>
@@ -3318,7 +3351,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -3346,7 +3379,7 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3371,7 +3404,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -3396,7 +3429,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -3421,7 +3454,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -3446,7 +3479,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -3471,7 +3504,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>150</v>
       </c>
@@ -3496,7 +3529,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N67" s="1">
         <f t="shared" ref="N67:N96" si="7">C67-D67*20-E67*0.8-F67*0.6-H67*5+I67*10+J67/300</f>
         <v>0</v>
@@ -3506,7 +3539,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -3531,7 +3564,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>178</v>
       </c>
@@ -3559,7 +3592,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>180</v>
       </c>
@@ -3584,7 +3617,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N71" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3594,7 +3627,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>197</v>
       </c>
@@ -3619,7 +3652,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>195</v>
       </c>
@@ -3644,7 +3677,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>199</v>
       </c>
@@ -3672,7 +3705,7 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N75" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3682,7 +3715,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>201</v>
       </c>
@@ -3707,7 +3740,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>203</v>
       </c>
@@ -3735,7 +3768,7 @@
         <v>0.22539999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N78" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3745,7 +3778,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -3773,7 +3806,7 @@
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -3801,7 +3834,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>156</v>
       </c>
@@ -3829,7 +3862,7 @@
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -3857,7 +3890,7 @@
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3888,7 +3921,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -3919,7 +3952,7 @@
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -3947,7 +3980,7 @@
         <v>0.15665079999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -3975,7 +4008,7 @@
         <v>0.16215408999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>166</v>
       </c>
@@ -4003,7 +4036,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>168</v>
       </c>
@@ -4031,7 +4064,7 @@
         <v>0.20069999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -4056,7 +4089,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -4084,7 +4117,7 @@
         <v>0.17079999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N91" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4094,7 +4127,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>32</v>
       </c>
@@ -4127,7 +4160,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>34</v>
       </c>
@@ -4160,7 +4193,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>54</v>
       </c>
@@ -4185,7 +4218,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>56</v>
       </c>
@@ -4210,7 +4243,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>64</v>
       </c>
@@ -4235,7 +4268,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -4263,7 +4296,7 @@
         <v>0.1227</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>60</v>
       </c>
@@ -4288,7 +4321,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>61</v>
       </c>
@@ -4313,7 +4346,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>62</v>
       </c>
@@ -4338,7 +4371,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4366,7 +4399,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4389,7 +4422,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -4414,7 +4447,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -4445,7 +4478,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N105" s="1">
         <f>C105-D105*20-E105*0.8-F105*0.6-H105*5+I105*10+J105/300</f>
         <v>0</v>
@@ -4455,7 +4488,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>209</v>
       </c>
@@ -4480,7 +4513,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>211</v>
       </c>
@@ -4511,17 +4544,17 @@
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N108" s="1">
-        <f t="shared" ref="N108:N134" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
+        <f t="shared" ref="N108:N137" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
         <v>0</v>
       </c>
       <c r="Q108">
-        <f t="shared" ref="Q108:Q149" si="13">P108*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q108:Q152" si="13">P108*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>213</v>
       </c>
@@ -4546,7 +4579,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -4574,7 +4607,7 @@
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N111" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4584,7 +4617,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -4609,7 +4642,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>219</v>
       </c>
@@ -4637,7 +4670,7 @@
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -4662,7 +4695,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N115" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4672,7 +4705,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>225</v>
       </c>
@@ -4700,7 +4733,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>223</v>
       </c>
@@ -4725,7 +4758,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -4756,237 +4789,246 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="B119" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C119">
         <v>-3</v>
       </c>
       <c r="D119">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F119">
         <v>-2</v>
       </c>
       <c r="M119">
-        <v>1750</v>
+        <v>1000</v>
       </c>
       <c r="N119" s="1">
         <f t="shared" si="12"/>
-        <v>-6.6</v>
-      </c>
-      <c r="P119">
-        <v>17.600000000000001</v>
+        <v>-6.4</v>
       </c>
       <c r="Q119">
         <f t="shared" si="13"/>
-        <v>0.24879999999999999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B120" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C120">
         <v>-3</v>
       </c>
       <c r="D120">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="F120">
         <v>-2</v>
       </c>
       <c r="M120">
-        <v>1500</v>
+        <v>1750</v>
       </c>
       <c r="N120" s="1">
         <f t="shared" si="12"/>
-        <v>-6.2</v>
+        <v>-6.6</v>
       </c>
       <c r="P120">
-        <v>15.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="Q120">
         <f t="shared" si="13"/>
-        <v>0.22279999999999997</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.24879999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>279</v>
+      </c>
+      <c r="B121" t="s">
+        <v>230</v>
+      </c>
+      <c r="C121">
+        <v>-3</v>
+      </c>
+      <c r="D121">
+        <v>0.24</v>
+      </c>
+      <c r="F121">
+        <v>-2</v>
+      </c>
+      <c r="M121">
+        <v>1750</v>
+      </c>
       <c r="N121" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-6.6</v>
       </c>
       <c r="Q121">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B122" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C122">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="D122">
-        <v>0.06</v>
+        <v>0.22</v>
+      </c>
+      <c r="F122">
+        <v>-2</v>
       </c>
       <c r="M122">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="N122" s="1">
         <f t="shared" si="12"/>
-        <v>-1.7</v>
+        <v>-6.2</v>
       </c>
       <c r="P122">
-        <v>6.5</v>
+        <v>15.6</v>
       </c>
       <c r="Q122">
         <f t="shared" si="13"/>
-        <v>0.1045</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.22279999999999997</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>251</v>
+        <v>277</v>
       </c>
       <c r="B123" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D123">
-        <v>0.01</v>
+        <v>0.22</v>
+      </c>
+      <c r="F123">
+        <v>-2</v>
       </c>
       <c r="M123">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="N123" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>-6.2</v>
       </c>
       <c r="Q123">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>257</v>
-      </c>
-      <c r="B124" t="s">
-        <v>258</v>
-      </c>
-      <c r="C124">
-        <v>0</v>
-      </c>
-      <c r="D124">
-        <v>0.03</v>
-      </c>
-      <c r="M124">
-        <v>200</v>
-      </c>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N124" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="Q124">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="B125" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D125">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="M125">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="N125" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-1.7</v>
+      </c>
+      <c r="P125">
+        <v>6.5</v>
       </c>
       <c r="Q125">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.1045</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B126" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C126">
         <v>0</v>
       </c>
       <c r="D126">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="M126">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N126" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>-0.2</v>
       </c>
       <c r="Q126">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B127" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C127">
         <v>0</v>
       </c>
       <c r="D127">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="M127">
         <v>200</v>
       </c>
       <c r="N127" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>-0.6</v>
       </c>
       <c r="Q127">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B128" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -4995,7 +5037,7 @@
         <v>0.02</v>
       </c>
       <c r="M128">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N128" s="1">
         <f t="shared" si="12"/>
@@ -5006,608 +5048,807 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B129" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C129">
         <v>0</v>
       </c>
       <c r="D129">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M129">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N129" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="Q129">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="B130" t="s">
-        <v>236</v>
+        <v>264</v>
       </c>
       <c r="C130">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
       <c r="M130">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="N130" s="1">
         <f t="shared" si="12"/>
-        <v>-3.2</v>
-      </c>
-      <c r="P130">
-        <v>8.6999999999999993</v>
+        <v>-0.2</v>
       </c>
       <c r="Q130">
         <f t="shared" si="13"/>
-        <v>0.1331</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="B131" t="s">
-        <v>238</v>
+        <v>266</v>
       </c>
       <c r="C131">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M131">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="N131" s="1">
         <f t="shared" si="12"/>
-        <v>-3.5</v>
-      </c>
-      <c r="P131">
-        <v>7.5</v>
+        <v>-0.4</v>
       </c>
       <c r="Q131">
         <f t="shared" si="13"/>
-        <v>0.11749999999999999</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="B132" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="C132">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="M132">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N132" s="1">
         <f t="shared" si="12"/>
-        <v>-2.8</v>
-      </c>
-      <c r="P132">
-        <v>6.7</v>
+        <v>-0.4</v>
       </c>
       <c r="Q132">
         <f t="shared" si="13"/>
-        <v>0.1071</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B133" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C133">
         <v>-1</v>
       </c>
       <c r="D133">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="M133">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="N133" s="1">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-3.2</v>
+      </c>
+      <c r="P133">
+        <v>8.6999999999999993</v>
       </c>
       <c r="Q133">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.1331</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B134" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C134">
-        <v>-5</v>
+        <v>-1.5</v>
       </c>
       <c r="D134">
-        <v>0.27</v>
-      </c>
-      <c r="F134">
-        <v>-2</v>
+        <v>0.1</v>
       </c>
       <c r="M134">
-        <v>4000</v>
+        <v>750</v>
       </c>
       <c r="N134" s="1">
         <f t="shared" si="12"/>
-        <v>-9.2000000000000011</v>
+        <v>-3.5</v>
       </c>
       <c r="P134">
-        <v>20.100000000000001</v>
+        <v>7.5</v>
       </c>
       <c r="Q134">
         <f t="shared" si="13"/>
-        <v>0.28130000000000005</v>
-      </c>
-    </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.11749999999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>239</v>
+      </c>
+      <c r="B135" t="s">
+        <v>240</v>
+      </c>
+      <c r="C135">
+        <v>-1</v>
+      </c>
+      <c r="D135">
+        <v>0.09</v>
+      </c>
+      <c r="M135">
+        <v>500</v>
+      </c>
       <c r="N135" s="1">
-        <f>C135-D135*20-E135*0.8-F135*0.6-H135*5+I135*10+J135/300</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-2.8</v>
+      </c>
+      <c r="P135">
+        <v>6.7</v>
       </c>
       <c r="Q135">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.1071</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B136" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C136">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="D136">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="M136">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N136" s="1">
-        <f>C136-D136*20-E136*0.8-F136*0.6-H136*5+I136*10+J136/300</f>
-        <v>-1.9000000000000001</v>
-      </c>
-      <c r="P136">
-        <v>6.6</v>
+        <f t="shared" si="12"/>
+        <v>-3</v>
       </c>
       <c r="Q136">
         <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>243</v>
+      </c>
+      <c r="B137" t="s">
+        <v>244</v>
+      </c>
+      <c r="C137">
+        <v>-5</v>
+      </c>
+      <c r="D137">
+        <v>0.27</v>
+      </c>
+      <c r="F137">
+        <v>-2</v>
+      </c>
+      <c r="M137">
+        <v>4000</v>
+      </c>
+      <c r="N137" s="1">
+        <f t="shared" si="12"/>
+        <v>-9.2000000000000011</v>
+      </c>
+      <c r="P137">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q137">
+        <f t="shared" si="13"/>
+        <v>0.28130000000000005</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N138" s="1">
+        <f t="shared" ref="N138:N153" si="14">C138-D138*20-E138*0.8-F138*0.6-H138*5+I138*10+J138/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q138">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>247</v>
+      </c>
+      <c r="B139" t="s">
+        <v>248</v>
+      </c>
+      <c r="C139">
+        <v>-0.5</v>
+      </c>
+      <c r="D139">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M139">
+        <v>1000</v>
+      </c>
+      <c r="N139" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.9000000000000001</v>
+      </c>
+      <c r="P139">
+        <v>6.6</v>
+      </c>
+      <c r="Q139">
+        <f t="shared" si="13"/>
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>253</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B140" t="s">
         <v>254</v>
       </c>
-      <c r="C137">
-        <v>0</v>
-      </c>
-      <c r="D137">
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
         <v>0.01</v>
       </c>
-      <c r="M137">
-        <v>0</v>
-      </c>
-      <c r="N137" s="1">
-        <f>C137-D137*20-E137*0.8-F137*0.6-H137*5+I137*10+J137/300</f>
+      <c r="M140">
+        <v>0</v>
+      </c>
+      <c r="N140" s="1">
+        <f t="shared" si="14"/>
         <v>-0.2</v>
       </c>
-      <c r="Q137">
-        <f>P137*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="Q140">
+        <f>P140*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>255</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B141" t="s">
         <v>256</v>
       </c>
-      <c r="C138">
-        <v>0</v>
-      </c>
-      <c r="D138">
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141">
         <v>0.03</v>
       </c>
-      <c r="M138">
+      <c r="M141">
         <v>200</v>
       </c>
-      <c r="N138" s="1">
-        <f>C138-D138*20-E138*0.8-F138*0.6-H138*5+I138*10+J138/300</f>
+      <c r="N141" s="1">
+        <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q138">
-        <f>P138*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="Q141">
+        <f>P141*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>259</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B142" t="s">
         <v>256</v>
       </c>
-      <c r="C139">
-        <v>0</v>
-      </c>
-      <c r="D139">
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
         <v>0.03</v>
       </c>
-      <c r="M139">
+      <c r="M142">
         <v>200</v>
       </c>
-      <c r="N139" s="1">
-        <f>C139-D139*20-E139*0.8-F139*0.6-H139*5+I139*10+J139/300</f>
+      <c r="N142" s="1">
+        <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q139">
-        <f>P139*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="Q142">
+        <f>P142*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>249</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B143" t="s">
         <v>250</v>
       </c>
-      <c r="C140">
+      <c r="C143">
         <v>-1</v>
       </c>
-      <c r="D140">
+      <c r="D143">
         <v>0.11</v>
       </c>
-      <c r="M140">
+      <c r="M143">
         <v>500</v>
       </c>
-      <c r="N140" s="1">
-        <f>C140-D140*20-E140*0.8-F140*0.6-H140*5+I140*10+J140/300</f>
+      <c r="N143" s="1">
+        <f t="shared" si="14"/>
         <v>-3.2</v>
       </c>
-      <c r="P140">
+      <c r="P143">
         <v>7.0195183999999999</v>
       </c>
-      <c r="Q140">
+      <c r="Q143">
         <f t="shared" si="13"/>
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>245</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B144" t="s">
         <v>246</v>
       </c>
-      <c r="C141">
+      <c r="C144">
         <v>-7</v>
       </c>
-      <c r="D141">
+      <c r="D144">
         <v>0.42</v>
       </c>
-      <c r="F141">
+      <c r="F144">
         <v>-4</v>
       </c>
-      <c r="M141">
+      <c r="M144">
         <v>5000</v>
       </c>
-      <c r="N141" s="1">
-        <f>C141-D141*20-E141*0.8-F141*0.6-H141*5+I141*10+J141/300</f>
+      <c r="N144" s="1">
+        <f t="shared" si="14"/>
         <v>-13</v>
       </c>
-      <c r="P141">
+      <c r="P144">
         <v>39.299999999999997</v>
       </c>
-      <c r="Q141">
+      <c r="Q144">
         <f t="shared" si="13"/>
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N142" s="1">
-        <f>C142-D142*20-E142*0.8-F142*0.6-H142*5+I142*10+J142/300</f>
-        <v>0</v>
-      </c>
-      <c r="Q142">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N145" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q145">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B146" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C143" s="1">
+      <c r="C146" s="1">
         <v>-2</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D146" s="1">
         <v>0.21</v>
       </c>
-      <c r="E143" s="1"/>
-      <c r="F143" s="1"/>
-      <c r="G143" s="1"/>
-      <c r="H143" s="1"/>
-      <c r="I143" s="1"/>
-      <c r="J143" s="1"/>
-      <c r="K143" s="1"/>
-      <c r="L143" s="1"/>
-      <c r="M143" s="1">
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1">
         <v>1000</v>
       </c>
-      <c r="N143" s="1">
-        <f>C143-D143*20-E143*0.8-F143*0.6-H143*5+I143*10+J143/300</f>
+      <c r="N146" s="1">
+        <f t="shared" si="14"/>
         <v>-6.2</v>
       </c>
-      <c r="P143">
+      <c r="P146">
         <v>15</v>
       </c>
-      <c r="Q143">
+      <c r="Q146">
         <f t="shared" si="13"/>
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>181</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B147" t="s">
         <v>182</v>
       </c>
-      <c r="C144">
+      <c r="C147">
         <v>-2.5</v>
       </c>
-      <c r="D144">
+      <c r="D147">
         <v>0.22</v>
       </c>
-      <c r="F144">
+      <c r="F147">
         <v>-1</v>
       </c>
-      <c r="M144">
+      <c r="M147">
         <v>1000</v>
       </c>
-      <c r="N144" s="1">
-        <f>C144-D144*20-E144*0.8-F144*0.6-H144*5+I144*10+J144/300</f>
+      <c r="N147" s="1">
+        <f t="shared" si="14"/>
         <v>-6.3000000000000007</v>
       </c>
-      <c r="P144">
+      <c r="P147">
         <v>15.4</v>
       </c>
-      <c r="Q144">
+      <c r="Q147">
         <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>183</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B148" t="s">
         <v>184</v>
       </c>
-      <c r="C145">
+      <c r="C148">
         <v>-5</v>
       </c>
-      <c r="D145">
+      <c r="D148">
         <v>0.26</v>
       </c>
-      <c r="F145">
+      <c r="F148">
         <v>-2</v>
       </c>
-      <c r="M145">
+      <c r="M148">
         <v>2000</v>
       </c>
-      <c r="N145" s="1">
-        <f>C145-D145*20-E145*0.8-F145*0.6-H145*5+I145*10+J145/300</f>
+      <c r="N148" s="1">
+        <f t="shared" si="14"/>
         <v>-9</v>
       </c>
-      <c r="P145">
+      <c r="P148">
         <v>17.3</v>
       </c>
-      <c r="Q145">
+      <c r="Q148">
         <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>187</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B149" t="s">
         <v>188</v>
       </c>
-      <c r="C146">
+      <c r="C149">
         <v>-3</v>
       </c>
-      <c r="D146">
+      <c r="D149">
         <v>0.33</v>
       </c>
-      <c r="F146">
+      <c r="F149">
         <v>-3</v>
       </c>
-      <c r="M146">
+      <c r="M149">
         <v>3000</v>
       </c>
-      <c r="N146" s="1">
-        <f>C146-D146*20-E146*0.8-F146*0.6-H146*5+I146*10+J146/300</f>
+      <c r="N149" s="1">
+        <f t="shared" si="14"/>
         <v>-7.8000000000000016</v>
       </c>
-      <c r="P146">
+      <c r="P149">
         <v>24.162700000000001</v>
       </c>
-      <c r="Q146">
+      <c r="Q149">
         <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>189</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B150" t="s">
         <v>190</v>
       </c>
-      <c r="C147">
+      <c r="C150">
         <v>-3</v>
       </c>
-      <c r="D147">
+      <c r="D150">
         <v>0.24</v>
       </c>
-      <c r="F147">
+      <c r="F150">
         <v>-2</v>
       </c>
-      <c r="M147">
+      <c r="M150">
         <v>3000</v>
       </c>
-      <c r="N147" s="1">
-        <f>C147-D147*20-E147*0.8-F147*0.6-H147*5+I147*10+J147/300</f>
+      <c r="N150" s="1">
+        <f t="shared" si="14"/>
         <v>-6.6</v>
       </c>
-      <c r="P147">
+      <c r="P150">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q147">
+      <c r="Q150">
         <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>191</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B151" t="s">
         <v>192</v>
       </c>
-      <c r="C148">
+      <c r="C151">
         <v>-3</v>
       </c>
-      <c r="D148">
+      <c r="D151">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F148">
+      <c r="F151">
         <v>-1</v>
       </c>
-      <c r="M148">
+      <c r="M151">
         <v>5000</v>
       </c>
-      <c r="N148" s="1">
-        <f>C148-D148*20-E148*0.8-F148*0.6-H148*5+I148*10+J148/300</f>
+      <c r="N151" s="1">
+        <f t="shared" si="14"/>
         <v>-8.0000000000000018</v>
       </c>
-      <c r="P148">
+      <c r="P151">
         <v>21.9</v>
       </c>
-      <c r="Q148">
+      <c r="Q151">
         <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>193</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B152" t="s">
         <v>194</v>
       </c>
-      <c r="C149">
+      <c r="C152">
         <v>-3</v>
       </c>
-      <c r="D149">
+      <c r="D152">
         <v>0.27</v>
       </c>
-      <c r="F149">
+      <c r="F152">
         <v>-2</v>
       </c>
-      <c r="M149">
+      <c r="M152">
         <v>2000</v>
       </c>
-      <c r="N149" s="1">
-        <f>C149-D149*20-E149*0.8-F149*0.6-H149*5+I149*10+J149/300</f>
+      <c r="N152" s="1">
+        <f t="shared" si="14"/>
         <v>-7.2</v>
       </c>
-      <c r="P149">
+      <c r="P152">
         <v>19.3</v>
       </c>
-      <c r="Q149">
+      <c r="Q152">
         <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N150" s="1">
-        <f>C150-D150*20-E150*0.8-F150*0.6-H150*5+I150*10+J150/300</f>
-        <v>0</v>
-      </c>
-      <c r="Q150">
-        <f>P150*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N151" s="1"/>
-    </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N152" s="1"/>
-    </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N153" s="1"/>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N153" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Q153">
+        <f>P153*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>273</v>
+      </c>
+      <c r="B154" t="s">
+        <v>274</v>
+      </c>
+      <c r="C154">
+        <v>-2</v>
+      </c>
+      <c r="D154">
+        <v>0.05</v>
+      </c>
+      <c r="M154">
+        <v>300</v>
+      </c>
       <c r="N154" s="1"/>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q154">
+        <f t="shared" ref="Q154:Q165" si="15">P154*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>269</v>
+      </c>
+      <c r="B155" t="s">
+        <v>270</v>
+      </c>
+      <c r="C155">
+        <v>-2</v>
+      </c>
+      <c r="D155">
+        <v>0.05</v>
+      </c>
+      <c r="M155">
+        <v>300</v>
+      </c>
       <c r="N155" s="1"/>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q155">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>275</v>
+      </c>
+      <c r="B156" t="s">
+        <v>276</v>
+      </c>
+      <c r="C156">
+        <v>-3</v>
+      </c>
+      <c r="D156">
+        <v>0.17</v>
+      </c>
+      <c r="M156">
+        <v>750</v>
+      </c>
       <c r="N156" s="1"/>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P156">
+        <v>13.3</v>
+      </c>
+      <c r="Q156">
+        <f>P156*0.013+0.02</f>
+        <v>0.19289999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>271</v>
+      </c>
+      <c r="B157" t="s">
+        <v>272</v>
+      </c>
+      <c r="C157">
+        <v>-3</v>
+      </c>
+      <c r="D157">
+        <v>0.18</v>
+      </c>
+      <c r="M157">
+        <v>1000</v>
+      </c>
       <c r="N157" s="1"/>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P157">
+        <v>13.28</v>
+      </c>
+      <c r="Q157">
+        <f>P157*0.013+0.02</f>
+        <v>0.19263999999999998</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N158" s="1"/>
+      <c r="Q158">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N159" s="1"/>
+      <c r="Q159">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N160" s="1"/>
+      <c r="Q160">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="161" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N161" s="1"/>
+      <c r="Q161">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="162" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N162" s="1"/>
+      <c r="Q162">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="163" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="N163" s="1"/>
+      <c r="Q163">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="164" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q164">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="165" spans="14:17" x14ac:dyDescent="0.3">
+      <c r="Q165">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix nv optics & price
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2089B1D-A95B-4461-81F0-75F1BA36F894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290FB4F0-9FBE-4053-979D-018C2828C644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="282">
   <si>
     <t>new</t>
   </si>
@@ -873,6 +873,12 @@
   </si>
   <si>
     <t>trijicon_acog_ta11d_bac_carry_handle</t>
+  </si>
+  <si>
+    <t>armasight_orion_3x_gen1_plus_nv_scope</t>
+  </si>
+  <si>
+    <t>Armasight Orion 3x Gen1+ Night Vision Scope</t>
   </si>
 </sst>
 </file>
@@ -1716,18 +1722,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="21" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="57.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="21" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1745,7 +1751,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1936,7 +1942,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1975,7 +1981,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2076,7 +2082,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2109,7 +2115,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2142,7 +2148,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2200,7 +2206,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -2272,7 +2278,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2295,7 +2301,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2320,7 +2326,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N21" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2380,7 +2386,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2455,7 +2461,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2480,7 +2486,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2505,7 +2511,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2530,7 +2536,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2555,7 +2561,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2608,7 +2614,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2633,7 +2639,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2658,7 +2664,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -2683,7 +2689,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -2708,7 +2714,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2736,7 +2742,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2820,7 +2826,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2851,7 +2857,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -2879,7 +2885,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2904,7 +2910,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -2929,7 +2935,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -2979,7 +2985,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N45" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2989,7 +2995,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -3039,7 +3045,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>116</v>
       </c>
@@ -3064,7 +3070,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -3095,7 +3101,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N50" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3105,7 +3111,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>120</v>
       </c>
@@ -3136,7 +3142,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -3167,7 +3173,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>130</v>
       </c>
@@ -3226,7 +3232,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -3251,7 +3257,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>136</v>
       </c>
@@ -3301,7 +3307,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>140</v>
       </c>
@@ -3351,7 +3357,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -3379,7 +3385,7 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -3429,7 +3435,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -3454,7 +3460,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -3504,7 +3510,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>150</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N67" s="1">
         <f t="shared" ref="N67:N96" si="7">C67-D67*20-E67*0.8-F67*0.6-H67*5+I67*10+J67/300</f>
         <v>0</v>
@@ -3539,7 +3545,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -3564,7 +3570,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>178</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>180</v>
       </c>
@@ -3617,7 +3623,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N71" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3627,7 +3633,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>197</v>
       </c>
@@ -3652,7 +3658,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>195</v>
       </c>
@@ -3677,7 +3683,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>199</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N75" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3715,7 +3721,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>201</v>
       </c>
@@ -3740,7 +3746,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>203</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>0.22539999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N78" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3778,7 +3784,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -3806,7 +3812,7 @@
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -3834,7 +3840,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>156</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -3890,7 +3896,7 @@
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3921,7 +3927,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -3952,7 +3958,7 @@
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -3980,7 +3986,7 @@
         <v>0.15665079999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -4008,7 +4014,7 @@
         <v>0.16215408999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>166</v>
       </c>
@@ -4036,7 +4042,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>168</v>
       </c>
@@ -4064,7 +4070,7 @@
         <v>0.20069999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -4089,7 +4095,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -4117,7 +4123,7 @@
         <v>0.17079999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N91" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4127,7 +4133,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>32</v>
       </c>
@@ -4160,7 +4166,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>34</v>
       </c>
@@ -4193,7 +4199,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>54</v>
       </c>
@@ -4218,7 +4224,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>56</v>
       </c>
@@ -4243,7 +4249,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>64</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -4296,7 +4302,7 @@
         <v>0.1227</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>60</v>
       </c>
@@ -4321,7 +4327,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>61</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>62</v>
       </c>
@@ -4371,7 +4377,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4422,7 +4428,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -4478,7 +4484,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N105" s="1">
         <f>C105-D105*20-E105*0.8-F105*0.6-H105*5+I105*10+J105/300</f>
         <v>0</v>
@@ -4488,7 +4494,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>209</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>211</v>
       </c>
@@ -4544,7 +4550,7 @@
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N108" s="1">
         <f t="shared" ref="N108:N137" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
         <v>0</v>
@@ -4554,7 +4560,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>213</v>
       </c>
@@ -4579,7 +4585,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -4607,7 +4613,7 @@
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N111" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4617,7 +4623,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -4642,7 +4648,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>219</v>
       </c>
@@ -4670,7 +4676,7 @@
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -4695,7 +4701,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N115" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4705,7 +4711,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>225</v>
       </c>
@@ -4733,7 +4739,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>223</v>
       </c>
@@ -4758,7 +4764,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -4789,7 +4795,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -4817,7 +4823,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>229</v>
       </c>
@@ -4848,7 +4854,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>279</v>
       </c>
@@ -4876,7 +4882,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>231</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>0.22279999999999997</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>277</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N124" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4945,7 +4951,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -4973,7 +4979,7 @@
         <v>0.1045</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>251</v>
       </c>
@@ -4998,7 +5004,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>257</v>
       </c>
@@ -5023,7 +5029,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>261</v>
       </c>
@@ -5048,7 +5054,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>260</v>
       </c>
@@ -5073,7 +5079,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>263</v>
       </c>
@@ -5098,7 +5104,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>265</v>
       </c>
@@ -5123,7 +5129,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>267</v>
       </c>
@@ -5148,7 +5154,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>235</v>
       </c>
@@ -5176,7 +5182,7 @@
         <v>0.1331</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>237</v>
       </c>
@@ -5204,7 +5210,7 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>239</v>
       </c>
@@ -5232,7 +5238,7 @@
         <v>0.1071</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -5257,7 +5263,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>243</v>
       </c>
@@ -5288,7 +5294,7 @@
         <v>0.28130000000000005</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N138" s="1">
         <f t="shared" ref="N138:N153" si="14">C138-D138*20-E138*0.8-F138*0.6-H138*5+I138*10+J138/300</f>
         <v>0</v>
@@ -5298,7 +5304,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>247</v>
       </c>
@@ -5326,7 +5332,7 @@
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>253</v>
       </c>
@@ -5351,7 +5357,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>255</v>
       </c>
@@ -5376,7 +5382,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -5401,7 +5407,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>249</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>245</v>
       </c>
@@ -5460,7 +5466,7 @@
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N145" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -5470,7 +5476,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>185</v>
       </c>
@@ -5506,7 +5512,7 @@
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>181</v>
       </c>
@@ -5537,7 +5543,7 @@
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>183</v>
       </c>
@@ -5568,7 +5574,7 @@
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>187</v>
       </c>
@@ -5599,7 +5605,7 @@
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>189</v>
       </c>
@@ -5630,7 +5636,7 @@
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>191</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>-1</v>
       </c>
       <c r="M151">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="N151" s="1">
         <f t="shared" si="14"/>
@@ -5661,7 +5667,7 @@
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>193</v>
       </c>
@@ -5692,7 +5698,7 @@
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N153" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -5702,7 +5708,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>273</v>
       </c>
@@ -5724,7 +5730,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>269</v>
       </c>
@@ -5746,7 +5752,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>275</v>
       </c>
@@ -5771,7 +5777,7 @@
         <v>0.19289999999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>271</v>
       </c>
@@ -5796,55 +5802,73 @@
         <v>0.19263999999999998</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N158" s="1"/>
       <c r="Q158">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>280</v>
+      </c>
+      <c r="B159" t="s">
+        <v>281</v>
+      </c>
+      <c r="C159">
+        <v>-8</v>
+      </c>
+      <c r="D159">
+        <v>0.36</v>
+      </c>
+      <c r="F159">
+        <v>-3</v>
+      </c>
+      <c r="M159">
+        <v>3000</v>
+      </c>
       <c r="N159" s="1"/>
       <c r="Q159">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N160" s="1"/>
       <c r="Q160">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="161" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N161" s="1"/>
       <c r="Q161">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="162" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N162" s="1"/>
       <c r="Q162">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="163" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="14:17" x14ac:dyDescent="0.3">
       <c r="N163" s="1"/>
       <c r="Q163">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="164" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="14:17" x14ac:dyDescent="0.3">
       <c r="Q164">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="165" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="14:17" x14ac:dyDescent="0.3">
       <c r="Q165">
         <f t="shared" si="15"/>
         <v>0.02</v>

</xml_diff>

<commit_message>
nerf tall rmr mount
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290FB4F0-9FBE-4053-979D-018C2828C644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB1A21-743D-4BE2-8DFA-C46FAAA21F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -1722,18 +1722,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" customWidth="1"/>
-    <col min="3" max="21" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" customWidth="1"/>
+    <col min="3" max="21" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1751,7 +1751,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>24</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D5" s="1">
         <v>0.05</v>
@@ -1896,14 +1896,14 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2082,7 +2082,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2301,7 +2301,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N21" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2386,7 +2386,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N45" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2995,7 +2995,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>116</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N50" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3111,7 +3111,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>120</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>130</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>136</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>140</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>150</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N67" s="1">
         <f t="shared" ref="N67:N96" si="7">C67-D67*20-E67*0.8-F67*0.6-H67*5+I67*10+J67/300</f>
         <v>0</v>
@@ -3545,7 +3545,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>178</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>180</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N71" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3633,7 +3633,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>197</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>195</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>199</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N75" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3721,7 +3721,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>201</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>203</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>0.22539999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N78" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3784,7 +3784,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>156</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>0.15665079999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>0.16215408999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>166</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>168</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>0.20069999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>0.17079999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N91" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4133,7 +4133,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>32</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>34</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>54</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>56</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>64</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>0.1227</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>60</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>61</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>62</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4428,7 +4428,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N105" s="1">
         <f>C105-D105*20-E105*0.8-F105*0.6-H105*5+I105*10+J105/300</f>
         <v>0</v>
@@ -4494,7 +4494,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>209</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>211</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N108" s="1">
         <f t="shared" ref="N108:N137" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
         <v>0</v>
@@ -4560,7 +4560,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>213</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N111" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4623,7 +4623,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>219</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N115" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4711,7 +4711,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>225</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>223</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>278</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>229</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>279</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>231</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>0.22279999999999997</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>277</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N124" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4951,7 +4951,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>233</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>0.1045</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>251</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>257</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>261</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>260</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>263</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>265</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>267</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>235</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>0.1331</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>237</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>239</v>
       </c>
@@ -5238,7 +5238,7 @@
         <v>0.1071</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>243</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>0.28130000000000005</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N138" s="1">
         <f t="shared" ref="N138:N153" si="14">C138-D138*20-E138*0.8-F138*0.6-H138*5+I138*10+J138/300</f>
         <v>0</v>
@@ -5304,7 +5304,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>247</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>253</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>255</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>249</v>
       </c>
@@ -5435,7 +5435,7 @@
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>245</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N145" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -5476,7 +5476,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>185</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>181</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>183</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>187</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>189</v>
       </c>
@@ -5636,7 +5636,7 @@
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>191</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>193</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N153" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -5708,7 +5708,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>273</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>269</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>275</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>0.19289999999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>271</v>
       </c>
@@ -5802,14 +5802,14 @@
         <v>0.19263999999999998</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N158" s="1"/>
       <c r="Q158">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>280</v>
       </c>
@@ -5834,41 +5834,41 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N160" s="1"/>
       <c r="Q160">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="161" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N161" s="1"/>
       <c r="Q161">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="162" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N162" s="1"/>
       <c r="Q162">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="163" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="14:17" x14ac:dyDescent="0.25">
       <c r="N163" s="1"/>
       <c r="Q163">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="164" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="14:17" x14ac:dyDescent="0.25">
       <c r="Q164">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="165" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="14:17" x14ac:dyDescent="0.25">
       <c r="Q165">
         <f t="shared" si="15"/>
         <v>0.02</v>

</xml_diff>

<commit_message>
update and add new acogs
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAB1A21-743D-4BE2-8DFA-C46FAAA21F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233DDB10-FCBD-4F2B-B855-579AFC9811D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="288">
   <si>
     <t>new</t>
   </si>
@@ -728,12 +728,6 @@
     <t>Trijicon Acog TA11D BAC</t>
   </si>
   <si>
-    <t>trijicon_ta01nsn</t>
-  </si>
-  <si>
-    <t>Trijicon Acog TA01NSN</t>
-  </si>
-  <si>
     <t>badger_ordnance_comm_30mm_mount_body</t>
   </si>
   <si>
@@ -866,9 +860,6 @@
     <t>Colt Retro A1 4x21 Scope</t>
   </si>
   <si>
-    <t>trijicon_ta01nsn_carry_handle</t>
-  </si>
-  <si>
     <t>burris_prism_ar332_carry_handle</t>
   </si>
   <si>
@@ -879,6 +870,33 @@
   </si>
   <si>
     <t>Armasight Orion 3x Gen1+ Night Vision Scope</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta01_4x_scope</t>
+  </si>
+  <si>
+    <t>Trijicon ACOG TA01 4x Scope</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta01_4x_scope_carry_handle</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta31_comspec_4x_scope</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta31_comspec_4x_scope_carry_handle</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta31_milspec_4x_scope</t>
+  </si>
+  <si>
+    <t>trijicon_acog_ta31_milspec_4x_scope_carry_handle</t>
+  </si>
+  <si>
+    <t>Trijicon ACOG TA31 Comspec 4x Scope</t>
+  </si>
+  <si>
+    <t>Trijicon ACOG TA31 Milspec 4x Scope</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R165"/>
+  <dimension ref="A1:R169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T125" sqref="T125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4552,11 +4570,11 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N108" s="1">
-        <f t="shared" ref="N108:N137" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
+        <f t="shared" ref="N108:N141" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
         <v>0</v>
       </c>
       <c r="Q108">
-        <f t="shared" ref="Q108:Q152" si="13">P108*0.013+0.02</f>
+        <f t="shared" ref="Q108:Q156" si="13">P108*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
@@ -4797,7 +4815,7 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B119" t="s">
         <v>228</v>
@@ -4840,7 +4858,7 @@
         <v>-2</v>
       </c>
       <c r="M120">
-        <v>1750</v>
+        <v>1800</v>
       </c>
       <c r="N120" s="1">
         <f t="shared" si="12"/>
@@ -4856,7 +4874,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B121" t="s">
         <v>230</v>
@@ -4871,7 +4889,7 @@
         <v>-2</v>
       </c>
       <c r="M121">
-        <v>1750</v>
+        <v>1800</v>
       </c>
       <c r="N121" s="1">
         <f t="shared" si="12"/>
@@ -4884,10 +4902,10 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="B122" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C122">
         <v>-3</v>
@@ -4896,14 +4914,14 @@
         <v>0.22</v>
       </c>
       <c r="F122">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M122">
         <v>1500</v>
       </c>
       <c r="N122" s="1">
         <f t="shared" si="12"/>
-        <v>-6.2</v>
+        <v>-6.8000000000000007</v>
       </c>
       <c r="P122">
         <v>15.6</v>
@@ -4915,10 +4933,10 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B123" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="C123">
         <v>-3</v>
@@ -4927,14 +4945,14 @@
         <v>0.22</v>
       </c>
       <c r="F123">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M123">
         <v>1500</v>
       </c>
       <c r="N123" s="1">
         <f t="shared" si="12"/>
-        <v>-6.2</v>
+        <v>-6.8000000000000007</v>
       </c>
       <c r="Q123">
         <f t="shared" si="13"/>
@@ -4942,149 +4960,146 @@
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>282</v>
+      </c>
+      <c r="B124" t="s">
+        <v>286</v>
+      </c>
+      <c r="C124">
+        <v>-3</v>
+      </c>
+      <c r="D124">
+        <v>0.17</v>
+      </c>
+      <c r="H124">
+        <v>0.05</v>
+      </c>
+      <c r="M124">
+        <v>1600</v>
+      </c>
       <c r="N124" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-6.65</v>
+      </c>
+      <c r="P124">
+        <v>10.9</v>
       </c>
       <c r="Q124">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.16169999999999998</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>233</v>
+        <v>283</v>
       </c>
       <c r="B125" t="s">
-        <v>234</v>
+        <v>286</v>
       </c>
       <c r="C125">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="D125">
-        <v>0.06</v>
+        <v>0.17</v>
+      </c>
+      <c r="H125">
+        <v>0.05</v>
       </c>
       <c r="M125">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="N125" s="1">
         <f t="shared" si="12"/>
+        <v>-6.65</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>284</v>
+      </c>
+      <c r="B126" t="s">
+        <v>287</v>
+      </c>
+      <c r="C126">
+        <v>-3</v>
+      </c>
+      <c r="D126">
+        <v>0.17</v>
+      </c>
+      <c r="M126">
+        <v>1700</v>
+      </c>
+      <c r="N126" s="1">
+        <f t="shared" si="12"/>
+        <v>-6.4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>285</v>
+      </c>
+      <c r="B127" t="s">
+        <v>287</v>
+      </c>
+      <c r="C127">
+        <v>-3</v>
+      </c>
+      <c r="D127">
+        <v>0.17</v>
+      </c>
+      <c r="M127">
+        <v>1700</v>
+      </c>
+      <c r="N127" s="1">
+        <f t="shared" si="12"/>
+        <v>-6.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N128" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q128">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>231</v>
+      </c>
+      <c r="B129" t="s">
+        <v>232</v>
+      </c>
+      <c r="C129">
+        <v>-0.5</v>
+      </c>
+      <c r="D129">
+        <v>0.06</v>
+      </c>
+      <c r="M129">
+        <v>1000</v>
+      </c>
+      <c r="N129" s="1">
+        <f t="shared" si="12"/>
         <v>-1.7</v>
       </c>
-      <c r="P125">
+      <c r="P129">
         <v>6.5</v>
       </c>
-      <c r="Q125">
+      <c r="Q129">
         <f t="shared" si="13"/>
         <v>0.1045</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>251</v>
-      </c>
-      <c r="B126" t="s">
-        <v>252</v>
-      </c>
-      <c r="C126">
-        <v>0</v>
-      </c>
-      <c r="D126">
-        <v>0.01</v>
-      </c>
-      <c r="M126">
-        <v>0</v>
-      </c>
-      <c r="N126" s="1">
-        <f t="shared" si="12"/>
-        <v>-0.2</v>
-      </c>
-      <c r="Q126">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>257</v>
-      </c>
-      <c r="B127" t="s">
-        <v>258</v>
-      </c>
-      <c r="C127">
-        <v>0</v>
-      </c>
-      <c r="D127">
-        <v>0.03</v>
-      </c>
-      <c r="M127">
-        <v>200</v>
-      </c>
-      <c r="N127" s="1">
-        <f t="shared" si="12"/>
-        <v>-0.6</v>
-      </c>
-      <c r="Q127">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>261</v>
-      </c>
-      <c r="B128" t="s">
-        <v>262</v>
-      </c>
-      <c r="C128">
-        <v>0</v>
-      </c>
-      <c r="D128">
-        <v>0.02</v>
-      </c>
-      <c r="M128">
-        <v>200</v>
-      </c>
-      <c r="N128" s="1">
-        <f t="shared" si="12"/>
-        <v>-0.4</v>
-      </c>
-      <c r="Q128">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>260</v>
-      </c>
-      <c r="B129" t="s">
-        <v>258</v>
-      </c>
-      <c r="C129">
-        <v>0</v>
-      </c>
-      <c r="D129">
-        <v>0.03</v>
-      </c>
-      <c r="M129">
-        <v>200</v>
-      </c>
-      <c r="N129" s="1">
-        <f t="shared" si="12"/>
-        <v>-0.6</v>
-      </c>
-      <c r="Q129">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="B130" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -5093,7 +5108,7 @@
         <v>0.01</v>
       </c>
       <c r="M130">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N130" s="1">
         <f t="shared" si="12"/>
@@ -5106,23 +5121,23 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B131" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C131">
         <v>0</v>
       </c>
       <c r="D131">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M131">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N131" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="Q131">
         <f t="shared" si="13"/>
@@ -5131,10 +5146,10 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B132" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -5143,7 +5158,7 @@
         <v>0.02</v>
       </c>
       <c r="M132">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N132" s="1">
         <f t="shared" si="12"/>
@@ -5156,107 +5171,98 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="B133" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="C133">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>0.11</v>
+        <v>0.03</v>
       </c>
       <c r="M133">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="N133" s="1">
         <f t="shared" si="12"/>
-        <v>-3.2</v>
-      </c>
-      <c r="P133">
-        <v>8.6999999999999993</v>
+        <v>-0.6</v>
       </c>
       <c r="Q133">
         <f t="shared" si="13"/>
-        <v>0.1331</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="B134" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="C134">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="D134">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="M134">
-        <v>750</v>
+        <v>200</v>
       </c>
       <c r="N134" s="1">
         <f t="shared" si="12"/>
-        <v>-3.5</v>
-      </c>
-      <c r="P134">
-        <v>7.5</v>
+        <v>-0.2</v>
       </c>
       <c r="Q134">
         <f t="shared" si="13"/>
-        <v>0.11749999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="B135" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="C135">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="M135">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N135" s="1">
         <f t="shared" si="12"/>
-        <v>-2.8</v>
-      </c>
-      <c r="P135">
-        <v>6.7</v>
+        <v>-0.4</v>
       </c>
       <c r="Q135">
         <f t="shared" si="13"/>
-        <v>0.1071</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="B136" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="C136">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D136">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M136">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N136" s="1">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-0.4</v>
       </c>
       <c r="Q136">
         <f t="shared" si="13"/>
@@ -5265,568 +5271,595 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B137" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C137">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="D137">
-        <v>0.27</v>
-      </c>
-      <c r="F137">
-        <v>-2</v>
+        <v>0.11</v>
       </c>
       <c r="M137">
-        <v>4000</v>
+        <v>800</v>
       </c>
       <c r="N137" s="1">
         <f t="shared" si="12"/>
-        <v>-9.2000000000000011</v>
+        <v>-3.2</v>
       </c>
       <c r="P137">
-        <v>20.100000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Q137">
         <f t="shared" si="13"/>
-        <v>0.28130000000000005</v>
+        <v>0.1331</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>235</v>
+      </c>
+      <c r="B138" t="s">
+        <v>236</v>
+      </c>
+      <c r="C138">
+        <v>-1.5</v>
+      </c>
+      <c r="D138">
+        <v>0.1</v>
+      </c>
+      <c r="M138">
+        <v>750</v>
+      </c>
       <c r="N138" s="1">
-        <f t="shared" ref="N138:N153" si="14">C138-D138*20-E138*0.8-F138*0.6-H138*5+I138*10+J138/300</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-3.5</v>
+      </c>
+      <c r="P138">
+        <v>7.5</v>
       </c>
       <c r="Q138">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.11749999999999999</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B139" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C139">
+        <v>-1</v>
+      </c>
+      <c r="D139">
+        <v>0.09</v>
+      </c>
+      <c r="M139">
+        <v>500</v>
+      </c>
+      <c r="N139" s="1">
+        <f t="shared" si="12"/>
+        <v>-2.8</v>
+      </c>
+      <c r="P139">
+        <v>6.7</v>
+      </c>
+      <c r="Q139">
+        <f t="shared" si="13"/>
+        <v>0.1071</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>239</v>
+      </c>
+      <c r="B140" t="s">
+        <v>240</v>
+      </c>
+      <c r="C140">
+        <v>-1</v>
+      </c>
+      <c r="D140">
+        <v>0.1</v>
+      </c>
+      <c r="M140">
+        <v>500</v>
+      </c>
+      <c r="N140" s="1">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
+      <c r="Q140">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>241</v>
+      </c>
+      <c r="B141" t="s">
+        <v>242</v>
+      </c>
+      <c r="C141">
+        <v>-5</v>
+      </c>
+      <c r="D141">
+        <v>0.27</v>
+      </c>
+      <c r="F141">
+        <v>-2</v>
+      </c>
+      <c r="M141">
+        <v>4000</v>
+      </c>
+      <c r="N141" s="1">
+        <f t="shared" si="12"/>
+        <v>-9.2000000000000011</v>
+      </c>
+      <c r="P141">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q141">
+        <f t="shared" si="13"/>
+        <v>0.28130000000000005</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N142" s="1">
+        <f t="shared" ref="N142:N157" si="14">C142-D142*20-E142*0.8-F142*0.6-H142*5+I142*10+J142/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q142">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>245</v>
+      </c>
+      <c r="B143" t="s">
+        <v>246</v>
+      </c>
+      <c r="C143">
         <v>-0.5</v>
       </c>
-      <c r="D139">
+      <c r="D143">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M139">
+      <c r="M143">
         <v>1000</v>
       </c>
-      <c r="N139" s="1">
+      <c r="N143" s="1">
         <f t="shared" si="14"/>
         <v>-1.9000000000000001</v>
       </c>
-      <c r="P139">
+      <c r="P143">
         <v>6.6</v>
       </c>
-      <c r="Q139">
+      <c r="Q143">
         <f t="shared" si="13"/>
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>253</v>
-      </c>
-      <c r="B140" t="s">
-        <v>254</v>
-      </c>
-      <c r="C140">
-        <v>0</v>
-      </c>
-      <c r="D140">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>251</v>
+      </c>
+      <c r="B144" t="s">
+        <v>252</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
         <v>0.01</v>
       </c>
-      <c r="M140">
-        <v>0</v>
-      </c>
-      <c r="N140" s="1">
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144" s="1">
         <f t="shared" si="14"/>
         <v>-0.2</v>
       </c>
-      <c r="Q140">
-        <f>P140*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>255</v>
-      </c>
-      <c r="B141" t="s">
-        <v>256</v>
-      </c>
-      <c r="C141">
-        <v>0</v>
-      </c>
-      <c r="D141">
+      <c r="Q144">
+        <f>P144*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>253</v>
+      </c>
+      <c r="B145" t="s">
+        <v>254</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
         <v>0.03</v>
       </c>
-      <c r="M141">
+      <c r="M145">
         <v>200</v>
       </c>
-      <c r="N141" s="1">
+      <c r="N145" s="1">
         <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q141">
-        <f>P141*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>259</v>
-      </c>
-      <c r="B142" t="s">
-        <v>256</v>
-      </c>
-      <c r="C142">
-        <v>0</v>
-      </c>
-      <c r="D142">
+      <c r="Q145">
+        <f>P145*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>257</v>
+      </c>
+      <c r="B146" t="s">
+        <v>254</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
         <v>0.03</v>
       </c>
-      <c r="M142">
+      <c r="M146">
         <v>200</v>
       </c>
-      <c r="N142" s="1">
+      <c r="N146" s="1">
         <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q142">
-        <f>P142*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>249</v>
-      </c>
-      <c r="B143" t="s">
-        <v>250</v>
-      </c>
-      <c r="C143">
+      <c r="Q146">
+        <f>P146*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>247</v>
+      </c>
+      <c r="B147" t="s">
+        <v>248</v>
+      </c>
+      <c r="C147">
         <v>-1</v>
       </c>
-      <c r="D143">
+      <c r="D147">
         <v>0.11</v>
       </c>
-      <c r="M143">
+      <c r="M147">
         <v>500</v>
       </c>
-      <c r="N143" s="1">
+      <c r="N147" s="1">
         <f t="shared" si="14"/>
         <v>-3.2</v>
       </c>
-      <c r="P143">
+      <c r="P147">
         <v>7.0195183999999999</v>
       </c>
-      <c r="Q143">
+      <c r="Q147">
         <f t="shared" si="13"/>
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>245</v>
-      </c>
-      <c r="B144" t="s">
-        <v>246</v>
-      </c>
-      <c r="C144">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>243</v>
+      </c>
+      <c r="B148" t="s">
+        <v>244</v>
+      </c>
+      <c r="C148">
         <v>-7</v>
       </c>
-      <c r="D144">
+      <c r="D148">
         <v>0.42</v>
       </c>
-      <c r="F144">
+      <c r="F148">
         <v>-4</v>
       </c>
-      <c r="M144">
+      <c r="M148">
         <v>5000</v>
       </c>
-      <c r="N144" s="1">
+      <c r="N148" s="1">
         <f t="shared" si="14"/>
         <v>-13</v>
       </c>
-      <c r="P144">
+      <c r="P148">
         <v>39.299999999999997</v>
       </c>
-      <c r="Q144">
+      <c r="Q148">
         <f t="shared" si="13"/>
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N145" s="1">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N149" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q145">
+      <c r="Q149">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B150" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C146" s="1">
+      <c r="C150" s="1">
         <v>-2</v>
       </c>
-      <c r="D146" s="1">
+      <c r="D150" s="1">
         <v>0.21</v>
       </c>
-      <c r="E146" s="1"/>
-      <c r="F146" s="1"/>
-      <c r="G146" s="1"/>
-      <c r="H146" s="1"/>
-      <c r="I146" s="1"/>
-      <c r="J146" s="1"/>
-      <c r="K146" s="1"/>
-      <c r="L146" s="1"/>
-      <c r="M146" s="1">
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1">
         <v>1000</v>
       </c>
-      <c r="N146" s="1">
+      <c r="N150" s="1">
         <f t="shared" si="14"/>
         <v>-6.2</v>
       </c>
-      <c r="P146">
+      <c r="P150">
         <v>15</v>
       </c>
-      <c r="Q146">
+      <c r="Q150">
         <f t="shared" si="13"/>
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>181</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B151" t="s">
         <v>182</v>
       </c>
-      <c r="C147">
+      <c r="C151">
         <v>-2.5</v>
       </c>
-      <c r="D147">
+      <c r="D151">
         <v>0.22</v>
       </c>
-      <c r="F147">
+      <c r="F151">
         <v>-1</v>
       </c>
-      <c r="M147">
+      <c r="M151">
         <v>1000</v>
       </c>
-      <c r="N147" s="1">
+      <c r="N151" s="1">
         <f t="shared" si="14"/>
         <v>-6.3000000000000007</v>
       </c>
-      <c r="P147">
+      <c r="P151">
         <v>15.4</v>
       </c>
-      <c r="Q147">
+      <c r="Q151">
         <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>183</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B152" t="s">
         <v>184</v>
       </c>
-      <c r="C148">
+      <c r="C152">
         <v>-5</v>
       </c>
-      <c r="D148">
+      <c r="D152">
         <v>0.26</v>
       </c>
-      <c r="F148">
+      <c r="F152">
         <v>-2</v>
       </c>
-      <c r="M148">
+      <c r="M152">
         <v>2000</v>
       </c>
-      <c r="N148" s="1">
+      <c r="N152" s="1">
         <f t="shared" si="14"/>
         <v>-9</v>
       </c>
-      <c r="P148">
+      <c r="P152">
         <v>17.3</v>
       </c>
-      <c r="Q148">
+      <c r="Q152">
         <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>187</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B153" t="s">
         <v>188</v>
       </c>
-      <c r="C149">
+      <c r="C153">
         <v>-3</v>
       </c>
-      <c r="D149">
+      <c r="D153">
         <v>0.33</v>
       </c>
-      <c r="F149">
+      <c r="F153">
         <v>-3</v>
       </c>
-      <c r="M149">
+      <c r="M153">
         <v>3000</v>
       </c>
-      <c r="N149" s="1">
+      <c r="N153" s="1">
         <f t="shared" si="14"/>
         <v>-7.8000000000000016</v>
       </c>
-      <c r="P149">
+      <c r="P153">
         <v>24.162700000000001</v>
       </c>
-      <c r="Q149">
+      <c r="Q153">
         <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>189</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B154" t="s">
         <v>190</v>
       </c>
-      <c r="C150">
+      <c r="C154">
         <v>-3</v>
       </c>
-      <c r="D150">
+      <c r="D154">
         <v>0.24</v>
       </c>
-      <c r="F150">
+      <c r="F154">
         <v>-2</v>
       </c>
-      <c r="M150">
+      <c r="M154">
         <v>3000</v>
       </c>
-      <c r="N150" s="1">
+      <c r="N154" s="1">
         <f t="shared" si="14"/>
         <v>-6.6</v>
       </c>
-      <c r="P150">
+      <c r="P154">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q150">
+      <c r="Q154">
         <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>191</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B155" t="s">
         <v>192</v>
       </c>
-      <c r="C151">
+      <c r="C155">
         <v>-3</v>
       </c>
-      <c r="D151">
+      <c r="D155">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F151">
+      <c r="F155">
         <v>-1</v>
       </c>
-      <c r="M151">
+      <c r="M155">
         <v>4000</v>
       </c>
-      <c r="N151" s="1">
+      <c r="N155" s="1">
         <f t="shared" si="14"/>
         <v>-8.0000000000000018</v>
       </c>
-      <c r="P151">
+      <c r="P155">
         <v>21.9</v>
       </c>
-      <c r="Q151">
+      <c r="Q155">
         <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>193</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B156" t="s">
         <v>194</v>
       </c>
-      <c r="C152">
+      <c r="C156">
         <v>-3</v>
       </c>
-      <c r="D152">
+      <c r="D156">
         <v>0.27</v>
       </c>
-      <c r="F152">
+      <c r="F156">
         <v>-2</v>
       </c>
-      <c r="M152">
+      <c r="M156">
         <v>2000</v>
       </c>
-      <c r="N152" s="1">
+      <c r="N156" s="1">
         <f t="shared" si="14"/>
         <v>-7.2</v>
       </c>
-      <c r="P152">
+      <c r="P156">
         <v>19.3</v>
       </c>
-      <c r="Q152">
+      <c r="Q156">
         <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N153" s="1">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N157" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
-      </c>
-      <c r="Q153">
-        <f>P153*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>273</v>
-      </c>
-      <c r="B154" t="s">
-        <v>274</v>
-      </c>
-      <c r="C154">
-        <v>-2</v>
-      </c>
-      <c r="D154">
-        <v>0.05</v>
-      </c>
-      <c r="M154">
-        <v>300</v>
-      </c>
-      <c r="N154" s="1"/>
-      <c r="Q154">
-        <f t="shared" ref="Q154:Q165" si="15">P154*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>269</v>
-      </c>
-      <c r="B155" t="s">
-        <v>270</v>
-      </c>
-      <c r="C155">
-        <v>-2</v>
-      </c>
-      <c r="D155">
-        <v>0.05</v>
-      </c>
-      <c r="M155">
-        <v>300</v>
-      </c>
-      <c r="N155" s="1"/>
-      <c r="Q155">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>275</v>
-      </c>
-      <c r="B156" t="s">
-        <v>276</v>
-      </c>
-      <c r="C156">
-        <v>-3</v>
-      </c>
-      <c r="D156">
-        <v>0.17</v>
-      </c>
-      <c r="M156">
-        <v>750</v>
-      </c>
-      <c r="N156" s="1"/>
-      <c r="P156">
-        <v>13.3</v>
-      </c>
-      <c r="Q156">
-        <f>P156*0.013+0.02</f>
-        <v>0.19289999999999999</v>
-      </c>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>271</v>
-      </c>
-      <c r="B157" t="s">
-        <v>272</v>
-      </c>
-      <c r="C157">
-        <v>-3</v>
-      </c>
-      <c r="D157">
-        <v>0.18</v>
-      </c>
-      <c r="M157">
-        <v>1000</v>
-      </c>
-      <c r="N157" s="1"/>
-      <c r="P157">
-        <v>13.28</v>
       </c>
       <c r="Q157">
         <f>P157*0.013+0.02</f>
-        <v>0.19263999999999998</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>271</v>
+      </c>
+      <c r="B158" t="s">
+        <v>272</v>
+      </c>
+      <c r="C158">
+        <v>-2</v>
+      </c>
+      <c r="D158">
+        <v>0.05</v>
+      </c>
+      <c r="M158">
+        <v>300</v>
+      </c>
       <c r="N158" s="1"/>
       <c r="Q158">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="Q158:Q169" si="15">P158*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B159" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C159">
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="D159">
-        <v>0.36</v>
-      </c>
-      <c r="F159">
-        <v>-3</v>
+        <v>0.05</v>
       </c>
       <c r="M159">
-        <v>3000</v>
+        <v>300</v>
       </c>
       <c r="N159" s="1"/>
       <c r="Q159">
@@ -5835,41 +5868,123 @@
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>273</v>
+      </c>
+      <c r="B160" t="s">
+        <v>274</v>
+      </c>
+      <c r="C160">
+        <v>-3</v>
+      </c>
+      <c r="D160">
+        <v>0.17</v>
+      </c>
+      <c r="M160">
+        <v>750</v>
+      </c>
       <c r="N160" s="1"/>
+      <c r="P160">
+        <v>13.3</v>
+      </c>
       <c r="Q160">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="161" spans="14:17" x14ac:dyDescent="0.25">
+        <f>P160*0.013+0.02</f>
+        <v>0.19289999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>269</v>
+      </c>
+      <c r="B161" t="s">
+        <v>270</v>
+      </c>
+      <c r="C161">
+        <v>-3</v>
+      </c>
+      <c r="D161">
+        <v>0.18</v>
+      </c>
+      <c r="M161">
+        <v>1000</v>
+      </c>
       <c r="N161" s="1"/>
+      <c r="P161">
+        <v>13.28</v>
+      </c>
       <c r="Q161">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="162" spans="14:17" x14ac:dyDescent="0.25">
+        <f>P161*0.013+0.02</f>
+        <v>0.19263999999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N162" s="1"/>
       <c r="Q162">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="163" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>277</v>
+      </c>
+      <c r="B163" t="s">
+        <v>278</v>
+      </c>
+      <c r="C163">
+        <v>-8</v>
+      </c>
+      <c r="D163">
+        <v>0.36</v>
+      </c>
+      <c r="F163">
+        <v>-3</v>
+      </c>
+      <c r="M163">
+        <v>3000</v>
+      </c>
       <c r="N163" s="1"/>
       <c r="Q163">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="164" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N164" s="1"/>
       <c r="Q164">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="165" spans="14:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N165" s="1"/>
       <c r="Q165">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N166" s="1"/>
+      <c r="Q166">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N167" s="1"/>
+      <c r="Q167">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q168">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q169">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>

</xml_diff>

<commit_message>
fix acog weights and add cosmic saturn
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334208E9-BC99-4A30-9DA7-D15C51750DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36012303-3058-459F-A854-08702076FB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="295">
   <si>
     <t>new</t>
   </si>
@@ -897,6 +897,27 @@
   </si>
   <si>
     <t>Trijicon ACOG TA31 Milspec 4x Scope</t>
+  </si>
+  <si>
+    <t>cosmic_tactical_saturn_scope_mount</t>
+  </si>
+  <si>
+    <t>Cosmic Tactical SATURN Scope Mount</t>
+  </si>
+  <si>
+    <t>Cosmic Tactical SATURN 4x Red Fiber Scope</t>
+  </si>
+  <si>
+    <t>Cosmic Tactical SATURN 4x Green Fiber Scope</t>
+  </si>
+  <si>
+    <t>cosmic_tactical_saturn_4x_red_scope</t>
+  </si>
+  <si>
+    <t>cosmic_tactical_saturn_4x_green_scope</t>
+  </si>
+  <si>
+    <t>https://www.trijicon.com/uploads/product-uploads/product-downloads/2020_Trijicon_ACOG.pdf</t>
   </si>
 </sst>
 </file>
@@ -1738,20 +1759,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R169"/>
+  <dimension ref="A1:S173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K123" sqref="K123"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I100" sqref="I100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.44140625" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" customWidth="1"/>
-    <col min="3" max="21" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" customWidth="1"/>
+    <col min="3" max="21" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1769,7 +1790,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1822,7 +1843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1855,7 +1876,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1888,7 +1909,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1921,7 +1942,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1960,7 +1981,7 @@
         <v>479.99</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -1999,7 +2020,7 @@
         <v>499.39</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2038,7 +2059,7 @@
         <v>448.52</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2077,7 +2098,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2100,7 +2121,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2133,7 +2154,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2166,7 +2187,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2199,7 +2220,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2224,7 +2245,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -2260,7 +2281,7 @@
         <v>4.4699999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -2296,7 +2317,7 @@
         <v>3.8199999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2319,7 +2340,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2344,7 +2365,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -2369,7 +2390,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2394,7 +2415,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N21" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2404,7 +2425,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -2429,7 +2450,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -2454,7 +2475,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2479,7 +2500,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2504,7 +2525,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -2529,7 +2550,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>75</v>
       </c>
@@ -2554,7 +2575,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2579,7 +2600,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2607,7 +2628,7 @@
         <v>6.5500000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2632,7 +2653,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2657,7 +2678,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -2682,7 +2703,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -2707,7 +2728,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -2732,7 +2753,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2760,7 +2781,7 @@
         <v>369.99</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2788,7 +2809,7 @@
         <v>0.11879999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -2813,7 +2834,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>98</v>
       </c>
@@ -2844,7 +2865,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -2875,7 +2896,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -2903,7 +2924,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2928,7 +2949,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -2953,7 +2974,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -2978,7 +2999,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>110</v>
       </c>
@@ -3003,7 +3024,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N45" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3013,7 +3034,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>112</v>
       </c>
@@ -3038,7 +3059,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>114</v>
       </c>
@@ -3063,7 +3084,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>116</v>
       </c>
@@ -3088,7 +3109,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -3119,7 +3140,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N50" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3129,7 +3150,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>120</v>
       </c>
@@ -3160,7 +3181,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -3191,7 +3212,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -3219,7 +3240,7 @@
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>130</v>
       </c>
@@ -3250,7 +3271,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -3275,7 +3296,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>134</v>
       </c>
@@ -3300,7 +3321,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>136</v>
       </c>
@@ -3325,7 +3346,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -3350,7 +3371,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>140</v>
       </c>
@@ -3375,7 +3396,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -3403,7 +3424,7 @@
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3428,7 +3449,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>138</v>
       </c>
@@ -3453,7 +3474,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -3478,7 +3499,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -3503,7 +3524,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -3528,7 +3549,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>150</v>
       </c>
@@ -3553,7 +3574,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N67" s="1">
         <f t="shared" ref="N67:N96" si="7">C67-D67*20-E67*0.8-F67*0.6-H67*5+I67*10+J67/300</f>
         <v>0</v>
@@ -3563,7 +3584,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -3588,7 +3609,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>178</v>
       </c>
@@ -3616,7 +3637,7 @@
         <v>7.46E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>180</v>
       </c>
@@ -3641,7 +3662,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N71" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3651,7 +3672,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>197</v>
       </c>
@@ -3676,7 +3697,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>195</v>
       </c>
@@ -3701,7 +3722,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>199</v>
       </c>
@@ -3729,7 +3750,7 @@
         <v>0.1123</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N75" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3739,7 +3760,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>201</v>
       </c>
@@ -3764,7 +3785,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>203</v>
       </c>
@@ -3792,7 +3813,7 @@
         <v>0.22539999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N78" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3802,7 +3823,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -3830,7 +3851,7 @@
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -3858,7 +3879,7 @@
         <v>0.124</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>156</v>
       </c>
@@ -3886,7 +3907,7 @@
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -3914,7 +3935,7 @@
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -3945,7 +3966,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -3976,7 +3997,7 @@
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>174</v>
       </c>
@@ -4004,7 +4025,7 @@
         <v>0.15665079999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -4032,7 +4053,7 @@
         <v>0.16215408999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>166</v>
       </c>
@@ -4060,7 +4081,7 @@
         <v>0.16169999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>168</v>
       </c>
@@ -4088,7 +4109,7 @@
         <v>0.20069999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -4113,7 +4134,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -4141,7 +4162,7 @@
         <v>0.17079999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N91" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4151,7 +4172,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>32</v>
       </c>
@@ -4184,7 +4205,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>34</v>
       </c>
@@ -4217,7 +4238,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>54</v>
       </c>
@@ -4242,7 +4263,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>56</v>
       </c>
@@ -4267,7 +4288,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>64</v>
       </c>
@@ -4292,7 +4313,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>58</v>
       </c>
@@ -4303,24 +4324,24 @@
         <v>-3</v>
       </c>
       <c r="D97">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="M97">
         <v>1200</v>
       </c>
       <c r="N97" s="1">
         <f t="shared" ref="N97:N102" si="11">C97-D97*20-E97*0.8-F97*0.6-H97*5+I97*10+J97/300</f>
-        <v>-5.4</v>
+        <v>-5</v>
       </c>
       <c r="P97">
-        <v>7.9</v>
+        <v>6.1</v>
       </c>
       <c r="Q97">
         <f t="shared" si="10"/>
-        <v>0.1227</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+        <v>9.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>60</v>
       </c>
@@ -4331,21 +4352,21 @@
         <v>-3</v>
       </c>
       <c r="D98">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="M98">
         <v>1200</v>
       </c>
       <c r="N98" s="1">
         <f t="shared" si="11"/>
-        <v>-5.4</v>
+        <v>-5</v>
       </c>
       <c r="Q98">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>61</v>
       </c>
@@ -4356,21 +4377,21 @@
         <v>-3</v>
       </c>
       <c r="D99">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="M99">
         <v>1500</v>
       </c>
       <c r="N99" s="1">
         <f t="shared" si="11"/>
-        <v>-5.4</v>
+        <v>-5</v>
       </c>
       <c r="Q99">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>62</v>
       </c>
@@ -4381,21 +4402,21 @@
         <v>-3</v>
       </c>
       <c r="D100">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="M100">
         <v>1500</v>
       </c>
       <c r="N100" s="1">
         <f t="shared" si="11"/>
-        <v>-5.4</v>
+        <v>-5</v>
       </c>
       <c r="Q100">
         <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>63</v>
       </c>
@@ -4423,7 +4444,7 @@
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4446,7 +4467,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -4471,7 +4492,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -4502,7 +4523,7 @@
         <v>0.24879999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N105" s="1">
         <f>C105-D105*20-E105*0.8-F105*0.6-H105*5+I105*10+J105/300</f>
         <v>0</v>
@@ -4512,7 +4533,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>209</v>
       </c>
@@ -4537,7 +4558,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>211</v>
       </c>
@@ -4568,17 +4589,17 @@
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N108" s="1">
-        <f t="shared" ref="N108:N141" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
+        <f t="shared" ref="N108:N145" si="12">C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
         <v>0</v>
       </c>
       <c r="Q108">
-        <f t="shared" ref="Q108:Q156" si="13">P108*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Q108:Q160" si="13">P108*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>213</v>
       </c>
@@ -4603,7 +4624,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -4631,7 +4652,7 @@
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N111" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4641,7 +4662,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -4666,7 +4687,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>219</v>
       </c>
@@ -4694,7 +4715,7 @@
         <v>0.14381161000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -4719,7 +4740,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N115" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -4729,7 +4750,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>225</v>
       </c>
@@ -4756,8 +4777,11 @@
         <f t="shared" si="13"/>
         <v>7.1999999999999995E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S116" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>223</v>
       </c>
@@ -4782,7 +4806,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -4793,17 +4817,17 @@
         <v>-3</v>
       </c>
       <c r="D118">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="F118">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M118">
         <v>1000</v>
       </c>
       <c r="N118" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
+        <v>-6</v>
       </c>
       <c r="P118">
         <v>16.600000000000001</v>
@@ -4813,7 +4837,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>275</v>
       </c>
@@ -4824,24 +4848,24 @@
         <v>-3</v>
       </c>
       <c r="D119">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="F119">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M119">
         <v>1000</v>
       </c>
       <c r="N119" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
+        <v>-6</v>
       </c>
       <c r="Q119">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>229</v>
       </c>
@@ -4852,7 +4876,7 @@
         <v>-3</v>
       </c>
       <c r="D120">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="F120">
         <v>-2</v>
@@ -4862,17 +4886,17 @@
       </c>
       <c r="N120" s="1">
         <f t="shared" si="12"/>
-        <v>-6.6</v>
+        <v>-5.8</v>
       </c>
       <c r="P120">
-        <v>17.600000000000001</v>
+        <v>14</v>
       </c>
       <c r="Q120">
         <f t="shared" si="13"/>
-        <v>0.24879999999999999</v>
-      </c>
-    </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.20199999999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>276</v>
       </c>
@@ -4883,7 +4907,7 @@
         <v>-3</v>
       </c>
       <c r="D121">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="F121">
         <v>-2</v>
@@ -4893,14 +4917,14 @@
       </c>
       <c r="N121" s="1">
         <f t="shared" si="12"/>
-        <v>-6.6</v>
+        <v>-5.8</v>
       </c>
       <c r="Q121">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>279</v>
       </c>
@@ -4911,7 +4935,7 @@
         <v>-3</v>
       </c>
       <c r="D122">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="F122">
         <v>-1</v>
@@ -4921,17 +4945,17 @@
       </c>
       <c r="N122" s="1">
         <f t="shared" si="12"/>
-        <v>-6.8000000000000007</v>
+        <v>-5.6000000000000005</v>
       </c>
       <c r="P122">
-        <v>15.6</v>
+        <v>10.9</v>
       </c>
       <c r="Q122">
         <f t="shared" si="13"/>
-        <v>0.22279999999999997</v>
-      </c>
-    </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.16169999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>281</v>
       </c>
@@ -4942,7 +4966,7 @@
         <v>-3</v>
       </c>
       <c r="D123">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="F123">
         <v>-1</v>
@@ -4952,14 +4976,14 @@
       </c>
       <c r="N123" s="1">
         <f t="shared" si="12"/>
-        <v>-6.8000000000000007</v>
+        <v>-5.6000000000000005</v>
       </c>
       <c r="Q123">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>282</v>
       </c>
@@ -4970,27 +4994,27 @@
         <v>-3</v>
       </c>
       <c r="D124">
-        <v>0.17</v>
-      </c>
-      <c r="H124">
-        <v>0.05</v>
+        <v>0.16</v>
+      </c>
+      <c r="F124">
+        <v>-1</v>
       </c>
       <c r="M124">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="N124" s="1">
         <f t="shared" si="12"/>
-        <v>-6.65</v>
+        <v>-5.6000000000000005</v>
       </c>
       <c r="P124">
-        <v>10.9</v>
+        <v>10.5</v>
       </c>
       <c r="Q124">
         <f t="shared" si="13"/>
-        <v>0.16169999999999998</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.15649999999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>283</v>
       </c>
@@ -5001,20 +5025,24 @@
         <v>-3</v>
       </c>
       <c r="D125">
-        <v>0.17</v>
-      </c>
-      <c r="H125">
-        <v>0.05</v>
+        <v>0.16</v>
+      </c>
+      <c r="F125">
+        <v>-1</v>
       </c>
       <c r="M125">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="N125" s="1">
         <f t="shared" si="12"/>
-        <v>-6.65</v>
-      </c>
-    </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-5.6000000000000005</v>
+      </c>
+      <c r="Q125">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>284</v>
       </c>
@@ -5025,17 +5053,24 @@
         <v>-3</v>
       </c>
       <c r="D126">
-        <v>0.17</v>
+        <v>0.16</v>
+      </c>
+      <c r="F126">
+        <v>-1</v>
       </c>
       <c r="M126">
-        <v>1800</v>
+        <v>1600</v>
       </c>
       <c r="N126" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-5.6000000000000005</v>
+      </c>
+      <c r="Q126">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>285</v>
       </c>
@@ -5046,17 +5081,24 @@
         <v>-3</v>
       </c>
       <c r="D127">
-        <v>0.17</v>
+        <v>0.16</v>
+      </c>
+      <c r="F127">
+        <v>-1</v>
       </c>
       <c r="M127">
-        <v>1800</v>
+        <v>1600</v>
       </c>
       <c r="N127" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+        <v>-5.6000000000000005</v>
+      </c>
+      <c r="Q127">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N128" s="1">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5066,140 +5108,131 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>231</v>
+        <v>288</v>
       </c>
       <c r="B129" t="s">
-        <v>232</v>
-      </c>
-      <c r="C129">
-        <v>-0.5</v>
+        <v>289</v>
       </c>
       <c r="D129">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="M129">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="N129" s="1">
         <f t="shared" si="12"/>
-        <v>-1.7</v>
-      </c>
-      <c r="P129">
-        <v>6.5</v>
+        <v>-0.8</v>
       </c>
       <c r="Q129">
         <f t="shared" si="13"/>
-        <v>0.1045</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>249</v>
+        <v>292</v>
       </c>
       <c r="B130" t="s">
-        <v>250</v>
+        <v>290</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D130">
-        <v>0.01</v>
+        <v>0.2</v>
+      </c>
+      <c r="F130">
+        <v>-1</v>
       </c>
       <c r="M130">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N130" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>-6.4</v>
+      </c>
+      <c r="P130">
+        <v>16.54</v>
       </c>
       <c r="Q130">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.23501999999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="B131" t="s">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D131">
-        <v>0.03</v>
+        <v>0.2</v>
+      </c>
+      <c r="F131">
+        <v>-1</v>
       </c>
       <c r="M131">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="N131" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>-6.4</v>
       </c>
       <c r="Q131">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>259</v>
-      </c>
-      <c r="B132" t="s">
-        <v>260</v>
-      </c>
-      <c r="C132">
-        <v>0</v>
-      </c>
-      <c r="D132">
-        <v>0.02</v>
-      </c>
-      <c r="M132">
-        <v>200</v>
-      </c>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N132" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="Q132">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="B133" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D133">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="M133">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="N133" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>-1.7</v>
+      </c>
+      <c r="P133">
+        <v>6.5</v>
       </c>
       <c r="Q133">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.1045</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B134" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -5208,7 +5241,7 @@
         <v>0.01</v>
       </c>
       <c r="M134">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N134" s="1">
         <f t="shared" si="12"/>
@@ -5219,37 +5252,37 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B135" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C135">
         <v>0</v>
       </c>
       <c r="D135">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M135">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N135" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="Q135">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B136" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -5258,7 +5291,7 @@
         <v>0.02</v>
       </c>
       <c r="M136">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N136" s="1">
         <f t="shared" si="12"/>
@@ -5269,679 +5302,697 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="B137" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="C137">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D137">
-        <v>0.11</v>
+        <v>0.03</v>
       </c>
       <c r="M137">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="N137" s="1">
         <f t="shared" si="12"/>
-        <v>-3.2</v>
-      </c>
-      <c r="P137">
-        <v>8.6999999999999993</v>
+        <v>-0.6</v>
       </c>
       <c r="Q137">
         <f t="shared" si="13"/>
-        <v>0.1331</v>
-      </c>
-    </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="B138" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="C138">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="M138">
-        <v>750</v>
+        <v>200</v>
       </c>
       <c r="N138" s="1">
         <f t="shared" si="12"/>
-        <v>-3.5</v>
-      </c>
-      <c r="P138">
-        <v>7.5</v>
+        <v>-0.2</v>
       </c>
       <c r="Q138">
         <f t="shared" si="13"/>
-        <v>0.11749999999999999</v>
-      </c>
-    </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="B139" t="s">
-        <v>238</v>
+        <v>264</v>
       </c>
       <c r="C139">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="M139">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N139" s="1">
         <f t="shared" si="12"/>
-        <v>-2.8</v>
-      </c>
-      <c r="P139">
-        <v>6.7</v>
+        <v>-0.4</v>
       </c>
       <c r="Q139">
         <f t="shared" si="13"/>
-        <v>0.1071</v>
-      </c>
-    </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="B140" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="C140">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="M140">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N140" s="1">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-0.4</v>
       </c>
       <c r="Q140">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B141" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C141">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="D141">
-        <v>0.27</v>
-      </c>
-      <c r="F141">
-        <v>-2</v>
+        <v>0.11</v>
       </c>
       <c r="M141">
-        <v>4000</v>
+        <v>800</v>
       </c>
       <c r="N141" s="1">
         <f t="shared" si="12"/>
-        <v>-9.2000000000000011</v>
+        <v>-3.2</v>
       </c>
       <c r="P141">
-        <v>20.100000000000001</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Q141">
         <f t="shared" si="13"/>
-        <v>0.28130000000000005</v>
-      </c>
-    </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.1331</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>235</v>
+      </c>
+      <c r="B142" t="s">
+        <v>236</v>
+      </c>
+      <c r="C142">
+        <v>-1.5</v>
+      </c>
+      <c r="D142">
+        <v>0.1</v>
+      </c>
+      <c r="M142">
+        <v>750</v>
+      </c>
       <c r="N142" s="1">
-        <f t="shared" ref="N142:N157" si="14">C142-D142*20-E142*0.8-F142*0.6-H142*5+I142*10+J142/300</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-3.5</v>
+      </c>
+      <c r="P142">
+        <v>7.5</v>
       </c>
       <c r="Q142">
         <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.11749999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>237</v>
+      </c>
+      <c r="B143" t="s">
+        <v>238</v>
+      </c>
+      <c r="C143">
+        <v>-1</v>
+      </c>
+      <c r="D143">
+        <v>0.09</v>
+      </c>
+      <c r="M143">
+        <v>500</v>
+      </c>
+      <c r="N143" s="1">
+        <f t="shared" si="12"/>
+        <v>-2.8</v>
+      </c>
+      <c r="P143">
+        <v>6.7</v>
+      </c>
+      <c r="Q143">
+        <f t="shared" si="13"/>
+        <v>0.1071</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B144" t="s">
+        <v>240</v>
+      </c>
+      <c r="C144">
+        <v>-1</v>
+      </c>
+      <c r="D144">
+        <v>0.1</v>
+      </c>
+      <c r="M144">
+        <v>500</v>
+      </c>
+      <c r="N144" s="1">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
+      <c r="Q144">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" t="s">
+        <v>242</v>
+      </c>
+      <c r="C145">
+        <v>-5</v>
+      </c>
+      <c r="D145">
+        <v>0.27</v>
+      </c>
+      <c r="F145">
+        <v>-2</v>
+      </c>
+      <c r="M145">
+        <v>4000</v>
+      </c>
+      <c r="N145" s="1">
+        <f t="shared" si="12"/>
+        <v>-9.2000000000000011</v>
+      </c>
+      <c r="P145">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="Q145">
+        <f t="shared" si="13"/>
+        <v>0.28130000000000005</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N146" s="1">
+        <f t="shared" ref="N146:N161" si="14">C146-D146*20-E146*0.8-F146*0.6-H146*5+I146*10+J146/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q146">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>245</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B147" t="s">
         <v>246</v>
       </c>
-      <c r="C143">
+      <c r="C147">
         <v>-0.5</v>
       </c>
-      <c r="D143">
+      <c r="D147">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M143">
+      <c r="M147">
         <v>1000</v>
       </c>
-      <c r="N143" s="1">
+      <c r="N147" s="1">
         <f t="shared" si="14"/>
         <v>-1.9000000000000001</v>
       </c>
-      <c r="P143">
+      <c r="P147">
         <v>6.6</v>
       </c>
-      <c r="Q143">
+      <c r="Q147">
         <f t="shared" si="13"/>
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>251</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B148" t="s">
         <v>252</v>
       </c>
-      <c r="C144">
-        <v>0</v>
-      </c>
-      <c r="D144">
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
         <v>0.01</v>
       </c>
-      <c r="M144">
-        <v>0</v>
-      </c>
-      <c r="N144" s="1">
+      <c r="M148">
+        <v>0</v>
+      </c>
+      <c r="N148" s="1">
         <f t="shared" si="14"/>
         <v>-0.2</v>
       </c>
-      <c r="Q144">
-        <f>P144*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+      <c r="Q148">
+        <f>P148*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>253</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B149" t="s">
         <v>254</v>
       </c>
-      <c r="C145">
-        <v>0</v>
-      </c>
-      <c r="D145">
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
         <v>0.03</v>
       </c>
-      <c r="M145">
+      <c r="M149">
         <v>200</v>
       </c>
-      <c r="N145" s="1">
+      <c r="N149" s="1">
         <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q145">
-        <f>P145*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="Q149">
+        <f>P149*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>257</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B150" t="s">
         <v>254</v>
       </c>
-      <c r="C146">
-        <v>0</v>
-      </c>
-      <c r="D146">
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
         <v>0.03</v>
       </c>
-      <c r="M146">
+      <c r="M150">
         <v>200</v>
       </c>
-      <c r="N146" s="1">
+      <c r="N150" s="1">
         <f t="shared" si="14"/>
         <v>-0.6</v>
       </c>
-      <c r="Q146">
-        <f>P146*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+      <c r="Q150">
+        <f>P150*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>247</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B151" t="s">
         <v>248</v>
       </c>
-      <c r="C147">
+      <c r="C151">
         <v>-1</v>
       </c>
-      <c r="D147">
+      <c r="D151">
         <v>0.11</v>
       </c>
-      <c r="M147">
+      <c r="M151">
         <v>500</v>
       </c>
-      <c r="N147" s="1">
+      <c r="N151" s="1">
         <f t="shared" si="14"/>
         <v>-3.2</v>
       </c>
-      <c r="P147">
+      <c r="P151">
         <v>7.0195183999999999</v>
       </c>
-      <c r="Q147">
+      <c r="Q151">
         <f t="shared" si="13"/>
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>243</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B152" t="s">
         <v>244</v>
       </c>
-      <c r="C148">
+      <c r="C152">
         <v>-7</v>
       </c>
-      <c r="D148">
+      <c r="D152">
         <v>0.42</v>
       </c>
-      <c r="F148">
+      <c r="F152">
         <v>-4</v>
       </c>
-      <c r="M148">
+      <c r="M152">
         <v>5000</v>
       </c>
-      <c r="N148" s="1">
+      <c r="N152" s="1">
         <f t="shared" si="14"/>
         <v>-13</v>
       </c>
-      <c r="P148">
+      <c r="P152">
         <v>39.299999999999997</v>
       </c>
-      <c r="Q148">
+      <c r="Q152">
         <f t="shared" si="13"/>
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N149" s="1">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N153" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q149">
+      <c r="Q153">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B154" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C154" s="1">
         <v>-2</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D154" s="1">
         <v>0.21</v>
       </c>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-      <c r="G150" s="1"/>
-      <c r="H150" s="1"/>
-      <c r="I150" s="1"/>
-      <c r="J150" s="1"/>
-      <c r="K150" s="1"/>
-      <c r="L150" s="1"/>
-      <c r="M150" s="1">
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1">
         <v>1000</v>
       </c>
-      <c r="N150" s="1">
+      <c r="N154" s="1">
         <f t="shared" si="14"/>
         <v>-6.2</v>
       </c>
-      <c r="P150">
+      <c r="P154">
         <v>15</v>
       </c>
-      <c r="Q150">
+      <c r="Q154">
         <f t="shared" si="13"/>
         <v>0.21499999999999997</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>181</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B155" t="s">
         <v>182</v>
       </c>
-      <c r="C151">
+      <c r="C155">
         <v>-2.5</v>
       </c>
-      <c r="D151">
+      <c r="D155">
         <v>0.22</v>
       </c>
-      <c r="F151">
+      <c r="F155">
         <v>-1</v>
       </c>
-      <c r="M151">
+      <c r="M155">
         <v>1000</v>
       </c>
-      <c r="N151" s="1">
+      <c r="N155" s="1">
         <f t="shared" si="14"/>
         <v>-6.3000000000000007</v>
       </c>
-      <c r="P151">
+      <c r="P155">
         <v>15.4</v>
       </c>
-      <c r="Q151">
+      <c r="Q155">
         <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>183</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B156" t="s">
         <v>184</v>
       </c>
-      <c r="C152">
+      <c r="C156">
         <v>-5</v>
       </c>
-      <c r="D152">
+      <c r="D156">
         <v>0.26</v>
       </c>
-      <c r="F152">
+      <c r="F156">
         <v>-2</v>
       </c>
-      <c r="M152">
+      <c r="M156">
         <v>2000</v>
       </c>
-      <c r="N152" s="1">
+      <c r="N156" s="1">
         <f t="shared" si="14"/>
         <v>-9</v>
       </c>
-      <c r="P152">
+      <c r="P156">
         <v>17.3</v>
       </c>
-      <c r="Q152">
+      <c r="Q156">
         <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>187</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B157" t="s">
         <v>188</v>
       </c>
-      <c r="C153">
+      <c r="C157">
         <v>-3</v>
       </c>
-      <c r="D153">
+      <c r="D157">
         <v>0.33</v>
       </c>
-      <c r="F153">
+      <c r="F157">
         <v>-3</v>
       </c>
-      <c r="M153">
+      <c r="M157">
         <v>3000</v>
       </c>
-      <c r="N153" s="1">
+      <c r="N157" s="1">
         <f t="shared" si="14"/>
         <v>-7.8000000000000016</v>
       </c>
-      <c r="P153">
+      <c r="P157">
         <v>24.162700000000001</v>
       </c>
-      <c r="Q153">
+      <c r="Q157">
         <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>189</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B158" t="s">
         <v>190</v>
       </c>
-      <c r="C154">
+      <c r="C158">
         <v>-3</v>
       </c>
-      <c r="D154">
+      <c r="D158">
         <v>0.24</v>
       </c>
-      <c r="F154">
+      <c r="F158">
         <v>-2</v>
       </c>
-      <c r="M154">
+      <c r="M158">
         <v>3000</v>
       </c>
-      <c r="N154" s="1">
+      <c r="N158" s="1">
         <f t="shared" si="14"/>
         <v>-6.6</v>
       </c>
-      <c r="P154">
+      <c r="P158">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q154">
+      <c r="Q158">
         <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>191</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B159" t="s">
         <v>192</v>
       </c>
-      <c r="C155">
+      <c r="C159">
         <v>-3</v>
       </c>
-      <c r="D155">
+      <c r="D159">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F155">
+      <c r="F159">
         <v>-1</v>
       </c>
-      <c r="M155">
+      <c r="M159">
         <v>4000</v>
       </c>
-      <c r="N155" s="1">
+      <c r="N159" s="1">
         <f t="shared" si="14"/>
         <v>-8.0000000000000018</v>
       </c>
-      <c r="P155">
+      <c r="P159">
         <v>21.9</v>
       </c>
-      <c r="Q155">
+      <c r="Q159">
         <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>193</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B160" t="s">
         <v>194</v>
       </c>
-      <c r="C156">
+      <c r="C160">
         <v>-3</v>
       </c>
-      <c r="D156">
+      <c r="D160">
         <v>0.27</v>
       </c>
-      <c r="F156">
+      <c r="F160">
         <v>-2</v>
       </c>
-      <c r="M156">
+      <c r="M160">
         <v>2000</v>
       </c>
-      <c r="N156" s="1">
+      <c r="N160" s="1">
         <f t="shared" si="14"/>
         <v>-7.2</v>
       </c>
-      <c r="P156">
+      <c r="P160">
         <v>19.3</v>
       </c>
-      <c r="Q156">
+      <c r="Q160">
         <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N157" s="1">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N161" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
-      </c>
-      <c r="Q157">
-        <f>P157*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>271</v>
-      </c>
-      <c r="B158" t="s">
-        <v>272</v>
-      </c>
-      <c r="C158">
-        <v>-2</v>
-      </c>
-      <c r="D158">
-        <v>0.05</v>
-      </c>
-      <c r="M158">
-        <v>300</v>
-      </c>
-      <c r="N158" s="1"/>
-      <c r="Q158">
-        <f t="shared" ref="Q158:Q169" si="15">P158*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>267</v>
-      </c>
-      <c r="B159" t="s">
-        <v>268</v>
-      </c>
-      <c r="C159">
-        <v>-2</v>
-      </c>
-      <c r="D159">
-        <v>0.05</v>
-      </c>
-      <c r="M159">
-        <v>300</v>
-      </c>
-      <c r="N159" s="1"/>
-      <c r="Q159">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>273</v>
-      </c>
-      <c r="B160" t="s">
-        <v>274</v>
-      </c>
-      <c r="C160">
-        <v>-3</v>
-      </c>
-      <c r="D160">
-        <v>0.17</v>
-      </c>
-      <c r="M160">
-        <v>750</v>
-      </c>
-      <c r="N160" s="1"/>
-      <c r="P160">
-        <v>13.3</v>
-      </c>
-      <c r="Q160">
-        <f>P160*0.013+0.02</f>
-        <v>0.19289999999999999</v>
-      </c>
-    </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>269</v>
-      </c>
-      <c r="B161" t="s">
-        <v>270</v>
-      </c>
-      <c r="C161">
-        <v>-3</v>
-      </c>
-      <c r="D161">
-        <v>0.18</v>
-      </c>
-      <c r="M161">
-        <v>1000</v>
-      </c>
-      <c r="N161" s="1"/>
-      <c r="P161">
-        <v>13.28</v>
       </c>
       <c r="Q161">
         <f>P161*0.013+0.02</f>
-        <v>0.19263999999999998</v>
-      </c>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>271</v>
+      </c>
+      <c r="B162" t="s">
+        <v>272</v>
+      </c>
+      <c r="C162">
+        <v>-2</v>
+      </c>
+      <c r="D162">
+        <v>0.05</v>
+      </c>
+      <c r="M162">
+        <v>300</v>
+      </c>
       <c r="N162" s="1"/>
       <c r="Q162">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Q162:Q173" si="15">P162*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B163" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C163">
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="D163">
-        <v>0.36</v>
-      </c>
-      <c r="F163">
-        <v>-3</v>
+        <v>0.05</v>
       </c>
       <c r="M163">
-        <v>3000</v>
+        <v>300</v>
       </c>
       <c r="N163" s="1"/>
       <c r="Q163">
@@ -5949,42 +6000,124 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>273</v>
+      </c>
+      <c r="B164" t="s">
+        <v>274</v>
+      </c>
+      <c r="C164">
+        <v>-3</v>
+      </c>
+      <c r="D164">
+        <v>0.17</v>
+      </c>
+      <c r="M164">
+        <v>750</v>
+      </c>
       <c r="N164" s="1"/>
+      <c r="P164">
+        <v>13.3</v>
+      </c>
       <c r="Q164">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+        <f>P164*0.013+0.02</f>
+        <v>0.19289999999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>269</v>
+      </c>
+      <c r="B165" t="s">
+        <v>270</v>
+      </c>
+      <c r="C165">
+        <v>-3</v>
+      </c>
+      <c r="D165">
+        <v>0.18</v>
+      </c>
+      <c r="M165">
+        <v>1000</v>
+      </c>
       <c r="N165" s="1"/>
+      <c r="P165">
+        <v>13.28</v>
+      </c>
       <c r="Q165">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+        <f>P165*0.013+0.02</f>
+        <v>0.19263999999999998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N166" s="1"/>
       <c r="Q166">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>277</v>
+      </c>
+      <c r="B167" t="s">
+        <v>278</v>
+      </c>
+      <c r="C167">
+        <v>-8</v>
+      </c>
+      <c r="D167">
+        <v>0.36</v>
+      </c>
+      <c r="F167">
+        <v>-3</v>
+      </c>
+      <c r="M167">
+        <v>3000</v>
+      </c>
       <c r="N167" s="1"/>
       <c r="Q167">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N168" s="1"/>
       <c r="Q168">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N169" s="1"/>
       <c r="Q169">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N170" s="1"/>
+      <c r="Q170">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N171" s="1"/>
+      <c r="Q171">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q172">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q173">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>

</xml_diff>

<commit_message>
add monstrum scope mount
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80FD72B-F843-40AD-B15F-0C04A1DC6E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BF4175-B590-4082-AD42-9167A2B26976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="297">
   <si>
     <t>new</t>
   </si>
@@ -918,6 +918,12 @@
   </si>
   <si>
     <t>monstrum_tactical_s232p_2x32_prism_scope</t>
+  </si>
+  <si>
+    <t>monstrum_tactical_compact_scope_mount</t>
+  </si>
+  <si>
+    <t>Monstrum Tactical Compact Scope Mount</t>
   </si>
 </sst>
 </file>
@@ -1759,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S173"/>
+  <dimension ref="A1:S175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154"/>
+    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M155" sqref="M155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4595,7 +4601,7 @@
         <v>0</v>
       </c>
       <c r="Q108">
-        <f t="shared" ref="Q108:Q160" si="13">P108*0.013+0.02</f>
+        <f t="shared" ref="Q108:Q162" si="13">P108*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
@@ -5544,7 +5550,7 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N146" s="1">
-        <f t="shared" ref="N146:N161" si="14">C146-D146*20-E146*0.8-F146*0.6-H146*5+I146*10+J146/300</f>
+        <f t="shared" ref="N146:N163" si="14">C146-D146*20-E146*0.8-F146*0.6-H146*5+I146*10+J146/300</f>
         <v>0</v>
       </c>
       <c r="Q146">
@@ -5715,371 +5721,373 @@
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N153" s="1">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="Q153">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
+      <c r="N153" s="1"/>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C154" s="1">
-        <v>-2</v>
-      </c>
-      <c r="D154" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="E154" s="1"/>
-      <c r="F154" s="1"/>
-      <c r="G154" s="1"/>
-      <c r="H154" s="1"/>
-      <c r="I154" s="1"/>
-      <c r="J154" s="1"/>
-      <c r="K154" s="1"/>
-      <c r="L154" s="1"/>
-      <c r="M154" s="1">
-        <v>1000</v>
+      <c r="A154" t="s">
+        <v>295</v>
+      </c>
+      <c r="B154" t="s">
+        <v>296</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>0.05</v>
+      </c>
+      <c r="M154">
+        <v>400</v>
       </c>
       <c r="N154" s="1">
         <f t="shared" si="14"/>
-        <v>-6.2</v>
-      </c>
-      <c r="P154">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="Q154">
         <f t="shared" si="13"/>
-        <v>0.21499999999999997</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>181</v>
-      </c>
-      <c r="B155" t="s">
-        <v>182</v>
-      </c>
-      <c r="C155">
-        <v>-2.5</v>
-      </c>
-      <c r="D155">
-        <v>0.22</v>
-      </c>
-      <c r="F155">
-        <v>-1</v>
-      </c>
-      <c r="M155">
+      <c r="A155" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C155" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="M155" s="1">
         <v>1000</v>
       </c>
       <c r="N155" s="1">
         <f t="shared" si="14"/>
-        <v>-6.3000000000000007</v>
+        <v>-5.2</v>
       </c>
       <c r="P155">
-        <v>15.4</v>
+        <v>15</v>
       </c>
       <c r="Q155">
         <f t="shared" si="13"/>
+        <v>0.21499999999999997</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>181</v>
+      </c>
+      <c r="B157" t="s">
+        <v>182</v>
+      </c>
+      <c r="C157">
+        <v>-2.5</v>
+      </c>
+      <c r="D157">
+        <v>0.22</v>
+      </c>
+      <c r="F157">
+        <v>-1</v>
+      </c>
+      <c r="M157">
+        <v>1000</v>
+      </c>
+      <c r="N157" s="1">
+        <f t="shared" si="14"/>
+        <v>-6.3000000000000007</v>
+      </c>
+      <c r="P157">
+        <v>15.4</v>
+      </c>
+      <c r="Q157">
+        <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>183</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B158" t="s">
         <v>184</v>
       </c>
-      <c r="C156">
+      <c r="C158">
         <v>-5</v>
       </c>
-      <c r="D156">
+      <c r="D158">
         <v>0.26</v>
       </c>
-      <c r="F156">
+      <c r="F158">
         <v>-2</v>
       </c>
-      <c r="M156">
+      <c r="M158">
         <v>2000</v>
       </c>
-      <c r="N156" s="1">
+      <c r="N158" s="1">
         <f t="shared" si="14"/>
         <v>-9</v>
       </c>
-      <c r="P156">
+      <c r="P158">
         <v>17.3</v>
       </c>
-      <c r="Q156">
+      <c r="Q158">
         <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>186</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B159" t="s">
         <v>187</v>
       </c>
-      <c r="C157">
+      <c r="C159">
         <v>-3</v>
       </c>
-      <c r="D157">
+      <c r="D159">
         <v>0.33</v>
       </c>
-      <c r="F157">
+      <c r="F159">
         <v>-3</v>
       </c>
-      <c r="M157">
+      <c r="M159">
         <v>3000</v>
       </c>
-      <c r="N157" s="1">
+      <c r="N159" s="1">
         <f t="shared" si="14"/>
         <v>-7.8000000000000016</v>
       </c>
-      <c r="P157">
+      <c r="P159">
         <v>24.162700000000001</v>
       </c>
-      <c r="Q157">
+      <c r="Q159">
         <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>188</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>189</v>
       </c>
-      <c r="C158">
+      <c r="C160">
         <v>-3</v>
       </c>
-      <c r="D158">
+      <c r="D160">
         <v>0.24</v>
       </c>
-      <c r="F158">
+      <c r="F160">
         <v>-2</v>
       </c>
-      <c r="M158">
+      <c r="M160">
         <v>3000</v>
       </c>
-      <c r="N158" s="1">
+      <c r="N160" s="1">
         <f t="shared" si="14"/>
         <v>-6.6</v>
       </c>
-      <c r="P158">
+      <c r="P160">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q158">
+      <c r="Q160">
         <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>190</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B161" t="s">
         <v>191</v>
       </c>
-      <c r="C159">
+      <c r="C161">
         <v>-3</v>
       </c>
-      <c r="D159">
+      <c r="D161">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F159">
+      <c r="F161">
         <v>-1</v>
       </c>
-      <c r="M159">
+      <c r="M161">
         <v>4000</v>
       </c>
-      <c r="N159" s="1">
+      <c r="N161" s="1">
         <f t="shared" si="14"/>
         <v>-8.0000000000000018</v>
       </c>
-      <c r="P159">
+      <c r="P161">
         <v>21.9</v>
       </c>
-      <c r="Q159">
+      <c r="Q161">
         <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>192</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B162" t="s">
         <v>193</v>
       </c>
-      <c r="C160">
+      <c r="C162">
         <v>-3</v>
       </c>
-      <c r="D160">
+      <c r="D162">
         <v>0.27</v>
       </c>
-      <c r="F160">
+      <c r="F162">
         <v>-2</v>
       </c>
-      <c r="M160">
+      <c r="M162">
         <v>2000</v>
       </c>
-      <c r="N160" s="1">
+      <c r="N162" s="1">
         <f t="shared" si="14"/>
         <v>-7.2</v>
       </c>
-      <c r="P160">
+      <c r="P162">
         <v>19.3</v>
       </c>
-      <c r="Q160">
+      <c r="Q162">
         <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N161" s="1">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N163" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q161">
-        <f>P161*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>270</v>
-      </c>
-      <c r="B162" t="s">
-        <v>271</v>
-      </c>
-      <c r="C162">
-        <v>-2</v>
-      </c>
-      <c r="D162">
-        <v>0.05</v>
-      </c>
-      <c r="M162">
-        <v>300</v>
-      </c>
-      <c r="N162" s="1"/>
-      <c r="Q162">
-        <f t="shared" ref="Q162:Q173" si="15">P162*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>266</v>
-      </c>
-      <c r="B163" t="s">
-        <v>267</v>
-      </c>
-      <c r="C163">
-        <v>-2</v>
-      </c>
-      <c r="D163">
-        <v>0.05</v>
-      </c>
-      <c r="M163">
-        <v>300</v>
-      </c>
-      <c r="N163" s="1"/>
       <c r="Q163">
-        <f t="shared" si="15"/>
+        <f>P163*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B164" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C164">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="D164">
-        <v>0.17</v>
+        <v>0.05</v>
       </c>
       <c r="M164">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="N164" s="1"/>
-      <c r="P164">
-        <v>13.3</v>
-      </c>
       <c r="Q164">
-        <f>P164*0.013+0.02</f>
-        <v>0.19289999999999999</v>
+        <f t="shared" ref="Q164:Q175" si="15">P164*0.013+0.02</f>
+        <v>0.02</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B165" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C165">
+        <v>-2</v>
+      </c>
+      <c r="D165">
+        <v>0.05</v>
+      </c>
+      <c r="M165">
+        <v>300</v>
+      </c>
+      <c r="N165" s="1"/>
+      <c r="Q165">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>272</v>
+      </c>
+      <c r="B166" t="s">
+        <v>273</v>
+      </c>
+      <c r="C166">
         <v>-3</v>
       </c>
-      <c r="D165">
-        <v>0.18</v>
-      </c>
-      <c r="M165">
-        <v>1000</v>
-      </c>
-      <c r="N165" s="1"/>
-      <c r="P165">
-        <v>13.28</v>
-      </c>
-      <c r="Q165">
-        <f>P165*0.013+0.02</f>
-        <v>0.19263999999999998</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D166">
+        <v>0.17</v>
+      </c>
+      <c r="M166">
+        <v>750</v>
+      </c>
       <c r="N166" s="1"/>
+      <c r="P166">
+        <v>13.3</v>
+      </c>
       <c r="Q166">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
+        <f>P166*0.013+0.02</f>
+        <v>0.19289999999999999</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B167" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C167">
-        <v>-8</v>
+        <v>-3</v>
       </c>
       <c r="D167">
-        <v>0.36</v>
-      </c>
-      <c r="F167">
-        <v>-3</v>
+        <v>0.18</v>
       </c>
       <c r="M167">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="N167" s="1"/>
+      <c r="P167">
+        <v>13.28</v>
+      </c>
       <c r="Q167">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
+        <f>P167*0.013+0.02</f>
+        <v>0.19263999999999998</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.25">
@@ -6090,6 +6098,24 @@
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>276</v>
+      </c>
+      <c r="B169" t="s">
+        <v>277</v>
+      </c>
+      <c r="C169">
+        <v>-8</v>
+      </c>
+      <c r="D169">
+        <v>0.36</v>
+      </c>
+      <c r="F169">
+        <v>-3</v>
+      </c>
+      <c r="M169">
+        <v>3000</v>
+      </c>
       <c r="N169" s="1"/>
       <c r="Q169">
         <f t="shared" si="15"/>
@@ -6111,13 +6137,27 @@
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N172" s="1"/>
       <c r="Q172">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N173" s="1"/>
       <c r="Q173">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q174">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q175">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>

</xml_diff>

<commit_message>
make the scar imperial bolt actually useful
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DBA052-39BB-4B36-9A2C-92557753D821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDAB5C5-3C3A-44FE-A4EC-08FB42BB9D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,9 +176,6 @@
     <t>eotech_eflx_mini_red_dot</t>
   </si>
   <si>
-    <t>Eotech EFLX Mini Red Dot</t>
-  </si>
-  <si>
     <t>sig_sauer_qd_1.41_cowitness_romeo3_riser</t>
   </si>
   <si>
@@ -398,99 +395,51 @@
     <t>eotech_553_holo_sight</t>
   </si>
   <si>
-    <t>Eotech 553</t>
-  </si>
-  <si>
     <t>eotech_552_holo_sight</t>
   </si>
   <si>
-    <t>Eotech 552</t>
-  </si>
-  <si>
     <t>eotech_512_holo_sight</t>
   </si>
   <si>
-    <t>Eotech 512</t>
-  </si>
-  <si>
     <t>eotech_exps3_holo_sight</t>
   </si>
   <si>
-    <t>Eotech EXPS-3</t>
-  </si>
-  <si>
     <t>eotech_exps2_holo_sight</t>
   </si>
   <si>
-    <t>Eotech EXPS-2</t>
-  </si>
-  <si>
     <t>eotech_xps3_holo_sight</t>
   </si>
   <si>
-    <t>Eotech XPS3</t>
-  </si>
-  <si>
     <t>eotech_xps2_holo_sight</t>
   </si>
   <si>
-    <t>Eotech XPS2</t>
-  </si>
-  <si>
     <t>eotech_xps2_green_holo_sight</t>
   </si>
   <si>
-    <t>Eotech XPS2 Green Holo Sight</t>
-  </si>
-  <si>
     <t>eotech_xps2z_zombie_stopper_holo_sight</t>
   </si>
   <si>
-    <t>Eotech XPS2Z Zombie Stopper Holo Sight</t>
-  </si>
-  <si>
     <t>eotech_exps2_green_holo_sight</t>
   </si>
   <si>
-    <t>Eotech EXPS2 Green Holo Sight</t>
-  </si>
-  <si>
     <t>eotech_exps2_mount</t>
   </si>
   <si>
-    <t>Eotech EXPS2 Mount</t>
-  </si>
-  <si>
     <t>eotech_exps3_mount</t>
   </si>
   <si>
-    <t>Eotech EXPS3 Mount</t>
-  </si>
-  <si>
     <t>eotech_exps2_hood</t>
   </si>
   <si>
-    <t>Eotech EXPS 2 Hood</t>
-  </si>
-  <si>
     <t>eotech_exps3_hood</t>
   </si>
   <si>
-    <t>Eotech EXPS 3 Hood</t>
-  </si>
-  <si>
     <t>eotech_exps2_green_hood</t>
   </si>
   <si>
-    <t>Eotech EXPS2 Green Hood</t>
-  </si>
-  <si>
     <t>eotech_553_hood</t>
   </si>
   <si>
-    <t>Eotech 553 Hood</t>
-  </si>
-  <si>
     <t>zenit_belomo_pk06</t>
   </si>
   <si>
@@ -942,6 +891,57 @@
   </si>
   <si>
     <t>Aimpoint Micro T-2 / H-2 Cordura Fabric Wrap</t>
+  </si>
+  <si>
+    <t>EOTECH EFLX Mini Red Dot</t>
+  </si>
+  <si>
+    <t>EOTECH 553</t>
+  </si>
+  <si>
+    <t>EOTECH 552</t>
+  </si>
+  <si>
+    <t>EOTECH 512</t>
+  </si>
+  <si>
+    <t>EOTECH XPS3</t>
+  </si>
+  <si>
+    <t>EOTECH XPS2</t>
+  </si>
+  <si>
+    <t>EOTECH XPS2 Green Holo Sight</t>
+  </si>
+  <si>
+    <t>EOTECH XPS2Z Zombie Stopper Holo Sight</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS3 Mount</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS2 Mount</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS-3</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS-2</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS2 Green Holo Sight</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS 3 Hood</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS 2 Hood</t>
+  </si>
+  <si>
+    <t>EOTECH EXPS2 Green Hood</t>
+  </si>
+  <si>
+    <t>EOTECH 553 Hood</t>
   </si>
 </sst>
 </file>
@@ -1785,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2310,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>286</v>
       </c>
       <c r="C16" s="1">
         <v>-1.5</v>
@@ -2366,10 +2366,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2391,10 +2391,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2416,10 +2416,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
       </c>
       <c r="C20">
         <v>-1.5</v>
@@ -2451,10 +2451,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
         <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2476,10 +2476,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
         <v>85</v>
-      </c>
-      <c r="B23" t="s">
-        <v>86</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2501,10 +2501,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
         <v>87</v>
-      </c>
-      <c r="B24" t="s">
-        <v>88</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2526,10 +2526,10 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>74</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2551,10 +2551,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
         <v>71</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -2576,10 +2576,10 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
         <v>75</v>
-      </c>
-      <c r="B27" t="s">
-        <v>76</v>
       </c>
       <c r="C27">
         <v>-0.5</v>
@@ -2601,10 +2601,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
         <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>70</v>
       </c>
       <c r="C28">
         <v>-0.5</v>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
         <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
         <v>79</v>
-      </c>
-      <c r="B30" t="s">
-        <v>80</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -2679,10 +2679,10 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
         <v>81</v>
-      </c>
-      <c r="B31" t="s">
-        <v>82</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -2704,10 +2704,10 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
         <v>83</v>
-      </c>
-      <c r="B32" t="s">
-        <v>84</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2729,10 +2729,10 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
         <v>92</v>
-      </c>
-      <c r="B33" t="s">
-        <v>93</v>
       </c>
       <c r="C33">
         <v>-0.5</v>
@@ -2754,10 +2754,10 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
         <v>94</v>
-      </c>
-      <c r="B34" t="s">
-        <v>95</v>
       </c>
       <c r="C34">
         <v>-0.5</v>
@@ -2779,10 +2779,10 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -2807,10 +2807,10 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
         <v>90</v>
-      </c>
-      <c r="B36" t="s">
-        <v>91</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -2835,10 +2835,10 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
         <v>96</v>
-      </c>
-      <c r="B37" t="s">
-        <v>97</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -2860,10 +2860,10 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" t="s">
         <v>98</v>
-      </c>
-      <c r="B38" t="s">
-        <v>99</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -2891,10 +2891,10 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="B39" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
         <v>100</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
       </c>
       <c r="C40">
         <v>-0.5</v>
@@ -2943,10 +2943,10 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
         <v>102</v>
-      </c>
-      <c r="B41" t="s">
-        <v>103</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -2971,10 +2971,10 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s">
         <v>106</v>
-      </c>
-      <c r="B42" t="s">
-        <v>107</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2996,10 +2996,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" t="s">
         <v>108</v>
-      </c>
-      <c r="B43" t="s">
-        <v>109</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -3021,10 +3021,10 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
         <v>104</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3046,10 +3046,10 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
         <v>110</v>
-      </c>
-      <c r="B45" t="s">
-        <v>111</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" t="s">
         <v>112</v>
-      </c>
-      <c r="B47" t="s">
-        <v>113</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -3106,10 +3106,10 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
         <v>114</v>
-      </c>
-      <c r="B48" t="s">
-        <v>115</v>
       </c>
       <c r="C48">
         <v>-0.5</v>
@@ -3131,10 +3131,10 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" t="s">
         <v>116</v>
-      </c>
-      <c r="B49" t="s">
-        <v>117</v>
       </c>
       <c r="C49">
         <v>-0.5</v>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
         <v>118</v>
-      </c>
-      <c r="B50" t="s">
-        <v>119</v>
       </c>
       <c r="C50">
         <v>-1</v>
@@ -3197,10 +3197,10 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>287</v>
       </c>
       <c r="C52">
         <v>-2</v>
@@ -3228,10 +3228,10 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>288</v>
       </c>
       <c r="C53">
         <v>-2</v>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>289</v>
       </c>
       <c r="C54">
         <v>-1</v>
@@ -3287,10 +3287,10 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>290</v>
       </c>
       <c r="C55">
         <v>-2</v>
@@ -3318,10 +3318,10 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>291</v>
       </c>
       <c r="C56">
         <v>-1</v>
@@ -3343,10 +3343,10 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>292</v>
       </c>
       <c r="C57">
         <v>-1</v>
@@ -3368,10 +3368,10 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>293</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -3393,10 +3393,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>294</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -3418,10 +3418,10 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B60" t="s">
-        <v>141</v>
+        <v>295</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -3443,10 +3443,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>296</v>
       </c>
       <c r="C61">
         <v>-2</v>
@@ -3471,10 +3471,10 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>297</v>
       </c>
       <c r="C62">
         <v>-1</v>
@@ -3496,10 +3496,10 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
-        <v>139</v>
+        <v>298</v>
       </c>
       <c r="C63">
         <v>-1</v>
@@ -3521,10 +3521,10 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>299</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3546,10 +3546,10 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>300</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -3571,10 +3571,10 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>149</v>
+        <v>301</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3596,10 +3596,10 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>302</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3631,10 +3631,10 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="B69" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -3656,10 +3656,10 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C70">
         <v>-2</v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C71">
         <v>-2</v>
@@ -3719,10 +3719,10 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C73">
         <v>-0.5</v>
@@ -3744,10 +3744,10 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="C74">
         <v>-1</v>
@@ -3769,10 +3769,10 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C75">
         <v>-2</v>
@@ -3807,10 +3807,10 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B77" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3832,10 +3832,10 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="C78">
         <v>-2</v>
@@ -3870,10 +3870,10 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C80">
         <v>-2.5</v>
@@ -3898,10 +3898,10 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C81">
         <v>-2</v>
@@ -3926,10 +3926,10 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C82">
         <v>-2.5</v>
@@ -3954,10 +3954,10 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C83">
         <v>-2</v>
@@ -3982,10 +3982,10 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C84">
         <v>-6</v>
@@ -4013,10 +4013,10 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="C85">
         <v>-7</v>
@@ -4044,10 +4044,10 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="C86">
         <v>-2</v>
@@ -4072,10 +4072,10 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C87">
         <v>-2</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B88" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C88">
         <v>-2</v>
@@ -4128,10 +4128,10 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B89" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C89">
         <v>-2.5</v>
@@ -4156,10 +4156,10 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B90" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C90">
         <v>-2</v>
@@ -4181,10 +4181,10 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B91" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C91">
         <v>-4</v>
@@ -4285,10 +4285,10 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95" t="s">
         <v>54</v>
-      </c>
-      <c r="B95" t="s">
-        <v>55</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -4310,10 +4310,10 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>55</v>
+      </c>
+      <c r="B96" t="s">
         <v>56</v>
-      </c>
-      <c r="B96" t="s">
-        <v>57</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -4335,10 +4335,10 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>63</v>
+      </c>
+      <c r="B97" t="s">
         <v>64</v>
-      </c>
-      <c r="B97" t="s">
-        <v>65</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -4360,10 +4360,10 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>57</v>
+      </c>
+      <c r="B98" t="s">
         <v>58</v>
-      </c>
-      <c r="B98" t="s">
-        <v>59</v>
       </c>
       <c r="C98">
         <v>-3</v>
@@ -4388,10 +4388,10 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B99" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C99">
         <v>-3</v>
@@ -4413,10 +4413,10 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B100" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C100">
         <v>-3</v>
@@ -4438,10 +4438,10 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B101" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C101">
         <v>-3</v>
@@ -4463,10 +4463,10 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B102" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C102">
         <v>-1</v>
@@ -4514,10 +4514,10 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B104" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -4539,10 +4539,10 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="B105" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="C105">
         <v>-3</v>
@@ -4580,10 +4580,10 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -4605,10 +4605,10 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="C108">
         <v>-3</v>
@@ -4646,10 +4646,10 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="B110" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -4671,10 +4671,10 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="B111" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="C111">
         <v>-3</v>
@@ -4709,10 +4709,10 @@
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="B113" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -4734,10 +4734,10 @@
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="B114" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="C114">
         <v>-3.5</v>
@@ -4762,10 +4762,10 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="B115" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="C115">
         <v>-3</v>
@@ -4797,10 +4797,10 @@
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="B117" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -4823,15 +4823,15 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="S117" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="B118" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="B119" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="C119">
         <v>-3</v>
@@ -4884,10 +4884,10 @@
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="C120">
         <v>-3</v>
@@ -4912,10 +4912,10 @@
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="C121">
         <v>-3</v>
@@ -4943,10 +4943,10 @@
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="B122" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="C122">
         <v>-3</v>
@@ -4971,10 +4971,10 @@
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B123" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C123">
         <v>-3</v>
@@ -5002,10 +5002,10 @@
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="B124" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C124">
         <v>-3</v>
@@ -5030,10 +5030,10 @@
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="B125" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C125">
         <v>-3</v>
@@ -5061,10 +5061,10 @@
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="B126" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="C126">
         <v>-3</v>
@@ -5089,10 +5089,10 @@
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="B127" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="C127">
         <v>-3</v>
@@ -5117,10 +5117,10 @@
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="B128" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="C128">
         <v>-3</v>
@@ -5155,10 +5155,10 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="B130" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="D130">
         <v>0.04</v>
@@ -5177,10 +5177,10 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="B131" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="C131">
         <v>-3</v>
@@ -5208,10 +5208,10 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="B132" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="C132">
         <v>-3</v>
@@ -5246,10 +5246,10 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="B134" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="C134">
         <v>-0.5</v>
@@ -5274,10 +5274,10 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="B135" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -5299,10 +5299,10 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="B136" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -5324,10 +5324,10 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="B137" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -5349,10 +5349,10 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B138" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -5374,10 +5374,10 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="B139" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -5399,10 +5399,10 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="B140" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -5424,10 +5424,10 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B141" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -5449,10 +5449,10 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="B142" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="C142">
         <v>-1</v>
@@ -5477,10 +5477,10 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="B143" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="C143">
         <v>-1.5</v>
@@ -5505,10 +5505,10 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="B144" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C144">
         <v>-1</v>
@@ -5533,10 +5533,10 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="B145" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="C145">
         <v>-1</v>
@@ -5558,10 +5558,10 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="B146" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="C146">
         <v>-5</v>
@@ -5599,10 +5599,10 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="B148" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="C148">
         <v>-0.5</v>
@@ -5627,10 +5627,10 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="B149" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -5652,10 +5652,10 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B150" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -5677,10 +5677,10 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="B151" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -5702,10 +5702,10 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="B152" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="C152">
         <v>-1</v>
@@ -5730,10 +5730,10 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="B153" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C153">
         <v>-7</v>
@@ -5764,10 +5764,10 @@
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="B155" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -5789,10 +5789,10 @@
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="C156" s="1">
         <v>-2</v>
@@ -5841,10 +5841,10 @@
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B158" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C158">
         <v>-2.5</v>
@@ -5872,10 +5872,10 @@
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B159" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C159">
         <v>-5</v>
@@ -5903,10 +5903,10 @@
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B160" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="C160">
         <v>-3</v>
@@ -5934,10 +5934,10 @@
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="B161" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C161">
         <v>-3</v>
@@ -5965,10 +5965,10 @@
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="B162" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="C162">
         <v>-3</v>
@@ -5996,10 +5996,10 @@
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B163" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="C163">
         <v>-3</v>
@@ -6037,10 +6037,10 @@
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="B165" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="C165">
         <v>-2</v>
@@ -6059,10 +6059,10 @@
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="B166" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="C166">
         <v>-2</v>
@@ -6081,10 +6081,10 @@
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B167" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="C167">
         <v>-3</v>
@@ -6106,10 +6106,10 @@
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B168" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="C168">
         <v>-3</v>
@@ -6138,10 +6138,10 @@
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="B170" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="C170">
         <v>-8</v>
@@ -6170,10 +6170,10 @@
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="B172" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="C172">
         <v>1</v>
@@ -6195,10 +6195,10 @@
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B173" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="C173">
         <v>-3</v>

</xml_diff>

<commit_message>
port kac aimpoint nvg high rise
</commit_message>
<xml_diff>
--- a/changes/optics.xlsx
+++ b/changes/optics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB19B065-FC50-484E-988D-6B5343B6A793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C576A942-9024-4050-BE7C-8866608083D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="307">
   <si>
     <t>new</t>
   </si>
@@ -948,6 +948,12 @@
   </si>
   <si>
     <t>Trijicon SRO Reflex Sight</t>
+  </si>
+  <si>
+    <t>kac_aimpoint_micro_nvg_high_rise_picatinny_mount</t>
+  </si>
+  <si>
+    <t>Aimpoint Micro NVG High Rise</t>
   </si>
 </sst>
 </file>
@@ -1789,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S177"/>
+  <dimension ref="A1:S178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,7 +1941,7 @@
         <v>-0.4</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q69" si="1">P4*0.013+0.02</f>
+        <f t="shared" ref="Q4:Q70" si="1">P4*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
@@ -2423,7 +2429,7 @@
         <v>300</v>
       </c>
       <c r="N19" s="1">
-        <f t="shared" ref="N19:N52" si="4">C19-D19*20-E19*0.8-F19*0.6-H19*5+I19*10+J19/300</f>
+        <f t="shared" ref="N19:N53" si="4">C19-D19*20-E19*0.8-F19*0.6-H19*5+I19*10+J19/300</f>
         <v>-0.8</v>
       </c>
       <c r="Q19">
@@ -2493,23 +2499,23 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>305</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>306</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D23">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="M23">
-        <v>200</v>
+        <v>1300</v>
       </c>
       <c r="N23" s="1">
-        <f t="shared" ref="N23:N29" si="5">C23-D23*20-E23*0.8-F23*0.6-H23*5+I23*10+J23/300</f>
-        <v>-0.4</v>
+        <f t="shared" si="4"/>
+        <v>-4</v>
       </c>
       <c r="Q23">
         <f t="shared" si="1"/>
@@ -2518,10 +2524,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2533,34 +2539,34 @@
         <v>200</v>
       </c>
       <c r="N24" s="1">
+        <f t="shared" ref="N24:N30" si="5">C24-D24*20-E24*0.8-F24*0.6-H24*5+I24*10+J24/300</f>
+        <v>-0.4</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.02</v>
+      </c>
+      <c r="M25">
+        <v>200</v>
+      </c>
+      <c r="N25" s="1">
         <f t="shared" si="5"/>
         <v>-0.4</v>
       </c>
-      <c r="Q24">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0.03</v>
-      </c>
-      <c r="M25">
-        <v>300</v>
-      </c>
-      <c r="N25" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.6</v>
-      </c>
       <c r="Q25">
         <f t="shared" si="1"/>
         <v>0.02</v>
@@ -2568,10 +2574,10 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2580,7 +2586,7 @@
         <v>0.03</v>
       </c>
       <c r="M26">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N26" s="1">
         <f t="shared" si="5"/>
@@ -2593,23 +2599,23 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C27">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="M27">
         <v>200</v>
       </c>
       <c r="N27" s="1">
         <f t="shared" si="5"/>
-        <v>-1.8</v>
+        <v>-0.6</v>
       </c>
       <c r="Q27">
         <f t="shared" si="1"/>
@@ -2618,23 +2624,23 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="D28">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M28">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N28" s="1">
         <f t="shared" si="5"/>
-        <v>-1.5</v>
+        <v>-1.8</v>
       </c>
       <c r="Q28">
         <f t="shared" si="1"/>
@@ -2643,10 +2649,10 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C29">
         <v>-0.5</v>
@@ -2655,7 +2661,7 @@
         <v>0.05</v>
       </c>
       <c r="M29">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="N29" s="1">
         <f t="shared" si="5"/>
@@ -2668,63 +2674,63 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30">
+        <v>-0.5</v>
+      </c>
+      <c r="D30">
+        <v>0.05</v>
+      </c>
+      <c r="M30">
+        <v>400</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.5</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>-1</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>0.06</v>
       </c>
-      <c r="M30">
+      <c r="M31">
         <v>500</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N31" s="1">
         <f t="shared" si="4"/>
         <v>-2.2000000000000002</v>
       </c>
-      <c r="P30">
+      <c r="P31">
         <v>3.5</v>
       </c>
-      <c r="Q30">
+      <c r="Q31">
         <f t="shared" si="1"/>
         <v>6.5500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31">
-        <v>-1</v>
-      </c>
-      <c r="D31">
-        <v>0.04</v>
-      </c>
-      <c r="M31">
-        <v>500</v>
-      </c>
-      <c r="N31" s="1">
-        <f t="shared" si="4"/>
-        <v>-1.8</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -2733,7 +2739,7 @@
         <v>0.04</v>
       </c>
       <c r="M32">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="N32" s="1">
         <f t="shared" si="4"/>
@@ -2746,23 +2752,23 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C33">
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M33">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="N33" s="1">
         <f t="shared" si="4"/>
-        <v>-2</v>
+        <v>-1.8</v>
       </c>
       <c r="Q33">
         <f t="shared" si="1"/>
@@ -2771,23 +2777,23 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C34">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="M34">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="N34" s="1">
-        <f>C34-D34*20-E34*0.8-F34*0.6-H34*5+I34*10+J34/300</f>
-        <v>-1.1000000000000001</v>
+        <f t="shared" si="4"/>
+        <v>-2</v>
       </c>
       <c r="Q34">
         <f t="shared" si="1"/>
@@ -2796,23 +2802,23 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C35">
         <v>-0.5</v>
       </c>
       <c r="D35">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M35">
         <v>200</v>
       </c>
       <c r="N35" s="1">
         <f>C35-D35*20-E35*0.8-F35*0.6-H35*5+I35*10+J35/300</f>
-        <v>-0.9</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="Q35">
         <f t="shared" si="1"/>
@@ -2821,38 +2827,35 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C36">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D36">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
       <c r="M36">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="N36" s="1">
-        <f t="shared" si="4"/>
-        <v>-2.6</v>
+        <f>C36-D36*20-E36*0.8-F36*0.6-H36*5+I36*10+J36/300</f>
+        <v>-0.9</v>
       </c>
       <c r="Q36">
         <f t="shared" si="1"/>
         <v>0.02</v>
-      </c>
-      <c r="R36">
-        <v>369.99</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -2861,51 +2864,54 @@
         <v>0.08</v>
       </c>
       <c r="M37">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="N37" s="1">
         <f t="shared" si="4"/>
         <v>-2.6</v>
       </c>
-      <c r="P37">
-        <v>7.6</v>
-      </c>
       <c r="Q37">
         <f t="shared" si="1"/>
-        <v>0.11879999999999999</v>
+        <v>0.02</v>
+      </c>
+      <c r="R37">
+        <v>369.99</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C38">
         <v>-1</v>
       </c>
       <c r="D38">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="M38">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="N38" s="1">
         <f t="shared" si="4"/>
-        <v>-2.2000000000000002</v>
+        <v>-2.6</v>
+      </c>
+      <c r="P38">
+        <v>7.6</v>
       </c>
       <c r="Q38">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>0.11879999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -2914,137 +2920,137 @@
         <v>0.06</v>
       </c>
       <c r="M39">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="N39" s="1">
         <f t="shared" si="4"/>
         <v>-2.2000000000000002</v>
       </c>
-      <c r="P39">
-        <v>3</v>
-      </c>
       <c r="Q39">
         <f t="shared" si="1"/>
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="R39">
-        <v>896</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>284</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
+        <v>98</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40">
-        <v>5.0000000000000001E-3</v>
+        <v>0.06</v>
       </c>
       <c r="M40">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="N40" s="1">
         <f t="shared" si="4"/>
-        <v>-0.1</v>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="P40">
+        <v>3</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="1"/>
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="R40">
+        <v>896</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>284</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>285</v>
       </c>
       <c r="C41">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0.1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="M41">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="N41" s="1">
         <f t="shared" si="4"/>
-        <v>-2.5</v>
-      </c>
-      <c r="P41">
-        <v>5.2</v>
-      </c>
-      <c r="Q41">
-        <f t="shared" si="1"/>
-        <v>8.7599999999999997E-2</v>
-      </c>
-      <c r="R41">
-        <v>950</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C42">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D42">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="M42">
-        <v>700</v>
+        <v>1400</v>
       </c>
       <c r="N42" s="1">
         <f t="shared" si="4"/>
-        <v>-2.2000000000000002</v>
+        <v>-2.5</v>
+      </c>
+      <c r="P42">
+        <v>5.2</v>
       </c>
       <c r="Q42">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>8.7599999999999997E-2</v>
       </c>
       <c r="R42">
-        <v>125</v>
+        <v>950</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D43">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="M43">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="N43" s="1">
         <f t="shared" si="4"/>
-        <v>0.6</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="Q43">
         <f t="shared" si="1"/>
         <v>0.02</v>
+      </c>
+      <c r="R43">
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44">
         <v>0.02</v>
@@ -3054,7 +3060,7 @@
       </c>
       <c r="N44" s="1">
         <f t="shared" si="4"/>
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="Q44">
         <f t="shared" si="1"/>
@@ -3063,23 +3069,23 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
       <c r="N45" s="1">
         <f t="shared" si="4"/>
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="Q45">
         <f t="shared" si="1"/>
@@ -3088,10 +3094,10 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3112,9 +3118,24 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.01</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
       <c r="N47" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="Q47">
         <f t="shared" si="1"/>
@@ -3122,24 +3143,9 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0.03</v>
-      </c>
-      <c r="M48">
-        <v>500</v>
-      </c>
       <c r="N48" s="1">
         <f t="shared" si="4"/>
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="Q48">
         <f t="shared" si="1"/>
@@ -3148,23 +3154,23 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C49">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="M49">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="N49" s="1">
         <f t="shared" si="4"/>
-        <v>-1.3</v>
+        <v>-0.6</v>
       </c>
       <c r="Q49">
         <f t="shared" si="1"/>
@@ -3173,23 +3179,23 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C50">
         <v>-0.5</v>
       </c>
       <c r="D50">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="M50">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="N50" s="1">
         <f t="shared" si="4"/>
-        <v>-1.5</v>
+        <v>-1.3</v>
       </c>
       <c r="Q50">
         <f t="shared" si="1"/>
@@ -3198,197 +3204,197 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C51">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D51">
         <v>0.05</v>
       </c>
       <c r="M51">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="N51" s="1">
         <f t="shared" si="4"/>
-        <v>-2</v>
-      </c>
-      <c r="P51">
-        <v>2.1</v>
+        <v>-1.5</v>
       </c>
       <c r="Q51">
         <f t="shared" si="1"/>
-        <v>4.7300000000000002E-2</v>
-      </c>
-      <c r="R51">
-        <v>599</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52">
+        <v>-1</v>
+      </c>
+      <c r="D52">
+        <v>0.05</v>
+      </c>
+      <c r="M52">
+        <v>1200</v>
+      </c>
       <c r="N52" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-2</v>
+      </c>
+      <c r="P52">
+        <v>2.1</v>
       </c>
       <c r="Q52">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="R52">
+        <v>599</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>119</v>
-      </c>
-      <c r="B53" t="s">
-        <v>287</v>
-      </c>
-      <c r="C53">
-        <v>-2</v>
-      </c>
-      <c r="D53">
-        <v>0.18</v>
-      </c>
-      <c r="M53">
-        <v>1400</v>
-      </c>
       <c r="N53" s="1">
-        <f t="shared" ref="N53:N67" si="6">C53-D53*20-E53*0.8-F53*0.6-H53*5+I53*10+J53/300</f>
-        <v>-5.6</v>
-      </c>
-      <c r="P53">
-        <v>12.3</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="Q53">
         <f t="shared" si="1"/>
-        <v>0.1799</v>
-      </c>
-      <c r="R53">
-        <v>659</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B54" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C54">
         <v>-2</v>
       </c>
       <c r="D54">
+        <v>0.18</v>
+      </c>
+      <c r="M54">
+        <v>1400</v>
+      </c>
+      <c r="N54" s="1">
+        <f t="shared" ref="N54:N68" si="6">C54-D54*20-E54*0.8-F54*0.6-H54*5+I54*10+J54/300</f>
+        <v>-5.6</v>
+      </c>
+      <c r="P54">
+        <v>12.3</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="1"/>
+        <v>0.1799</v>
+      </c>
+      <c r="R54">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
+        <v>288</v>
+      </c>
+      <c r="C55">
+        <v>-2</v>
+      </c>
+      <c r="D55">
         <v>0.17</v>
       </c>
-      <c r="M54">
+      <c r="M55">
         <v>1300</v>
       </c>
-      <c r="N54" s="1">
+      <c r="N55" s="1">
         <f t="shared" si="6"/>
         <v>-5.4</v>
       </c>
-      <c r="P54">
+      <c r="P55">
         <v>11.5</v>
       </c>
-      <c r="Q54">
+      <c r="Q55">
         <f t="shared" si="1"/>
         <v>0.16949999999999998</v>
       </c>
-      <c r="R54">
+      <c r="R55">
         <v>601</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>121</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>289</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>-1</v>
       </c>
-      <c r="D55">
+      <c r="D56">
         <v>0.17</v>
       </c>
-      <c r="M55">
+      <c r="M56">
         <v>1100</v>
       </c>
-      <c r="N55" s="1">
+      <c r="N56" s="1">
         <f t="shared" si="6"/>
         <v>-4.4000000000000004</v>
       </c>
-      <c r="P55">
+      <c r="P56">
         <v>11.5</v>
       </c>
-      <c r="Q55">
+      <c r="Q56">
         <f t="shared" si="1"/>
         <v>0.16949999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>124</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>290</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>-2</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M56">
+      <c r="M57">
         <v>1800</v>
       </c>
-      <c r="N56" s="1">
+      <c r="N57" s="1">
         <f t="shared" si="6"/>
         <v>-4.8000000000000007</v>
       </c>
-      <c r="P56">
+      <c r="P57">
         <v>9</v>
       </c>
-      <c r="Q56">
+      <c r="Q57">
         <f t="shared" si="1"/>
         <v>0.13699999999999998</v>
       </c>
-      <c r="R56">
+      <c r="R57">
         <v>649</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" t="s">
-        <v>291</v>
-      </c>
-      <c r="C57">
-        <v>-1</v>
-      </c>
-      <c r="D57">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="M57">
-        <v>1600</v>
-      </c>
-      <c r="N57" s="1">
-        <f t="shared" si="6"/>
-        <v>-3.8000000000000003</v>
-      </c>
-      <c r="Q57">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -3397,7 +3403,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="M58">
-        <v>1700</v>
+        <v>1600</v>
       </c>
       <c r="N58" s="1">
         <f t="shared" si="6"/>
@@ -3410,10 +3416,10 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B59" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C59">
         <v>-1</v>
@@ -3422,7 +3428,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="M59">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="N59" s="1">
         <f t="shared" si="6"/>
@@ -3435,23 +3441,23 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D60">
-        <v>0.03</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M60">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="N60" s="1">
-        <f>C60-D60*20-E60*0.8-F60*0.6-H60*5+I60*10+J60/300</f>
-        <v>-0.6</v>
+        <f t="shared" si="6"/>
+        <v>-3.8000000000000003</v>
       </c>
       <c r="Q60">
         <f t="shared" si="1"/>
@@ -3460,10 +3466,10 @@
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B61" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3475,87 +3481,87 @@
         <v>300</v>
       </c>
       <c r="N61" s="1">
+        <f>C61-D61*20-E61*0.8-F61*0.6-H61*5+I61*10+J61/300</f>
+        <v>-0.6</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" t="s">
+        <v>295</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0.03</v>
+      </c>
+      <c r="M62">
+        <v>300</v>
+      </c>
+      <c r="N62" s="1">
         <f t="shared" si="6"/>
         <v>-0.6</v>
       </c>
-      <c r="Q61">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="Q62">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>122</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>296</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>-2</v>
       </c>
-      <c r="D62">
+      <c r="D63">
         <v>0.12</v>
       </c>
-      <c r="M62">
+      <c r="M63">
         <v>1700</v>
       </c>
-      <c r="N62" s="1">
+      <c r="N63" s="1">
         <f t="shared" si="6"/>
         <v>-4.4000000000000004</v>
       </c>
-      <c r="P62">
+      <c r="P63">
         <v>11.2</v>
       </c>
-      <c r="Q62">
+      <c r="Q63">
         <f t="shared" si="1"/>
         <v>0.16559999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>123</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>297</v>
       </c>
-      <c r="C63">
+      <c r="C64">
         <v>-1</v>
       </c>
-      <c r="D63">
+      <c r="D64">
         <v>0.12</v>
       </c>
-      <c r="M63">
+      <c r="M64">
         <v>1500</v>
       </c>
-      <c r="N63" s="1">
+      <c r="N64" s="1">
         <f t="shared" si="6"/>
         <v>-3.4</v>
       </c>
-      <c r="Q63">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" t="s">
-        <v>298</v>
-      </c>
-      <c r="C64">
-        <v>-1</v>
-      </c>
-      <c r="D64">
-        <v>0.12</v>
-      </c>
-      <c r="M64">
-        <v>1600</v>
-      </c>
-      <c r="N64" s="1">
-        <f>C64-D64*20-E64*0.8-F64*0.6-H64*5+I64*10+J64/300</f>
-        <v>-3.4</v>
-      </c>
       <c r="Q64">
         <f t="shared" si="1"/>
         <v>0.02</v>
@@ -3563,23 +3569,23 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="M65">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="N65" s="1">
         <f>C65-D65*20-E65*0.8-F65*0.6-H65*5+I65*10+J65/300</f>
-        <v>0</v>
+        <v>-3.4</v>
       </c>
       <c r="Q65">
         <f t="shared" si="1"/>
@@ -3588,10 +3594,10 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3603,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="N66" s="1">
-        <f t="shared" si="6"/>
+        <f>C66-D66*20-E66*0.8-F66*0.6-H66*5+I66*10+J66/300</f>
         <v>0</v>
       </c>
       <c r="Q66">
@@ -3613,10 +3619,10 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3638,32 +3644,47 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" t="s">
+        <v>301</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>134</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>302</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="M68">
-        <v>0</v>
-      </c>
-      <c r="N68" s="1">
-        <f>C68-D68*20-E68*0.8-F68*0.6-H68*5+I68*10+J68/300</f>
-        <v>0</v>
-      </c>
-      <c r="Q68">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
       <c r="N69" s="1">
-        <f t="shared" ref="N69:N98" si="7">C69-D69*20-E69*0.8-F69*0.6-H69*5+I69*10+J69/300</f>
+        <f>C69-D69*20-E69*0.8-F69*0.6-H69*5+I69*10+J69/300</f>
         <v>0</v>
       </c>
       <c r="Q69">
@@ -3672,61 +3693,43 @@
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>159</v>
-      </c>
-      <c r="B70" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-      <c r="D70">
-        <v>0.04</v>
-      </c>
-      <c r="M70">
-        <v>200</v>
-      </c>
       <c r="N70" s="1">
-        <f t="shared" ref="N70:N80" si="8">C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
-        <v>-0.8</v>
+        <f t="shared" ref="N70:N99" si="7">C70-D70*20-E70*0.8-F70*0.6-H70*5+I70*10+J70/300</f>
+        <v>0</v>
       </c>
       <c r="Q70">
-        <f t="shared" ref="Q70:Q80" si="9">P70*0.013+0.02</f>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C71">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="M71">
-        <v>900</v>
+        <v>200</v>
       </c>
       <c r="N71" s="1">
-        <f t="shared" si="8"/>
-        <v>-3.6</v>
-      </c>
-      <c r="P71">
-        <v>4.2</v>
+        <f t="shared" ref="N71:N81" si="8">C71-D71*20-E71*0.8-F71*0.6-H71*5+I71*10+J71/300</f>
+        <v>-0.8</v>
       </c>
       <c r="Q71">
-        <f t="shared" si="9"/>
-        <v>7.46E-2</v>
+        <f t="shared" ref="Q71:Q81" si="9">P71*0.013+0.02</f>
+        <v>0.02</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B72" t="s">
         <v>162</v>
@@ -3744,15 +3747,33 @@
         <f t="shared" si="8"/>
         <v>-3.6</v>
       </c>
+      <c r="P72">
+        <v>4.2</v>
+      </c>
       <c r="Q72">
         <f t="shared" si="9"/>
-        <v>0.02</v>
+        <v>7.46E-2</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73">
+        <v>-2</v>
+      </c>
+      <c r="D73">
+        <v>0.08</v>
+      </c>
+      <c r="M73">
+        <v>900</v>
+      </c>
       <c r="N73" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-3.6</v>
       </c>
       <c r="Q73">
         <f t="shared" si="9"/>
@@ -3760,24 +3781,9 @@
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>179</v>
-      </c>
-      <c r="B74" t="s">
-        <v>180</v>
-      </c>
-      <c r="C74">
-        <v>-0.5</v>
-      </c>
-      <c r="D74">
-        <v>0.03</v>
-      </c>
-      <c r="M74">
-        <v>200</v>
-      </c>
       <c r="N74" s="1">
         <f t="shared" si="8"/>
-        <v>-1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="Q74">
         <f t="shared" si="9"/>
@@ -3786,23 +3792,23 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B75" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C75">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="D75">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="M75">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N75" s="1">
         <f t="shared" si="8"/>
-        <v>-2.2000000000000002</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="Q75">
         <f t="shared" si="9"/>
@@ -3811,61 +3817,61 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B76" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C76">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="D76">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="M76">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="N76" s="1">
         <f t="shared" si="8"/>
-        <v>-4.2</v>
-      </c>
-      <c r="P76">
-        <v>7.1</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="Q76">
         <f t="shared" si="9"/>
-        <v>0.1123</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>181</v>
+      </c>
+      <c r="B77" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77">
+        <v>-2</v>
+      </c>
+      <c r="D77">
+        <v>0.11</v>
+      </c>
+      <c r="M77">
+        <v>800</v>
+      </c>
       <c r="N77" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-4.2</v>
+      </c>
+      <c r="P77">
+        <v>7.1</v>
       </c>
       <c r="Q77">
         <f t="shared" si="9"/>
-        <v>0.02</v>
+        <v>0.1123</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>183</v>
-      </c>
-      <c r="B78" t="s">
-        <v>184</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>0.05</v>
-      </c>
-      <c r="M78">
-        <v>300</v>
-      </c>
       <c r="N78" s="1">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="Q78">
         <f t="shared" si="9"/>
@@ -3874,250 +3880,247 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B79" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C79">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>0.17</v>
+        <v>0.05</v>
       </c>
       <c r="M79">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="N79" s="1">
         <f t="shared" si="8"/>
-        <v>-5.4</v>
-      </c>
-      <c r="P79">
-        <v>15.8</v>
+        <v>-1</v>
       </c>
       <c r="Q79">
         <f t="shared" si="9"/>
-        <v>0.22539999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80">
+        <v>-2</v>
+      </c>
+      <c r="D80">
+        <v>0.17</v>
+      </c>
+      <c r="M80">
+        <v>1000</v>
+      </c>
       <c r="N80" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-5.4</v>
+      </c>
+      <c r="P80">
+        <v>15.8</v>
       </c>
       <c r="Q80">
         <f t="shared" si="9"/>
-        <v>0.02</v>
+        <v>0.22539999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="N81" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q81">
+        <f t="shared" si="9"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>135</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>136</v>
       </c>
-      <c r="C81">
+      <c r="C82">
         <v>-2.5</v>
       </c>
-      <c r="D81">
+      <c r="D82">
         <v>0.06</v>
       </c>
-      <c r="M81">
+      <c r="M82">
         <v>900</v>
       </c>
-      <c r="N81" s="1">
+      <c r="N82" s="1">
         <f t="shared" si="7"/>
         <v>-3.7</v>
       </c>
-      <c r="P81">
+      <c r="P82">
         <v>3.1746569999999998</v>
       </c>
-      <c r="Q81">
-        <f t="shared" ref="Q81:Q104" si="10">P81*0.013+0.02</f>
+      <c r="Q82">
+        <f t="shared" ref="Q82:Q105" si="10">P82*0.013+0.02</f>
         <v>6.1270540999999998E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>137</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>138</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>-2</v>
       </c>
-      <c r="D82">
+      <c r="D83">
         <v>0.12</v>
       </c>
-      <c r="M82">
+      <c r="M83">
         <v>1000</v>
       </c>
-      <c r="N82" s="1">
+      <c r="N83" s="1">
         <f t="shared" si="7"/>
         <v>-4.4000000000000004</v>
       </c>
-      <c r="P82">
+      <c r="P83">
         <v>8</v>
       </c>
-      <c r="Q82">
+      <c r="Q83">
         <f t="shared" si="10"/>
         <v>0.124</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>139</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>140</v>
       </c>
-      <c r="C83">
+      <c r="C84">
         <v>-2.5</v>
       </c>
-      <c r="D83">
+      <c r="D84">
         <v>0.09</v>
       </c>
-      <c r="M83">
+      <c r="M84">
         <v>1000</v>
       </c>
-      <c r="N83" s="1">
+      <c r="N84" s="1">
         <f t="shared" si="7"/>
         <v>-4.3</v>
       </c>
-      <c r="P83">
+      <c r="P84">
         <v>5.6085599999999998</v>
       </c>
-      <c r="Q83">
+      <c r="Q84">
         <f t="shared" si="10"/>
         <v>9.2911279999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>143</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>144</v>
       </c>
-      <c r="C84">
+      <c r="C85">
         <v>-2</v>
       </c>
-      <c r="D84">
+      <c r="D85">
         <v>0.19</v>
       </c>
-      <c r="M84">
+      <c r="M85">
         <v>800</v>
       </c>
-      <c r="N84" s="1">
+      <c r="N85" s="1">
         <f t="shared" si="7"/>
         <v>-5.8</v>
       </c>
-      <c r="P84">
+      <c r="P85">
         <v>13.4041</v>
       </c>
-      <c r="Q84">
+      <c r="Q85">
         <f t="shared" si="10"/>
         <v>0.19425329999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>145</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>146</v>
       </c>
-      <c r="C85">
+      <c r="C86">
         <v>-6</v>
       </c>
-      <c r="D85">
+      <c r="D86">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H85">
+      <c r="H86">
         <v>0.25</v>
       </c>
-      <c r="M85">
+      <c r="M86">
         <v>600</v>
       </c>
-      <c r="N85" s="1">
+      <c r="N86" s="1">
         <f t="shared" si="7"/>
         <v>-8.65</v>
       </c>
-      <c r="P85">
+      <c r="P86">
         <v>4</v>
       </c>
-      <c r="Q85">
+      <c r="Q86">
         <f t="shared" si="10"/>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>147</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>148</v>
       </c>
-      <c r="C86">
+      <c r="C87">
         <v>-7</v>
       </c>
-      <c r="D86">
+      <c r="D87">
         <v>0.19</v>
       </c>
-      <c r="H86">
+      <c r="H87">
         <v>0.25</v>
       </c>
-      <c r="M86">
+      <c r="M87">
         <v>2000</v>
       </c>
-      <c r="N86" s="1">
+      <c r="N87" s="1">
         <f t="shared" si="7"/>
         <v>-12.05</v>
       </c>
-      <c r="P86">
+      <c r="P87">
         <v>9.6</v>
       </c>
-      <c r="Q86">
+      <c r="Q87">
         <f t="shared" si="10"/>
         <v>0.14479999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>157</v>
-      </c>
-      <c r="B87" t="s">
-        <v>158</v>
-      </c>
-      <c r="C87">
-        <v>-2</v>
-      </c>
-      <c r="D87">
-        <v>0.16</v>
-      </c>
-      <c r="M87">
-        <v>1000</v>
-      </c>
-      <c r="N87" s="1">
-        <f t="shared" si="7"/>
-        <v>-5.2</v>
-      </c>
-      <c r="P87">
-        <v>10.5116</v>
-      </c>
-      <c r="Q87">
-        <f t="shared" si="10"/>
-        <v>0.15665079999999998</v>
-      </c>
-    </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B88" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C88">
         <v>-2</v>
@@ -4126,26 +4129,26 @@
         <v>0.16</v>
       </c>
       <c r="M88">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="N88" s="1">
         <f t="shared" si="7"/>
         <v>-5.2</v>
       </c>
       <c r="P88">
-        <v>10.93493</v>
+        <v>10.5116</v>
       </c>
       <c r="Q88">
         <f t="shared" si="10"/>
-        <v>0.16215408999999997</v>
+        <v>0.15665079999999998</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B89" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C89">
         <v>-2</v>
@@ -4154,138 +4157,133 @@
         <v>0.16</v>
       </c>
       <c r="M89">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="N89" s="1">
         <f t="shared" si="7"/>
         <v>-5.2</v>
       </c>
       <c r="P89">
-        <v>10.9</v>
+        <v>10.93493</v>
       </c>
       <c r="Q89">
         <f t="shared" si="10"/>
-        <v>0.16169999999999998</v>
+        <v>0.16215408999999997</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B90" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C90">
-        <v>-2.5</v>
+        <v>-2</v>
       </c>
       <c r="D90">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="M90">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="N90" s="1">
         <f t="shared" si="7"/>
-        <v>-6.5</v>
+        <v>-5.2</v>
       </c>
       <c r="P90">
-        <v>13.9</v>
+        <v>10.9</v>
       </c>
       <c r="Q90">
         <f t="shared" si="10"/>
-        <v>0.20069999999999999</v>
+        <v>0.16169999999999998</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B91" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C91">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="D91">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="M91">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="N91" s="1">
         <f t="shared" si="7"/>
-        <v>-5.4</v>
+        <v>-6.5</v>
+      </c>
+      <c r="P91">
+        <v>13.9</v>
       </c>
       <c r="Q91">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>0.20069999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C92">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D92">
         <v>0.17</v>
       </c>
       <c r="M92">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="N92" s="1">
         <f t="shared" si="7"/>
-        <v>-7.4</v>
-      </c>
-      <c r="P92">
-        <v>11.6</v>
+        <v>-5.4</v>
       </c>
       <c r="Q92">
         <f t="shared" si="10"/>
-        <v>0.17079999999999998</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>155</v>
+      </c>
+      <c r="B93" t="s">
+        <v>156</v>
+      </c>
+      <c r="C93">
+        <v>-4</v>
+      </c>
+      <c r="D93">
+        <v>0.17</v>
+      </c>
+      <c r="M93">
+        <v>1600</v>
+      </c>
       <c r="N93" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-7.4</v>
+      </c>
+      <c r="P93">
+        <v>11.6</v>
       </c>
       <c r="Q93">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>0.17079999999999998</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C94" s="1">
-        <v>0</v>
-      </c>
-      <c r="D94" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="L94" s="1"/>
-      <c r="M94" s="1">
-        <v>400</v>
-      </c>
       <c r="N94" s="1">
         <f t="shared" si="7"/>
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="Q94">
         <f t="shared" si="10"/>
@@ -4294,16 +4292,16 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C95" s="1">
         <v>0</v>
       </c>
       <c r="D95" s="1">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
@@ -4314,11 +4312,11 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="N95" s="1">
         <f t="shared" si="7"/>
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="Q95">
         <f t="shared" si="10"/>
@@ -4326,24 +4324,32 @@
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>53</v>
-      </c>
-      <c r="B96" t="s">
-        <v>54</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="D96">
-        <v>0.03</v>
-      </c>
-      <c r="M96">
-        <v>350</v>
+      <c r="A96" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C96" s="1">
+        <v>0</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1">
+        <v>200</v>
       </c>
       <c r="N96" s="1">
         <f t="shared" si="7"/>
-        <v>-0.6</v>
+        <v>-0.4</v>
       </c>
       <c r="Q96">
         <f t="shared" si="10"/>
@@ -4352,10 +4358,10 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -4364,7 +4370,7 @@
         <v>0.03</v>
       </c>
       <c r="M97">
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="N97" s="1">
         <f t="shared" si="7"/>
@@ -4377,23 +4383,23 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B98" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="M98">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="N98" s="1">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>-0.6</v>
       </c>
       <c r="Q98">
         <f t="shared" si="10"/>
@@ -4402,35 +4408,32 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B99" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C99">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="M99">
-        <v>1200</v>
+        <v>100</v>
       </c>
       <c r="N99" s="1">
-        <f t="shared" ref="N99:N104" si="11">C99-D99*20-E99*0.8-F99*0.6-H99*5+I99*10+J99/300</f>
-        <v>-5</v>
-      </c>
-      <c r="P99">
-        <v>6.1</v>
+        <f t="shared" si="7"/>
+        <v>-1</v>
       </c>
       <c r="Q99">
         <f t="shared" si="10"/>
-        <v>9.9299999999999999E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B100" t="s">
         <v>58</v>
@@ -4445,17 +4448,20 @@
         <v>1200</v>
       </c>
       <c r="N100" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="N100:N105" si="11">C100-D100*20-E100*0.8-F100*0.6-H100*5+I100*10+J100/300</f>
         <v>-5</v>
+      </c>
+      <c r="P100">
+        <v>6.1</v>
       </c>
       <c r="Q100">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>9.9299999999999999E-2</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B101" t="s">
         <v>58</v>
@@ -4467,7 +4473,7 @@
         <v>0.1</v>
       </c>
       <c r="M101">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="N101" s="1">
         <f t="shared" si="11"/>
@@ -4480,7 +4486,7 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B102" t="s">
         <v>58</v>
@@ -4505,140 +4511,140 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B103" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C103">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="D103">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="M103">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="N103" s="1">
         <f t="shared" si="11"/>
-        <v>-2.6</v>
-      </c>
-      <c r="P103">
-        <v>5.5</v>
+        <v>-5</v>
       </c>
       <c r="Q103">
         <f t="shared" si="10"/>
-        <v>9.1499999999999998E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
+      <c r="A104" t="s">
+        <v>62</v>
+      </c>
+      <c r="B104" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104">
+        <v>-1</v>
+      </c>
+      <c r="D104">
+        <v>0.08</v>
+      </c>
+      <c r="M104">
+        <v>1300</v>
+      </c>
       <c r="N104" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-2.6</v>
+      </c>
+      <c r="P104">
+        <v>5.5</v>
       </c>
       <c r="Q104">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>9.1499999999999998E-2</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>187</v>
-      </c>
-      <c r="B105" t="s">
-        <v>188</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105">
-        <v>0.06</v>
-      </c>
-      <c r="M105">
-        <v>300</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
       <c r="N105" s="1">
-        <f>C105-D105*20-E105*0.8-F105*0.6-H105*5+I105*10+J105/300</f>
-        <v>-1.2</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="Q105">
-        <f>P105*0.013+0.02</f>
+        <f t="shared" si="10"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B106" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C106">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>0.19</v>
-      </c>
-      <c r="F106">
-        <v>-1</v>
+        <v>0.06</v>
       </c>
       <c r="M106">
-        <v>1200</v>
+        <v>300</v>
       </c>
       <c r="N106" s="1">
         <f>C106-D106*20-E106*0.8-F106*0.6-H106*5+I106*10+J106/300</f>
-        <v>-6.2</v>
-      </c>
-      <c r="P106">
-        <v>17.600000000000001</v>
+        <v>-1.2</v>
       </c>
       <c r="Q106">
         <f>P106*0.013+0.02</f>
-        <v>0.24879999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>189</v>
+      </c>
+      <c r="B107" t="s">
+        <v>190</v>
+      </c>
+      <c r="C107">
+        <v>-3</v>
+      </c>
+      <c r="D107">
+        <v>0.19</v>
+      </c>
+      <c r="F107">
+        <v>-1</v>
+      </c>
+      <c r="M107">
+        <v>1200</v>
+      </c>
       <c r="N107" s="1">
         <f>C107-D107*20-E107*0.8-F107*0.6-H107*5+I107*10+J107/300</f>
-        <v>0</v>
+        <v>-6.2</v>
+      </c>
+      <c r="P107">
+        <v>17.600000000000001</v>
       </c>
       <c r="Q107">
         <f>P107*0.013+0.02</f>
-        <v>0.02</v>
+        <v>0.24879999999999999</v>
       </c>
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>191</v>
-      </c>
-      <c r="B108" t="s">
-        <v>192</v>
-      </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
-      <c r="D108">
-        <v>0.06</v>
-      </c>
-      <c r="M108">
-        <v>300</v>
-      </c>
       <c r="N108" s="1">
         <f>C108-D108*20-E108*0.8-F108*0.6-H108*5+I108*10+J108/300</f>
-        <v>-1.2</v>
+        <v>0</v>
       </c>
       <c r="Q108">
         <f>P108*0.013+0.02</f>
@@ -4647,127 +4653,127 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B109" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C109">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>0.25</v>
-      </c>
-      <c r="F109">
-        <v>-2</v>
+        <v>0.06</v>
       </c>
       <c r="M109">
-        <v>950</v>
+        <v>300</v>
       </c>
       <c r="N109" s="1">
         <f>C109-D109*20-E109*0.8-F109*0.6-H109*5+I109*10+J109/300</f>
-        <v>-6.8</v>
-      </c>
-      <c r="P109">
-        <v>17.460599999999999</v>
+        <v>-1.2</v>
       </c>
       <c r="Q109">
         <f>P109*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>193</v>
+      </c>
+      <c r="B110" t="s">
+        <v>194</v>
+      </c>
+      <c r="C110">
+        <v>-3</v>
+      </c>
+      <c r="D110">
+        <v>0.25</v>
+      </c>
+      <c r="F110">
+        <v>-2</v>
+      </c>
+      <c r="M110">
+        <v>950</v>
+      </c>
+      <c r="N110" s="1">
+        <f>C110-D110*20-E110*0.8-F110*0.6-H110*5+I110*10+J110/300</f>
+        <v>-6.8</v>
+      </c>
+      <c r="P110">
+        <v>17.460599999999999</v>
+      </c>
+      <c r="Q110">
+        <f>P110*0.013+0.02</f>
         <v>0.24698779999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N110" s="1">
-        <f t="shared" ref="N110:N147" si="12">C110-D110*20-E110*0.8-F110*0.6-H110*5+I110*10+J110/300</f>
-        <v>0</v>
-      </c>
-      <c r="Q110">
-        <f t="shared" ref="Q110:Q164" si="13">P110*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="N111" s="1">
+        <f t="shared" ref="N111:N148" si="12">C111-D111*20-E111*0.8-F111*0.6-H111*5+I111*10+J111/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q111">
+        <f t="shared" ref="Q111:Q165" si="13">P111*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>195</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>196</v>
       </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-      <c r="D111">
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
         <v>0.06</v>
       </c>
-      <c r="M111">
+      <c r="M112">
         <v>400</v>
       </c>
-      <c r="N111" s="1">
+      <c r="N112" s="1">
         <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
-      <c r="Q111">
+      <c r="Q112">
         <f t="shared" si="13"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>197</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>198</v>
       </c>
-      <c r="C112">
+      <c r="C113">
         <v>-3</v>
       </c>
-      <c r="D112">
+      <c r="D113">
         <v>0.16</v>
       </c>
-      <c r="M112">
+      <c r="M113">
         <v>750</v>
       </c>
-      <c r="N112" s="1">
+      <c r="N113" s="1">
         <f t="shared" si="12"/>
         <v>-6.2</v>
       </c>
-      <c r="P112">
+      <c r="P113">
         <v>10.5822</v>
       </c>
-      <c r="Q112">
+      <c r="Q113">
         <f t="shared" si="13"/>
         <v>0.15756859999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N113" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Q113">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>199</v>
-      </c>
-      <c r="B114" t="s">
-        <v>200</v>
-      </c>
-      <c r="C114">
-        <v>0</v>
-      </c>
-      <c r="D114">
-        <v>0.06</v>
-      </c>
-      <c r="M114">
-        <v>400</v>
-      </c>
       <c r="N114" s="1">
         <f t="shared" si="12"/>
-        <v>-1.2</v>
+        <v>0</v>
       </c>
       <c r="Q114">
         <f t="shared" si="13"/>
@@ -4776,61 +4782,76 @@
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B115" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C115">
-        <v>-3.5</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>0.14000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="M115">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="N115" s="1">
         <f t="shared" si="12"/>
-        <v>-6.3000000000000007</v>
-      </c>
-      <c r="P115">
-        <v>9.5239700000000003</v>
+        <v>-1.2</v>
       </c>
       <c r="Q115">
         <f t="shared" si="13"/>
-        <v>0.14381161000000001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B116" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C116">
-        <v>-3</v>
+        <v>-3.5</v>
       </c>
       <c r="D116">
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M116">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="N116" s="1">
         <f t="shared" si="12"/>
-        <v>-6.2</v>
+        <v>-6.3000000000000007</v>
+      </c>
+      <c r="P116">
+        <v>9.5239700000000003</v>
       </c>
       <c r="Q116">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.14381161000000001</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>203</v>
+      </c>
+      <c r="B117" t="s">
+        <v>204</v>
+      </c>
+      <c r="C117">
+        <v>-3</v>
+      </c>
+      <c r="D117">
+        <v>0.16</v>
+      </c>
+      <c r="M117">
+        <v>800</v>
+      </c>
       <c r="N117" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-6.2</v>
       </c>
       <c r="Q117">
         <f t="shared" si="13"/>
@@ -4838,42 +4859,21 @@
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>207</v>
-      </c>
-      <c r="B118" t="s">
-        <v>208</v>
-      </c>
-      <c r="C118">
-        <v>0</v>
-      </c>
-      <c r="D118">
-        <v>0.06</v>
-      </c>
-      <c r="M118">
-        <v>400</v>
-      </c>
       <c r="N118" s="1">
         <f t="shared" si="12"/>
-        <v>-1.2</v>
-      </c>
-      <c r="P118">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q118">
         <f t="shared" si="13"/>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="S118" t="s">
-        <v>276</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B119" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -4888,45 +4888,45 @@
         <f t="shared" si="12"/>
         <v>-1.2</v>
       </c>
+      <c r="P119">
+        <v>4</v>
+      </c>
       <c r="Q119">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="S119" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B120" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C120">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>0.18</v>
-      </c>
-      <c r="F120">
-        <v>-1</v>
+        <v>0.06</v>
       </c>
       <c r="M120">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="N120" s="1">
         <f t="shared" si="12"/>
-        <v>-6</v>
-      </c>
-      <c r="P120">
-        <v>16.600000000000001</v>
+        <v>-1.2</v>
       </c>
       <c r="Q120">
         <f t="shared" si="13"/>
-        <v>0.23580000000000001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
       <c r="B121" t="s">
         <v>210</v>
@@ -4947,45 +4947,45 @@
         <f t="shared" si="12"/>
         <v>-6</v>
       </c>
+      <c r="P121">
+        <v>16.600000000000001</v>
+      </c>
       <c r="Q121">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.23580000000000001</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
       <c r="B122" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C122">
         <v>-3</v>
       </c>
       <c r="D122">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="F122">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M122">
-        <v>1900</v>
+        <v>1000</v>
       </c>
       <c r="N122" s="1">
         <f t="shared" si="12"/>
-        <v>-5.8</v>
-      </c>
-      <c r="P122">
-        <v>14</v>
+        <v>-6</v>
       </c>
       <c r="Q122">
         <f t="shared" si="13"/>
-        <v>0.20199999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="B123" t="s">
         <v>212</v>
@@ -5006,45 +5006,45 @@
         <f t="shared" si="12"/>
         <v>-5.8</v>
       </c>
+      <c r="P123">
+        <v>14</v>
+      </c>
       <c r="Q123">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.20199999999999999</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B124" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="C124">
         <v>-3</v>
       </c>
       <c r="D124">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="F124">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M124">
-        <v>1500</v>
+        <v>1900</v>
       </c>
       <c r="N124" s="1">
         <f t="shared" si="12"/>
-        <v>-5.6000000000000005</v>
-      </c>
-      <c r="P124">
-        <v>10.9</v>
+        <v>-5.8</v>
       </c>
       <c r="Q124">
         <f t="shared" si="13"/>
-        <v>0.16169999999999998</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B125" t="s">
         <v>262</v>
@@ -5065,17 +5065,20 @@
         <f t="shared" si="12"/>
         <v>-5.6000000000000005</v>
       </c>
+      <c r="P125">
+        <v>10.9</v>
+      </c>
       <c r="Q125">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.16169999999999998</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B126" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C126">
         <v>-3</v>
@@ -5087,23 +5090,20 @@
         <v>-1</v>
       </c>
       <c r="M126">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="N126" s="1">
         <f t="shared" si="12"/>
         <v>-5.6000000000000005</v>
       </c>
-      <c r="P126">
-        <v>10.5</v>
-      </c>
       <c r="Q126">
         <f t="shared" si="13"/>
-        <v>0.15649999999999997</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B127" t="s">
         <v>268</v>
@@ -5124,17 +5124,20 @@
         <f t="shared" si="12"/>
         <v>-5.6000000000000005</v>
       </c>
+      <c r="P127">
+        <v>10.5</v>
+      </c>
       <c r="Q127">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.15649999999999997</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B128" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C128">
         <v>-3</v>
@@ -5146,7 +5149,7 @@
         <v>-1</v>
       </c>
       <c r="M128">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="N128" s="1">
         <f t="shared" si="12"/>
@@ -5159,7 +5162,7 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B129" t="s">
         <v>269</v>
@@ -5186,9 +5189,27 @@
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>267</v>
+      </c>
+      <c r="B130" t="s">
+        <v>269</v>
+      </c>
+      <c r="C130">
+        <v>-3</v>
+      </c>
+      <c r="D130">
+        <v>0.16</v>
+      </c>
+      <c r="F130">
+        <v>-1</v>
+      </c>
+      <c r="M130">
+        <v>1600</v>
+      </c>
       <c r="N130" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-5.6000000000000005</v>
       </c>
       <c r="Q130">
         <f t="shared" si="13"/>
@@ -5196,21 +5217,9 @@
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>270</v>
-      </c>
-      <c r="B131" t="s">
-        <v>271</v>
-      </c>
-      <c r="D131">
-        <v>0.04</v>
-      </c>
-      <c r="M131">
-        <v>100</v>
-      </c>
       <c r="N131" s="1">
         <f t="shared" si="12"/>
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="Q131">
         <f t="shared" si="13"/>
@@ -5219,41 +5228,32 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B132" t="s">
-        <v>272</v>
-      </c>
-      <c r="C132">
-        <v>-3</v>
+        <v>271</v>
       </c>
       <c r="D132">
-        <v>0.2</v>
-      </c>
-      <c r="F132">
-        <v>-1</v>
+        <v>0.04</v>
       </c>
       <c r="M132">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="N132" s="1">
         <f t="shared" si="12"/>
-        <v>-6.4</v>
-      </c>
-      <c r="P132">
-        <v>16.54</v>
+        <v>-0.8</v>
       </c>
       <c r="Q132">
         <f t="shared" si="13"/>
-        <v>0.23501999999999998</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B133" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C133">
         <v>-3</v>
@@ -5265,21 +5265,42 @@
         <v>-1</v>
       </c>
       <c r="M133">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="N133" s="1">
         <f t="shared" si="12"/>
         <v>-6.4</v>
       </c>
+      <c r="P133">
+        <v>16.54</v>
+      </c>
       <c r="Q133">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.23501999999999998</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>275</v>
+      </c>
+      <c r="B134" t="s">
+        <v>273</v>
+      </c>
+      <c r="C134">
+        <v>-3</v>
+      </c>
+      <c r="D134">
+        <v>0.2</v>
+      </c>
+      <c r="F134">
+        <v>-1</v>
+      </c>
+      <c r="M134">
+        <v>1200</v>
+      </c>
       <c r="N134" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-6.4</v>
       </c>
       <c r="Q134">
         <f t="shared" si="13"/>
@@ -5287,77 +5308,62 @@
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>213</v>
-      </c>
-      <c r="B135" t="s">
-        <v>214</v>
-      </c>
-      <c r="C135">
-        <v>-0.5</v>
-      </c>
-      <c r="D135">
-        <v>0.06</v>
-      </c>
-      <c r="M135">
-        <v>1000</v>
-      </c>
       <c r="N135" s="1">
         <f t="shared" si="12"/>
-        <v>-1.7</v>
-      </c>
-      <c r="P135">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="Q135">
         <f t="shared" si="13"/>
-        <v>0.1045</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B136" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="D136">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="M136">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N136" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>-1.7</v>
+      </c>
+      <c r="P136">
+        <v>6.5</v>
       </c>
       <c r="Q136">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.1045</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B137" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C137">
         <v>0</v>
       </c>
       <c r="D137">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="M137">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="N137" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>-0.2</v>
       </c>
       <c r="Q137">
         <f t="shared" si="13"/>
@@ -5366,23 +5372,23 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B138" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C138">
         <v>0</v>
       </c>
       <c r="D138">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="M138">
         <v>200</v>
       </c>
       <c r="N138" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
       <c r="Q138">
         <f t="shared" si="13"/>
@@ -5391,23 +5397,23 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B139" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C139">
         <v>0</v>
       </c>
       <c r="D139">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="M139">
         <v>200</v>
       </c>
       <c r="N139" s="1">
         <f t="shared" si="12"/>
-        <v>-0.6</v>
+        <v>-0.4</v>
       </c>
       <c r="Q139">
         <f t="shared" si="13"/>
@@ -5416,23 +5422,23 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B140" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C140">
         <v>0</v>
       </c>
       <c r="D140">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="M140">
         <v>200</v>
       </c>
       <c r="N140" s="1">
         <f t="shared" si="12"/>
-        <v>-0.2</v>
+        <v>-0.6</v>
       </c>
       <c r="Q140">
         <f t="shared" si="13"/>
@@ -5441,23 +5447,23 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B141" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C141">
         <v>0</v>
       </c>
       <c r="D141">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="M141">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="N141" s="1">
         <f t="shared" si="12"/>
-        <v>-0.4</v>
+        <v>-0.2</v>
       </c>
       <c r="Q141">
         <f t="shared" si="13"/>
@@ -5466,10 +5472,10 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B142" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -5491,227 +5497,227 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="B143" t="s">
-        <v>216</v>
+        <v>248</v>
       </c>
       <c r="C143">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D143">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="M143">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="N143" s="1">
         <f t="shared" si="12"/>
-        <v>-3.2</v>
-      </c>
-      <c r="P143">
-        <v>8.6999999999999993</v>
+        <v>-0.4</v>
       </c>
       <c r="Q143">
         <f t="shared" si="13"/>
-        <v>0.1331</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B144" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C144">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="D144">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="M144">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="N144" s="1">
         <f t="shared" si="12"/>
-        <v>-3.5</v>
+        <v>-3.2</v>
       </c>
       <c r="P144">
-        <v>7.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Q144">
         <f t="shared" si="13"/>
-        <v>0.11749999999999999</v>
+        <v>0.1331</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B145" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C145">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="D145">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="M145">
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="N145" s="1">
         <f t="shared" si="12"/>
-        <v>-2.8</v>
+        <v>-3.5</v>
       </c>
       <c r="P145">
-        <v>6.7</v>
+        <v>7.5</v>
       </c>
       <c r="Q145">
         <f t="shared" si="13"/>
-        <v>0.1071</v>
+        <v>0.11749999999999999</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B146" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C146">
         <v>-1</v>
       </c>
       <c r="D146">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="M146">
         <v>500</v>
       </c>
       <c r="N146" s="1">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-2.8</v>
+      </c>
+      <c r="P146">
+        <v>6.7</v>
       </c>
       <c r="Q146">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.1071</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B147" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C147">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="D147">
-        <v>0.27</v>
-      </c>
-      <c r="F147">
-        <v>-2</v>
+        <v>0.1</v>
       </c>
       <c r="M147">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="N147" s="1">
         <f t="shared" si="12"/>
-        <v>-9.2000000000000011</v>
-      </c>
-      <c r="P147">
-        <v>20.100000000000001</v>
+        <v>-3</v>
       </c>
       <c r="Q147">
         <f t="shared" si="13"/>
-        <v>0.28130000000000005</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>223</v>
+      </c>
+      <c r="B148" t="s">
+        <v>224</v>
+      </c>
+      <c r="C148">
+        <v>-5</v>
+      </c>
+      <c r="D148">
+        <v>0.27</v>
+      </c>
+      <c r="F148">
+        <v>-2</v>
+      </c>
+      <c r="M148">
+        <v>4000</v>
+      </c>
       <c r="N148" s="1">
-        <f t="shared" ref="N148:N165" si="14">C148-D148*20-E148*0.8-F148*0.6-H148*5+I148*10+J148/300</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-9.2000000000000011</v>
+      </c>
+      <c r="P148">
+        <v>20.100000000000001</v>
       </c>
       <c r="Q148">
         <f t="shared" si="13"/>
-        <v>0.02</v>
+        <v>0.28130000000000005</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="N149" s="1">
+        <f t="shared" ref="N149:N166" si="14">C149-D149*20-E149*0.8-F149*0.6-H149*5+I149*10+J149/300</f>
+        <v>0</v>
+      </c>
+      <c r="Q149">
+        <f t="shared" si="13"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>227</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>228</v>
       </c>
-      <c r="C149">
+      <c r="C150">
         <v>-0.5</v>
       </c>
-      <c r="D149">
+      <c r="D150">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M149">
+      <c r="M150">
         <v>1000</v>
       </c>
-      <c r="N149" s="1">
+      <c r="N150" s="1">
         <f t="shared" si="14"/>
         <v>-1.9000000000000001</v>
       </c>
-      <c r="P149">
+      <c r="P150">
         <v>6.6</v>
       </c>
-      <c r="Q149">
+      <c r="Q150">
         <f t="shared" si="13"/>
         <v>0.10579999999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>233</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>234</v>
       </c>
-      <c r="C150">
-        <v>0</v>
-      </c>
-      <c r="D150">
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
         <v>0.01</v>
       </c>
-      <c r="M150">
-        <v>0</v>
-      </c>
-      <c r="N150" s="1">
+      <c r="M151">
+        <v>0</v>
+      </c>
+      <c r="N151" s="1">
         <f t="shared" si="14"/>
         <v>-0.2</v>
       </c>
-      <c r="Q150">
-        <f>P150*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>235</v>
-      </c>
-      <c r="B151" t="s">
-        <v>236</v>
-      </c>
-      <c r="C151">
-        <v>0</v>
-      </c>
-      <c r="D151">
-        <v>0.03</v>
-      </c>
-      <c r="M151">
-        <v>200</v>
-      </c>
-      <c r="N151" s="1">
-        <f t="shared" si="14"/>
-        <v>-0.6</v>
-      </c>
       <c r="Q151">
         <f>P151*0.013+0.02</f>
         <v>0.02</v>
@@ -5719,7 +5725,7 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B152" t="s">
         <v>236</v>
@@ -5744,132 +5750,129 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B153" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C153">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D153">
-        <v>0.11</v>
+        <v>0.03</v>
       </c>
       <c r="M153">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="N153" s="1">
         <f t="shared" si="14"/>
+        <v>-0.6</v>
+      </c>
+      <c r="Q153">
+        <f>P153*0.013+0.02</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>229</v>
+      </c>
+      <c r="B154" t="s">
+        <v>230</v>
+      </c>
+      <c r="C154">
+        <v>-1</v>
+      </c>
+      <c r="D154">
+        <v>0.11</v>
+      </c>
+      <c r="M154">
+        <v>500</v>
+      </c>
+      <c r="N154" s="1">
+        <f t="shared" si="14"/>
         <v>-3.2</v>
       </c>
-      <c r="P153">
+      <c r="P154">
         <v>7.0195183999999999</v>
       </c>
-      <c r="Q153">
+      <c r="Q154">
         <f t="shared" si="13"/>
         <v>0.11125373919999999</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>225</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B155" t="s">
         <v>226</v>
       </c>
-      <c r="C154">
+      <c r="C155">
         <v>-7</v>
       </c>
-      <c r="D154">
+      <c r="D155">
         <v>0.42</v>
       </c>
-      <c r="F154">
+      <c r="F155">
         <v>-4</v>
       </c>
-      <c r="M154">
+      <c r="M155">
         <v>5000</v>
       </c>
-      <c r="N154" s="1">
+      <c r="N155" s="1">
         <f t="shared" si="14"/>
         <v>-13</v>
       </c>
-      <c r="P154">
+      <c r="P155">
         <v>39.299999999999997</v>
       </c>
-      <c r="Q154">
+      <c r="Q155">
         <f t="shared" si="13"/>
         <v>0.53089999999999993</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N155" s="1"/>
-    </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="N156" s="1"/>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>278</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B157" t="s">
         <v>279</v>
       </c>
-      <c r="C156">
-        <v>0</v>
-      </c>
-      <c r="D156">
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
         <v>0.05</v>
       </c>
-      <c r="M156">
+      <c r="M157">
         <v>400</v>
       </c>
-      <c r="N156" s="1">
+      <c r="N157" s="1">
         <f t="shared" si="14"/>
         <v>-1</v>
       </c>
-      <c r="Q156">
-        <f t="shared" si="13"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C157" s="1">
-        <v>-2</v>
-      </c>
-      <c r="D157" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
-      <c r="H157" s="1"/>
-      <c r="I157" s="1"/>
-      <c r="J157" s="1"/>
-      <c r="K157" s="1"/>
-      <c r="L157" s="1"/>
-      <c r="M157" s="1">
-        <v>1000</v>
-      </c>
-      <c r="N157" s="1">
-        <f t="shared" si="14"/>
-        <v>-5.2</v>
-      </c>
-      <c r="P157">
-        <v>15</v>
-      </c>
       <c r="Q157">
         <f t="shared" si="13"/>
-        <v>0.21499999999999997</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C158" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0.16</v>
+      </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
@@ -5878,233 +5881,239 @@
       <c r="J158" s="1"/>
       <c r="K158" s="1"/>
       <c r="L158" s="1"/>
-      <c r="M158" s="1"/>
-      <c r="N158" s="1"/>
+      <c r="M158" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N158" s="1">
+        <f t="shared" si="14"/>
+        <v>-5.2</v>
+      </c>
+      <c r="P158">
+        <v>15</v>
+      </c>
+      <c r="Q158">
+        <f t="shared" si="13"/>
+        <v>0.21499999999999997</v>
+      </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>164</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B160" t="s">
         <v>165</v>
       </c>
-      <c r="C159">
+      <c r="C160">
         <v>-2.5</v>
       </c>
-      <c r="D159">
+      <c r="D160">
         <v>0.22</v>
       </c>
-      <c r="F159">
+      <c r="F160">
         <v>-1</v>
       </c>
-      <c r="M159">
+      <c r="M160">
         <v>1000</v>
       </c>
-      <c r="N159" s="1">
+      <c r="N160" s="1">
         <f t="shared" si="14"/>
         <v>-6.3000000000000007</v>
       </c>
-      <c r="P159">
+      <c r="P160">
         <v>15.4</v>
       </c>
-      <c r="Q159">
+      <c r="Q160">
         <f t="shared" si="13"/>
         <v>0.22019999999999998</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>166</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B161" t="s">
         <v>167</v>
       </c>
-      <c r="C160">
+      <c r="C161">
         <v>-5</v>
       </c>
-      <c r="D160">
+      <c r="D161">
         <v>0.26</v>
       </c>
-      <c r="F160">
+      <c r="F161">
         <v>-2</v>
       </c>
-      <c r="M160">
+      <c r="M161">
         <v>2000</v>
       </c>
-      <c r="N160" s="1">
+      <c r="N161" s="1">
         <f t="shared" si="14"/>
         <v>-9</v>
       </c>
-      <c r="P160">
+      <c r="P161">
         <v>17.3</v>
       </c>
-      <c r="Q160">
+      <c r="Q161">
         <f t="shared" si="13"/>
         <v>0.24489999999999998</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>169</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B162" t="s">
         <v>170</v>
       </c>
-      <c r="C161">
+      <c r="C162">
         <v>-3</v>
       </c>
-      <c r="D161">
+      <c r="D162">
         <v>0.33</v>
       </c>
-      <c r="F161">
+      <c r="F162">
         <v>-3</v>
       </c>
-      <c r="M161">
+      <c r="M162">
         <v>3000</v>
       </c>
-      <c r="N161" s="1">
+      <c r="N162" s="1">
         <f t="shared" si="14"/>
         <v>-7.8000000000000016</v>
       </c>
-      <c r="P161">
+      <c r="P162">
         <v>24.162700000000001</v>
       </c>
-      <c r="Q161">
+      <c r="Q162">
         <f t="shared" si="13"/>
         <v>0.3341151</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>171</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" t="s">
         <v>172</v>
       </c>
-      <c r="C162">
+      <c r="C163">
         <v>-3</v>
       </c>
-      <c r="D162">
+      <c r="D163">
         <v>0.24</v>
       </c>
-      <c r="F162">
+      <c r="F163">
         <v>-2</v>
       </c>
-      <c r="M162">
+      <c r="M163">
         <v>3000</v>
       </c>
-      <c r="N162" s="1">
+      <c r="N163" s="1">
         <f t="shared" si="14"/>
         <v>-6.6</v>
       </c>
-      <c r="P162">
+      <c r="P163">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q162">
+      <c r="Q163">
         <f t="shared" si="13"/>
         <v>0.24619999999999997</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>173</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B164" t="s">
         <v>174</v>
       </c>
-      <c r="C163">
+      <c r="C164">
         <v>-3</v>
       </c>
-      <c r="D163">
+      <c r="D164">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F163">
+      <c r="F164">
         <v>-1</v>
       </c>
-      <c r="M163">
+      <c r="M164">
         <v>4000</v>
       </c>
-      <c r="N163" s="1">
+      <c r="N164" s="1">
         <f t="shared" si="14"/>
         <v>-8.0000000000000018</v>
       </c>
-      <c r="P163">
+      <c r="P164">
         <v>21.9</v>
       </c>
-      <c r="Q163">
+      <c r="Q164">
         <f t="shared" si="13"/>
         <v>0.30469999999999997</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>175</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B165" t="s">
         <v>176</v>
       </c>
-      <c r="C164">
+      <c r="C165">
         <v>-3</v>
       </c>
-      <c r="D164">
+      <c r="D165">
         <v>0.27</v>
       </c>
-      <c r="F164">
+      <c r="F165">
         <v>-2</v>
       </c>
-      <c r="M164">
+      <c r="M165">
         <v>2000</v>
       </c>
-      <c r="N164" s="1">
+      <c r="N165" s="1">
         <f t="shared" si="14"/>
         <v>-7.2</v>
       </c>
-      <c r="P164">
+      <c r="P165">
         <v>19.3</v>
       </c>
-      <c r="Q164">
+      <c r="Q165">
         <f t="shared" si="13"/>
         <v>0.27090000000000003</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N165" s="1">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N166" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="Q165">
-        <f>P165*0.013+0.02</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>253</v>
-      </c>
-      <c r="B166" t="s">
-        <v>254</v>
-      </c>
-      <c r="C166">
-        <v>-2</v>
-      </c>
-      <c r="D166">
-        <v>0.05</v>
-      </c>
-      <c r="M166">
-        <v>300</v>
-      </c>
-      <c r="N166" s="1"/>
       <c r="Q166">
-        <f t="shared" ref="Q166:Q177" si="15">P166*0.013+0.02</f>
+        <f>P166*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B167" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C167">
         <v>-2</v>
@@ -6117,86 +6126,83 @@
       </c>
       <c r="N167" s="1"/>
       <c r="Q167">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="Q167:Q178" si="15">P167*0.013+0.02</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B168" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C168">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="D168">
-        <v>0.17</v>
+        <v>0.05</v>
       </c>
       <c r="M168">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="N168" s="1"/>
-      <c r="P168">
-        <v>13.3</v>
-      </c>
       <c r="Q168">
-        <f>P168*0.013+0.02</f>
-        <v>0.19289999999999999</v>
+        <f t="shared" si="15"/>
+        <v>0.02</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B169" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C169">
         <v>-3</v>
       </c>
       <c r="D169">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="M169">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="N169" s="1"/>
       <c r="P169">
-        <v>13.28</v>
+        <v>13.3</v>
       </c>
       <c r="Q169">
         <f>P169*0.013+0.02</f>
+        <v>0.19289999999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>251</v>
+      </c>
+      <c r="B170" t="s">
+        <v>252</v>
+      </c>
+      <c r="C170">
+        <v>-3</v>
+      </c>
+      <c r="D170">
+        <v>0.18</v>
+      </c>
+      <c r="M170">
+        <v>1000</v>
+      </c>
+      <c r="N170" s="1"/>
+      <c r="P170">
+        <v>13.28</v>
+      </c>
+      <c r="Q170">
+        <f>P170*0.013+0.02</f>
         <v>0.19263999999999998</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N170" s="1"/>
-      <c r="Q170">
-        <f t="shared" si="15"/>
-        <v>0.02</v>
-      </c>
-    </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>259</v>
-      </c>
-      <c r="B171" t="s">
-        <v>260</v>
-      </c>
-      <c r="C171">
-        <v>-8</v>
-      </c>
-      <c r="D171">
-        <v>0.36</v>
-      </c>
-      <c r="F171">
-        <v>-3</v>
-      </c>
-      <c r="M171">
-        <v>3000</v>
-      </c>
       <c r="N171" s="1"/>
       <c r="Q171">
         <f t="shared" si="15"/>
@@ -6204,6 +6210,24 @@
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>259</v>
+      </c>
+      <c r="B172" t="s">
+        <v>260</v>
+      </c>
+      <c r="C172">
+        <v>-8</v>
+      </c>
+      <c r="D172">
+        <v>0.36</v>
+      </c>
+      <c r="F172">
+        <v>-3</v>
+      </c>
+      <c r="M172">
+        <v>3000</v>
+      </c>
       <c r="N172" s="1"/>
       <c r="Q172">
         <f t="shared" si="15"/>
@@ -6211,53 +6235,53 @@
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>280</v>
-      </c>
-      <c r="B173" t="s">
-        <v>281</v>
-      </c>
-      <c r="C173">
-        <v>1</v>
-      </c>
-      <c r="D173">
-        <v>0.13</v>
-      </c>
-      <c r="M173">
-        <v>1000</v>
-      </c>
       <c r="N173" s="1"/>
-      <c r="P173">
-        <v>12.1</v>
-      </c>
       <c r="Q173">
         <f t="shared" si="15"/>
-        <v>0.17729999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B174" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C174">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="D174">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
       <c r="M174">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="N174" s="1"/>
+      <c r="P174">
+        <v>12.1</v>
+      </c>
       <c r="Q174">
         <f t="shared" si="15"/>
-        <v>0.02</v>
+        <v>0.17729999999999999</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>282</v>
+      </c>
+      <c r="B175" t="s">
+        <v>283</v>
+      </c>
+      <c r="C175">
+        <v>-3</v>
+      </c>
+      <c r="D175">
+        <v>0.06</v>
+      </c>
+      <c r="M175">
+        <v>700</v>
+      </c>
       <c r="N175" s="1"/>
       <c r="Q175">
         <f t="shared" si="15"/>
@@ -6265,6 +6289,7 @@
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N176" s="1"/>
       <c r="Q176">
         <f t="shared" si="15"/>
         <v>0.02</v>
@@ -6272,6 +6297,12 @@
     </row>
     <row r="177" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q177">
+        <f t="shared" si="15"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="178" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q178">
         <f t="shared" si="15"/>
         <v>0.02</v>
       </c>

</xml_diff>